<commit_message>
make power consumption an extended datapoint
</commit_message>
<xml_diff>
--- a/dataland-framework-toolbox/inputs/sme/sme.xlsx
+++ b/dataland-framework-toolbox/inputs/sme/sme.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d92432\Documents\Projekte\02-Dataland\Dataland\dataland-framework-toolbox\inputs\sme\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{247DEE1F-0FA9-4F78-AB26-4F80266EE398}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{968CC488-A0DE-422E-8342-F7AD2C77280C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="-110" windowWidth="38620" windowHeight="21220" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="75">
   <si>
     <t>Field Identifier</t>
   </si>
@@ -280,6 +280,9 @@
   </si>
   <si>
     <t>Financial Information</t>
+  </si>
+  <si>
+    <t>Extended</t>
   </si>
 </sst>
 </file>
@@ -711,7 +714,7 @@
   <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -996,7 +999,9 @@
       <c r="I9" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="J9" s="7"/>
+      <c r="J9" s="11" t="s">
+        <v>74</v>
+      </c>
       <c r="K9" s="9"/>
       <c r="L9" s="7"/>
       <c r="M9" s="11"/>

</xml_diff>

<commit_message>
prepare everything for sme upload page
</commit_message>
<xml_diff>
--- a/dataland-framework-toolbox/inputs/sme/sme.xlsx
+++ b/dataland-framework-toolbox/inputs/sme/sme.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d92432\Documents\Projekte\02-Dataland\Dataland\dataland-framework-toolbox\inputs\sme\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{968CC488-A0DE-422E-8342-F7AD2C77280C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{574A87D5-2576-41C6-92D6-49A794C4E9F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="38620" windowHeight="21220" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Framework Data Model" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="86">
   <si>
     <t>Field Identifier</t>
   </si>
@@ -258,12 +258,6 @@
     <t>10</t>
   </si>
   <si>
-    <t>less than 25 percent|between 25 and 50 percent|between 50 and 75 percent|over 75 percent</t>
-  </si>
-  <si>
-    <t>less than 1 percent|between 1 and 5 percent|between 5 and 10 percent|between 10 and 15 percent|between 15 and 20 percent|between 20 and 25 percent|over 25 percent</t>
-  </si>
-  <si>
     <t>Sectors</t>
   </si>
   <si>
@@ -283,6 +277,45 @@
   </si>
   <si>
     <t>Extended</t>
+  </si>
+  <si>
+    <t>Less than 1 percent|Between 1 and 5 percent|Between 5 and 10 percent|Between 10 and 15 percent|Between 15 and 20 percent|Between 20 and 25 percent|Over 25 percent</t>
+  </si>
+  <si>
+    <t>Less than 25 percent|Between 25 and 50 percent|Between 50 and 75 percent|Over 75 percent</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>Reporting Date</t>
+  </si>
+  <si>
+    <t>Please select a date on which the specified values can be considered valid.</t>
+  </si>
+  <si>
+    <t>Referenced Reports</t>
+  </si>
+  <si>
+    <t>Provide all documents that need to be referenced in this dataset.</t>
+  </si>
+  <si>
+    <t>Report Preupload</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>11</t>
   </si>
 </sst>
 </file>
@@ -408,7 +441,7 @@
       <alignment vertical="top"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
@@ -447,6 +480,24 @@
     </xf>
     <xf numFmtId="49" fontId="4" fillId="3" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -711,10 +762,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M16"/>
+  <dimension ref="A1:M18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -773,37 +824,37 @@
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A2" s="10">
-        <v>1</v>
-      </c>
-      <c r="B2" s="11" t="s">
+      <c r="A2" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="B2" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="F2" s="8"/>
-      <c r="G2" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="11" t="s">
+      <c r="D2" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="F2" s="17"/>
+      <c r="G2" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="16"/>
+      <c r="M2" s="19" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A3" s="10">
-        <v>3</v>
+    <row r="3" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+      <c r="A3" s="10" t="s">
+        <v>76</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>13</v>
@@ -812,14 +863,14 @@
         <v>31</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>35</v>
+        <v>66</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F3" s="8"/>
       <c r="G3" s="11" t="s">
-        <v>28</v>
+        <v>64</v>
       </c>
       <c r="H3" s="11"/>
       <c r="I3" s="11"/>
@@ -832,7 +883,7 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" s="10">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" s="11" t="s">
         <v>13</v>
@@ -841,14 +892,14 @@
         <v>31</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F4" s="8"/>
       <c r="G4" s="11" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="H4" s="11"/>
       <c r="I4" s="11"/>
@@ -861,77 +912,75 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" s="10">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" s="11" t="s">
         <v>13</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>73</v>
+        <v>31</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F5" s="8"/>
       <c r="G5" s="11" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="H5" s="11"/>
-      <c r="I5" s="11" t="s">
-        <v>61</v>
-      </c>
+      <c r="I5" s="11"/>
       <c r="J5" s="7"/>
       <c r="K5" s="9"/>
       <c r="L5" s="7"/>
-      <c r="M5" s="11"/>
+      <c r="M5" s="11" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A6" s="10">
-        <v>6</v>
+      <c r="A6" s="10" t="s">
+        <v>82</v>
       </c>
       <c r="B6" s="11" t="s">
         <v>13</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>73</v>
+        <v>31</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>38</v>
+        <v>79</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="F6" s="8"/>
       <c r="G6" s="11" t="s">
-        <v>27</v>
+        <v>81</v>
       </c>
       <c r="H6" s="11"/>
-      <c r="I6" s="11" t="s">
-        <v>61</v>
-      </c>
+      <c r="I6" s="11"/>
       <c r="J6" s="7"/>
       <c r="K6" s="9"/>
       <c r="L6" s="7"/>
       <c r="M6" s="11"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A7" s="10">
-        <v>7</v>
+      <c r="A7" s="10" t="s">
+        <v>83</v>
       </c>
       <c r="B7" s="11" t="s">
         <v>13</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F7" s="8"/>
       <c r="G7" s="11" t="s">
@@ -946,30 +995,30 @@
       <c r="L7" s="7"/>
       <c r="M7" s="11"/>
     </row>
-    <row r="8" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" s="10" t="s">
-        <v>19</v>
+        <v>84</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>32</v>
+        <v>71</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F8" s="8"/>
       <c r="G8" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="H8" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="I8" s="11"/>
+        <v>27</v>
+      </c>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11" t="s">
+        <v>61</v>
+      </c>
       <c r="J8" s="7"/>
       <c r="K8" s="9"/>
       <c r="L8" s="7"/>
@@ -977,19 +1026,19 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>33</v>
+        <v>71</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>70</v>
+        <v>39</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F9" s="8"/>
       <c r="G9" s="11" t="s">
@@ -997,45 +1046,45 @@
       </c>
       <c r="H9" s="11"/>
       <c r="I9" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="J9" s="11" t="s">
-        <v>74</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="J9" s="7"/>
       <c r="K9" s="9"/>
       <c r="L9" s="7"/>
       <c r="M9" s="11"/>
     </row>
     <row r="10" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="10" t="s">
-        <v>65</v>
+        <v>20</v>
       </c>
       <c r="B10" s="11" t="s">
         <v>29</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F10" s="8"/>
       <c r="G10" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="H10" s="11"/>
+        <v>18</v>
+      </c>
+      <c r="H10" s="11" t="s">
+        <v>73</v>
+      </c>
       <c r="I10" s="11"/>
       <c r="J10" s="7"/>
       <c r="K10" s="9"/>
       <c r="L10" s="7"/>
       <c r="M10" s="11"/>
     </row>
-    <row r="11" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" s="10" t="s">
-        <v>21</v>
+        <v>65</v>
       </c>
       <c r="B11" s="11" t="s">
         <v>29</v>
@@ -1044,10 +1093,10 @@
         <v>33</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F11" s="8"/>
       <c r="G11" s="11" t="s">
@@ -1057,14 +1106,16 @@
       <c r="I11" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="J11" s="7"/>
+      <c r="J11" s="11" t="s">
+        <v>72</v>
+      </c>
       <c r="K11" s="9"/>
       <c r="L11" s="7"/>
       <c r="M11" s="11"/>
     </row>
     <row r="12" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" s="10" t="s">
-        <v>22</v>
+        <v>85</v>
       </c>
       <c r="B12" s="11" t="s">
         <v>29</v>
@@ -1073,18 +1124,16 @@
         <v>33</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F12" s="8"/>
       <c r="G12" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="H12" s="11" t="s">
-        <v>63</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="H12" s="11"/>
       <c r="I12" s="11"/>
       <c r="J12" s="7"/>
       <c r="K12" s="9"/>
@@ -1093,7 +1142,7 @@
     </row>
     <row r="13" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A13" s="10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B13" s="11" t="s">
         <v>29</v>
@@ -1102,19 +1151,19 @@
         <v>33</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>43</v>
+        <v>69</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F13" s="8"/>
       <c r="G13" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="H13" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="I13" s="11"/>
+        <v>27</v>
+      </c>
+      <c r="H13" s="11"/>
+      <c r="I13" s="11" t="s">
+        <v>62</v>
+      </c>
       <c r="J13" s="7"/>
       <c r="K13" s="9"/>
       <c r="L13" s="7"/>
@@ -1122,25 +1171,27 @@
     </row>
     <row r="14" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A14" s="10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F14" s="8"/>
       <c r="G14" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="H14" s="11"/>
+        <v>18</v>
+      </c>
+      <c r="H14" s="11" t="s">
+        <v>63</v>
+      </c>
       <c r="I14" s="11"/>
       <c r="J14" s="7"/>
       <c r="K14" s="9"/>
@@ -1149,40 +1200,36 @@
     </row>
     <row r="15" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" s="10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>72</v>
+        <v>43</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F15" s="8"/>
       <c r="G15" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="H15" s="11"/>
-      <c r="I15" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="J15" s="13"/>
-      <c r="K15" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="H15" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="I15" s="11"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="9"/>
+      <c r="L15" s="7"/>
+      <c r="M15" s="11"/>
+    </row>
+    <row r="16" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+      <c r="A16" s="10" t="s">
         <v>24</v>
-      </c>
-      <c r="L15" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="M15" s="11"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A16" s="10" t="s">
-        <v>26</v>
       </c>
       <c r="B16" s="11" t="s">
         <v>30</v>
@@ -1191,27 +1238,87 @@
         <v>34</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F16" s="8"/>
       <c r="G16" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="H16" s="11" t="s">
-        <v>69</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="H16" s="11"/>
       <c r="I16" s="11"/>
       <c r="J16" s="7"/>
-      <c r="K16" s="14" t="s">
+      <c r="K16" s="9"/>
+      <c r="L16" s="7"/>
+      <c r="M16" s="11"/>
+    </row>
+    <row r="17" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+      <c r="A17" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="F17" s="8"/>
+      <c r="G17" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="H17" s="11"/>
+      <c r="I17" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="J17" s="13"/>
+      <c r="K17" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="L16" s="11" t="s">
+      <c r="L17" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="M16" s="11"/>
+      <c r="M17" s="11"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A18" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="E18" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="F18" s="8"/>
+      <c r="G18" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="H18" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="I18" s="11"/>
+      <c r="J18" s="7"/>
+      <c r="K18" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="L18" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="M18" s="11"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:M1" xr:uid="{00000000-0009-0000-0000-000000000000}"/>

</xml_diff>

<commit_message>
wip sme generation in toolbox part 3
</commit_message>
<xml_diff>
--- a/dataland-framework-toolbox/inputs/sme/sme.xlsx
+++ b/dataland-framework-toolbox/inputs/sme/sme.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d92048\IdeaProjects\Dataland5\dataland-framework-toolbox\inputs\sme\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{416D9BC3-99A1-4252-8974-FB7DBE1EB2FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AACFCC4-0C62-412B-92DA-6CACD4E82399}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C4E498E0-8E09-4328-BD54-6E3CD29DBCBD}"/>
   </bookViews>
@@ -336,9 +336,6 @@
     <t>34</t>
   </si>
   <si>
-    <t>Total nature-oriented area off-site previous_year</t>
-  </si>
-  <si>
     <t>35</t>
   </si>
   <si>
@@ -966,9 +963,6 @@
     <t>Subsidiary</t>
   </si>
   <si>
-    <t>Custom Component Subsidiary</t>
-  </si>
-  <si>
     <t>Custom Component Pollution</t>
   </si>
   <si>
@@ -1033,6 +1027,12 @@
   </si>
   <si>
     <t>Dummy Value Please Delete</t>
+  </si>
+  <si>
+    <t>Sme Subsidiary</t>
+  </si>
+  <si>
+    <t>Total nature-oriented area off-site previous year</t>
   </si>
 </sst>
 </file>
@@ -1639,8 +1639,8 @@
   <dimension ref="A1:N94"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B14" sqref="A14:XFD14"/>
+      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1661,43 +1661,43 @@
   <sheetData>
     <row r="1" spans="1:14" s="24" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="20" t="s">
+        <v>284</v>
+      </c>
+      <c r="B1" s="21" t="s">
         <v>285</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="C1" s="16" t="s">
         <v>286</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="D1" s="21" t="s">
         <v>287</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="E1" s="22" t="s">
         <v>288</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="F1" s="22" t="s">
         <v>289</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="G1" s="16" t="s">
         <v>290</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="H1" s="21" t="s">
         <v>291</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="I1" s="21" t="s">
         <v>292</v>
       </c>
-      <c r="I1" s="21" t="s">
+      <c r="J1" s="21" t="s">
         <v>293</v>
       </c>
-      <c r="J1" s="21" t="s">
+      <c r="K1" s="23" t="s">
         <v>294</v>
       </c>
-      <c r="K1" s="23" t="s">
+      <c r="L1" s="21" t="s">
         <v>295</v>
       </c>
-      <c r="L1" s="21" t="s">
+      <c r="M1" s="21" t="s">
         <v>296</v>
-      </c>
-      <c r="M1" s="21" t="s">
-        <v>297</v>
       </c>
       <c r="N1" s="21"/>
     </row>
@@ -1706,10 +1706,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="26" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C2" s="27" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>3</v>
@@ -1736,20 +1736,20 @@
         <v>11</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C3" s="27" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>8</v>
       </c>
       <c r="F3" s="5"/>
-      <c r="G3" s="3" t="s">
-        <v>300</v>
+      <c r="G3" s="27" t="s">
+        <v>321</v>
       </c>
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
@@ -1764,10 +1764,10 @@
         <v>14</v>
       </c>
       <c r="B4" s="26" t="s">
+        <v>305</v>
+      </c>
+      <c r="C4" s="28" t="s">
         <v>307</v>
-      </c>
-      <c r="C4" s="28" t="s">
-        <v>309</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>12</v>
@@ -1777,7 +1777,7 @@
       </c>
       <c r="F4" s="10"/>
       <c r="G4" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
@@ -1792,10 +1792,10 @@
         <v>19</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C5" s="28" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>15</v>
@@ -1822,10 +1822,10 @@
         <v>22</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C6" s="28" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>20</v>
@@ -1842,7 +1842,7 @@
         <v>18</v>
       </c>
       <c r="J6" s="11" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="K6" s="12"/>
       <c r="L6" s="11"/>
@@ -1854,10 +1854,10 @@
         <v>24</v>
       </c>
       <c r="B7" s="26" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C7" s="28" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>23</v>
@@ -1882,10 +1882,10 @@
         <v>26</v>
       </c>
       <c r="B8" s="26" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C8" s="28" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>25</v>
@@ -1910,10 +1910,10 @@
         <v>30</v>
       </c>
       <c r="B9" s="26" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C9" s="28" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>27</v>
@@ -1930,7 +1930,7 @@
         <v>29</v>
       </c>
       <c r="J9" s="11" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="K9" s="12"/>
       <c r="L9" s="11"/>
@@ -1942,10 +1942,10 @@
         <v>33</v>
       </c>
       <c r="B10" s="26" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C10" s="28" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>31</v>
@@ -1962,7 +1962,7 @@
         <v>29</v>
       </c>
       <c r="J10" s="11" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="K10" s="12"/>
       <c r="L10" s="11"/>
@@ -1974,10 +1974,10 @@
         <v>36</v>
       </c>
       <c r="B11" s="26" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C11" s="28" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>34</v>
@@ -1994,7 +1994,7 @@
         <v>29</v>
       </c>
       <c r="J11" s="11" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="K11" s="12"/>
       <c r="L11" s="11"/>
@@ -2006,10 +2006,10 @@
         <v>39</v>
       </c>
       <c r="B12" s="26" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C12" s="28" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>37</v>
@@ -2026,7 +2026,7 @@
         <v>29</v>
       </c>
       <c r="J12" s="11" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="K12" s="12"/>
       <c r="L12" s="11"/>
@@ -2038,10 +2038,10 @@
         <v>42</v>
       </c>
       <c r="B13" s="26" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C13" s="28" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="9" t="s">
@@ -2049,7 +2049,7 @@
       </c>
       <c r="F13" s="10"/>
       <c r="G13" s="19" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
@@ -2064,16 +2064,16 @@
         <v>45</v>
       </c>
       <c r="B14" s="32" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C14" s="33" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="D14" s="34" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="E14" s="33" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="F14" s="35"/>
       <c r="G14" s="36" t="s">
@@ -2092,10 +2092,10 @@
         <v>48</v>
       </c>
       <c r="B15" s="26" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C15" s="28" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="9" t="s">
@@ -2103,7 +2103,7 @@
       </c>
       <c r="F15" s="10"/>
       <c r="G15" s="3" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
@@ -2118,10 +2118,10 @@
         <v>52</v>
       </c>
       <c r="B16" s="26" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C16" s="28" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="D16" s="9" t="s">
         <v>84</v>
@@ -2146,10 +2146,10 @@
         <v>55</v>
       </c>
       <c r="B17" s="26" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C17" s="28" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="D17" s="9" t="s">
         <v>86</v>
@@ -2174,10 +2174,10 @@
         <v>57</v>
       </c>
       <c r="B18" s="26" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C18" s="28" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="D18" s="9" t="s">
         <v>88</v>
@@ -2202,10 +2202,10 @@
         <v>59</v>
       </c>
       <c r="B19" s="26" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C19" s="28" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="D19" s="9" t="s">
         <v>91</v>
@@ -2230,10 +2230,10 @@
         <v>61</v>
       </c>
       <c r="B20" s="26" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C20" s="28" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="D20" s="9" t="s">
         <v>93</v>
@@ -2258,10 +2258,10 @@
         <v>63</v>
       </c>
       <c r="B21" s="26" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C21" s="28" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="D21" s="9" t="s">
         <v>95</v>
@@ -2286,13 +2286,13 @@
         <v>66</v>
       </c>
       <c r="B22" s="26" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C22" s="28" t="s">
-        <v>312</v>
-      </c>
-      <c r="D22" s="9" t="s">
-        <v>97</v>
+        <v>310</v>
+      </c>
+      <c r="D22" s="28" t="s">
+        <v>322</v>
       </c>
       <c r="E22" s="9" t="s">
         <v>82</v>
@@ -2314,13 +2314,13 @@
         <v>69</v>
       </c>
       <c r="B23" s="26" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C23" s="28" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E23" s="9" t="s">
         <v>82</v>
@@ -2342,13 +2342,13 @@
         <v>71</v>
       </c>
       <c r="B24" s="26" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C24" s="28" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E24" s="9" t="s">
         <v>82</v>
@@ -2370,13 +2370,13 @@
         <v>73</v>
       </c>
       <c r="B25" s="26" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C25" s="28" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E25" s="9" t="s">
         <v>82</v>
@@ -2398,13 +2398,13 @@
         <v>75</v>
       </c>
       <c r="B26" s="26" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C26" s="28" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E26" s="9" t="s">
         <v>82</v>
@@ -2426,13 +2426,13 @@
         <v>77</v>
       </c>
       <c r="B27" s="26" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C27" s="28" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E27" s="9" t="s">
         <v>82</v>
@@ -2454,16 +2454,16 @@
         <v>81</v>
       </c>
       <c r="B28" s="26" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C28" s="28" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D28" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="E28" s="9" t="s">
         <v>109</v>
-      </c>
-      <c r="E28" s="9" t="s">
-        <v>110</v>
       </c>
       <c r="F28" s="9"/>
       <c r="G28" s="9" t="s">
@@ -2471,10 +2471,10 @@
       </c>
       <c r="H28" s="9"/>
       <c r="I28" s="29" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="J28" s="11" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="K28" s="9"/>
       <c r="L28" s="9"/>
@@ -2486,13 +2486,13 @@
         <v>83</v>
       </c>
       <c r="B29" s="26" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C29" s="28" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E29" s="9"/>
       <c r="F29" s="9"/>
@@ -2501,7 +2501,7 @@
       </c>
       <c r="H29" s="9"/>
       <c r="I29" s="29" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="J29" s="9"/>
       <c r="K29" s="9"/>
@@ -2514,16 +2514,16 @@
         <v>85</v>
       </c>
       <c r="B30" s="26" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C30" s="28" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E30" s="9" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="F30" s="9"/>
       <c r="G30" s="9" t="s">
@@ -2531,7 +2531,7 @@
       </c>
       <c r="H30" s="9"/>
       <c r="I30" s="29" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="J30" s="9"/>
       <c r="K30" s="9"/>
@@ -2544,13 +2544,13 @@
         <v>87</v>
       </c>
       <c r="B31" s="26" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C31" s="28" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E31" s="9"/>
       <c r="F31" s="9"/>
@@ -2559,7 +2559,7 @@
       </c>
       <c r="H31" s="9"/>
       <c r="I31" s="29" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="J31" s="9"/>
       <c r="K31" s="9"/>
@@ -2572,13 +2572,13 @@
         <v>90</v>
       </c>
       <c r="B32" s="26" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C32" s="28" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E32" s="9"/>
       <c r="F32" s="9"/>
@@ -2587,7 +2587,7 @@
       </c>
       <c r="H32" s="9"/>
       <c r="I32" s="29" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="J32" s="9"/>
       <c r="K32" s="9"/>
@@ -2600,13 +2600,13 @@
         <v>92</v>
       </c>
       <c r="B33" s="26" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C33" s="28" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E33" s="9"/>
       <c r="F33" s="9"/>
@@ -2615,7 +2615,7 @@
       </c>
       <c r="H33" s="9"/>
       <c r="I33" s="29" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="J33" s="9"/>
       <c r="K33" s="9"/>
@@ -2628,13 +2628,13 @@
         <v>94</v>
       </c>
       <c r="B34" s="26" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C34" s="28" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E34" s="9"/>
       <c r="F34" s="9"/>
@@ -2643,7 +2643,7 @@
       </c>
       <c r="H34" s="9"/>
       <c r="I34" s="29" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="J34" s="9"/>
       <c r="K34" s="9"/>
@@ -2656,13 +2656,13 @@
         <v>96</v>
       </c>
       <c r="B35" s="26" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C35" s="28" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E35" s="9"/>
       <c r="F35" s="9"/>
@@ -2671,7 +2671,7 @@
       </c>
       <c r="H35" s="9"/>
       <c r="I35" s="29" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="J35" s="9"/>
       <c r="K35" s="9"/>
@@ -2681,19 +2681,19 @@
     </row>
     <row r="36" spans="1:14" ht="391.5" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B36" s="26" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C36" s="28" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="D36" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="E36" s="9" t="s">
         <v>128</v>
-      </c>
-      <c r="E36" s="9" t="s">
-        <v>129</v>
       </c>
       <c r="F36" s="9"/>
       <c r="G36" s="9" t="s">
@@ -2701,7 +2701,7 @@
       </c>
       <c r="H36" s="9"/>
       <c r="I36" s="9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J36" s="9"/>
       <c r="K36" s="9"/>
@@ -2711,16 +2711,16 @@
     </row>
     <row r="37" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B37" s="26" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C37" s="28" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E37" s="9"/>
       <c r="F37" s="9"/>
@@ -2729,7 +2729,7 @@
       </c>
       <c r="H37" s="9"/>
       <c r="I37" s="9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J37" s="9"/>
       <c r="K37" s="9"/>
@@ -2739,16 +2739,16 @@
     </row>
     <row r="38" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A38" s="30" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B38" s="26" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C38" s="28" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E38" s="9"/>
       <c r="F38" s="9"/>
@@ -2765,16 +2765,16 @@
     </row>
     <row r="39" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B39" s="26" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C39" s="28" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E39" s="9"/>
       <c r="F39" s="9"/>
@@ -2783,7 +2783,7 @@
       </c>
       <c r="H39" s="9"/>
       <c r="I39" s="9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J39" s="9"/>
       <c r="K39" s="9"/>
@@ -2793,16 +2793,16 @@
     </row>
     <row r="40" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B40" s="26" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C40" s="28" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="D40" s="9" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="E40" s="9"/>
       <c r="F40" s="9"/>
@@ -2819,26 +2819,26 @@
     </row>
     <row r="41" spans="1:14" ht="174" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B41" s="26" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C41" s="28" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="D41" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="E41" s="9" t="s">
         <v>139</v>
-      </c>
-      <c r="E41" s="9" t="s">
-        <v>140</v>
       </c>
       <c r="F41" s="9"/>
       <c r="G41" s="25" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="H41" s="9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I41" s="9"/>
       <c r="J41" s="2"/>
@@ -2849,19 +2849,19 @@
     </row>
     <row r="42" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A42" s="30" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B42" s="26" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C42" s="28" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="D42" s="9"/>
       <c r="E42" s="9"/>
       <c r="F42" s="9"/>
       <c r="G42" s="8" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="H42" s="9"/>
       <c r="I42" s="9"/>
@@ -2873,26 +2873,26 @@
     </row>
     <row r="43" spans="1:14" ht="116" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B43" s="26" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C43" s="28" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="D43" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="E43" s="9" t="s">
         <v>164</v>
-      </c>
-      <c r="E43" s="9" t="s">
-        <v>165</v>
       </c>
       <c r="F43" s="9"/>
       <c r="G43" s="25" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="H43" s="9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="I43" s="9"/>
       <c r="J43" s="9"/>
@@ -2903,19 +2903,19 @@
     </row>
     <row r="44" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B44" s="26" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C44" s="28" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="D44" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="E44" s="9" t="s">
         <v>168</v>
-      </c>
-      <c r="E44" s="9" t="s">
-        <v>169</v>
       </c>
       <c r="F44" s="9"/>
       <c r="G44" s="9" t="s">
@@ -2923,33 +2923,33 @@
       </c>
       <c r="H44" s="9"/>
       <c r="I44" s="9" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J44" s="9"/>
       <c r="K44" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="L44" s="18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="M44" s="9"/>
       <c r="N44" s="2"/>
     </row>
     <row r="45" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B45" s="26" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C45" s="28" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="D45" s="9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E45" s="9" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F45" s="9"/>
       <c r="G45" s="9" t="s">
@@ -2957,33 +2957,33 @@
       </c>
       <c r="H45" s="9"/>
       <c r="I45" s="9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J45" s="9"/>
       <c r="K45" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="L45" s="18" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="M45" s="9"/>
       <c r="N45" s="2"/>
     </row>
     <row r="46" spans="1:14" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A46" s="30" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B46" s="26" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C46" s="28" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="D46" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="E46" s="9" t="s">
         <v>177</v>
-      </c>
-      <c r="E46" s="9" t="s">
-        <v>178</v>
       </c>
       <c r="F46" s="9"/>
       <c r="G46" s="9" t="s">
@@ -2991,33 +2991,33 @@
       </c>
       <c r="H46" s="9"/>
       <c r="I46" s="9" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J46" s="9"/>
       <c r="K46" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="L46" s="18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="M46" s="9"/>
       <c r="N46" s="2"/>
     </row>
     <row r="47" spans="1:14" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B47" s="26" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C47" s="28" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="D47" s="9" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E47" s="9" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F47" s="9"/>
       <c r="G47" s="9" t="s">
@@ -3025,30 +3025,30 @@
       </c>
       <c r="H47" s="9"/>
       <c r="I47" s="9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J47" s="9"/>
       <c r="K47" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="L47" s="18" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="M47" s="9"/>
       <c r="N47" s="2"/>
     </row>
     <row r="48" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B48" s="26" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C48" s="28" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="D48" s="9" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E48" s="9"/>
       <c r="F48" s="9"/>
@@ -3057,30 +3057,30 @@
       </c>
       <c r="H48" s="9"/>
       <c r="I48" s="9" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J48" s="9"/>
       <c r="K48" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="L48" s="18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="M48" s="9"/>
       <c r="N48" s="2"/>
     </row>
     <row r="49" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B49" s="26" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C49" s="28" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="D49" s="9" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E49" s="9"/>
       <c r="F49" s="9"/>
@@ -3089,33 +3089,33 @@
       </c>
       <c r="H49" s="9"/>
       <c r="I49" s="9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J49" s="9"/>
       <c r="K49" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="L49" s="18" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="M49" s="9"/>
       <c r="N49" s="2"/>
     </row>
     <row r="50" spans="1:14" ht="87" x14ac:dyDescent="0.35">
       <c r="A50" s="30" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B50" s="26" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C50" s="28" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="D50" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="E50" s="9" t="s">
         <v>186</v>
-      </c>
-      <c r="E50" s="9" t="s">
-        <v>187</v>
       </c>
       <c r="F50" s="9"/>
       <c r="G50" s="9" t="s">
@@ -3123,33 +3123,33 @@
       </c>
       <c r="H50" s="9"/>
       <c r="I50" s="9" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J50" s="9"/>
       <c r="K50" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="L50" s="18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="M50" s="9"/>
       <c r="N50" s="2"/>
     </row>
     <row r="51" spans="1:14" ht="87" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B51" s="26" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C51" s="28" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="D51" s="9" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E51" s="9" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F51" s="9"/>
       <c r="G51" s="9" t="s">
@@ -3157,30 +3157,30 @@
       </c>
       <c r="H51" s="9"/>
       <c r="I51" s="9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J51" s="9"/>
       <c r="K51" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="L51" s="18" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="M51" s="9"/>
       <c r="N51" s="2"/>
     </row>
     <row r="52" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B52" s="26" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C52" s="28" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="D52" s="9" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E52" s="9"/>
       <c r="F52" s="9"/>
@@ -3189,30 +3189,30 @@
       </c>
       <c r="H52" s="9"/>
       <c r="I52" s="9" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J52" s="9"/>
       <c r="K52" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="L52" s="18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="M52" s="9"/>
       <c r="N52" s="2"/>
     </row>
     <row r="53" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B53" s="26" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C53" s="28" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="D53" s="9" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E53" s="9"/>
       <c r="F53" s="9"/>
@@ -3221,30 +3221,30 @@
       </c>
       <c r="H53" s="9"/>
       <c r="I53" s="9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J53" s="9"/>
       <c r="K53" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="L53" s="18" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="M53" s="9"/>
       <c r="N53" s="2"/>
     </row>
     <row r="54" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A54" s="30" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B54" s="26" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C54" s="28" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="D54" s="9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E54" s="9"/>
       <c r="F54" s="9"/>
@@ -3253,30 +3253,30 @@
       </c>
       <c r="H54" s="9"/>
       <c r="I54" s="9" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J54" s="9"/>
       <c r="K54" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="L54" s="18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="M54" s="9"/>
       <c r="N54" s="2"/>
     </row>
     <row r="55" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B55" s="26" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C55" s="28" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="D55" s="9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E55" s="9"/>
       <c r="F55" s="9"/>
@@ -3285,30 +3285,30 @@
       </c>
       <c r="H55" s="9"/>
       <c r="I55" s="9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J55" s="9"/>
       <c r="K55" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="L55" s="18" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="M55" s="9"/>
       <c r="N55" s="2"/>
     </row>
     <row r="56" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B56" s="26" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C56" s="28" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="D56" s="9" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E56" s="9"/>
       <c r="F56" s="9"/>
@@ -3317,30 +3317,30 @@
       </c>
       <c r="H56" s="9"/>
       <c r="I56" s="9" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J56" s="9"/>
       <c r="K56" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="L56" s="18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="M56" s="9"/>
       <c r="N56" s="2"/>
     </row>
     <row r="57" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B57" s="26" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C57" s="28" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="D57" s="9" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E57" s="9"/>
       <c r="F57" s="9"/>
@@ -3349,35 +3349,35 @@
       </c>
       <c r="H57" s="9"/>
       <c r="I57" s="9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J57" s="9"/>
       <c r="K57" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="L57" s="9" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="M57" s="9"/>
       <c r="N57" s="2"/>
     </row>
     <row r="58" spans="1:14" ht="87" x14ac:dyDescent="0.35">
       <c r="A58" s="30" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B58" s="26" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C58" s="28" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="D58" s="9"/>
       <c r="E58" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F58" s="9"/>
       <c r="G58" s="19" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="H58" s="9"/>
       <c r="I58" s="9"/>
@@ -3389,19 +3389,19 @@
     </row>
     <row r="59" spans="1:14" ht="58" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B59" s="26" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C59" s="28" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="D59" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="E59" s="9" t="s">
         <v>210</v>
-      </c>
-      <c r="E59" s="9" t="s">
-        <v>211</v>
       </c>
       <c r="F59" s="9"/>
       <c r="G59" s="9" t="s">
@@ -3409,7 +3409,7 @@
       </c>
       <c r="H59" s="9"/>
       <c r="I59" s="9" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="J59" s="9"/>
       <c r="K59" s="9"/>
@@ -3419,23 +3419,23 @@
     </row>
     <row r="60" spans="1:14" ht="58" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B60" s="26" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C60" s="28" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="D60" s="9" t="s">
+        <v>213</v>
+      </c>
+      <c r="E60" s="9" t="s">
         <v>214</v>
-      </c>
-      <c r="E60" s="9" t="s">
-        <v>215</v>
       </c>
       <c r="F60" s="9"/>
       <c r="G60" s="9" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H60" s="9"/>
       <c r="I60" s="9"/>
@@ -3447,19 +3447,19 @@
     </row>
     <row r="61" spans="1:14" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B61" s="26" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C61" s="28" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="D61" s="9" t="s">
+        <v>217</v>
+      </c>
+      <c r="E61" s="9" t="s">
         <v>218</v>
-      </c>
-      <c r="E61" s="9" t="s">
-        <v>219</v>
       </c>
       <c r="F61" s="9"/>
       <c r="G61" s="9" t="s">
@@ -3475,219 +3475,219 @@
     </row>
     <row r="62" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A62" s="30" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B62" s="26" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C62" s="28" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="D62" s="9" t="s">
+        <v>220</v>
+      </c>
+      <c r="E62" s="9" t="s">
         <v>221</v>
-      </c>
-      <c r="E62" s="9" t="s">
-        <v>222</v>
       </c>
       <c r="F62" s="9"/>
       <c r="G62" s="9" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H62" s="9"/>
       <c r="I62" s="9" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J62" s="9"/>
       <c r="K62" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="L62" s="18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="M62" s="9"/>
       <c r="N62" s="2"/>
     </row>
     <row r="63" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B63" s="26" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C63" s="28" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="D63" s="9" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E63" s="9" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F63" s="9"/>
       <c r="G63" s="9" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H63" s="9"/>
       <c r="I63" s="9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J63" s="9"/>
       <c r="K63" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="L63" s="18" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="M63" s="9"/>
       <c r="N63" s="2"/>
     </row>
     <row r="64" spans="1:14" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B64" s="26" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C64" s="28" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="D64" s="9" t="s">
+        <v>225</v>
+      </c>
+      <c r="E64" s="9" t="s">
         <v>226</v>
-      </c>
-      <c r="E64" s="9" t="s">
-        <v>227</v>
       </c>
       <c r="F64" s="9"/>
       <c r="G64" s="9" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H64" s="9"/>
       <c r="I64" s="9" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J64" s="9"/>
       <c r="K64" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="L64" s="18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="M64" s="9"/>
       <c r="N64" s="2"/>
     </row>
     <row r="65" spans="1:14" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B65" s="26" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C65" s="28" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="D65" s="9" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E65" s="9" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F65" s="9"/>
       <c r="G65" s="9" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H65" s="9"/>
       <c r="I65" s="9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J65" s="9"/>
       <c r="K65" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="L65" s="18" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="M65" s="9"/>
       <c r="N65" s="2"/>
     </row>
     <row r="66" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A66" s="30" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B66" s="26" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C66" s="28" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="D66" s="9" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E66" s="9"/>
       <c r="F66" s="9"/>
       <c r="G66" s="9" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H66" s="9"/>
       <c r="I66" s="9" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J66" s="9"/>
       <c r="K66" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="L66" s="18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="M66" s="9"/>
       <c r="N66" s="2"/>
     </row>
     <row r="67" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B67" s="26" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C67" s="28" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="D67" s="9" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E67" s="9"/>
       <c r="F67" s="9"/>
       <c r="G67" s="9" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H67" s="9"/>
       <c r="I67" s="9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J67" s="9"/>
       <c r="K67" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="L67" s="18" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="M67" s="9"/>
       <c r="N67" s="2"/>
     </row>
     <row r="68" spans="1:14" ht="87" x14ac:dyDescent="0.35">
       <c r="A68" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B68" s="26" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C68" s="28" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D68" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="E68" s="9" t="s">
         <v>235</v>
-      </c>
-      <c r="E68" s="9" t="s">
-        <v>236</v>
       </c>
       <c r="F68" s="9"/>
       <c r="G68" s="9" t="s">
@@ -3695,33 +3695,33 @@
       </c>
       <c r="H68" s="9"/>
       <c r="I68" s="9" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J68" s="9"/>
       <c r="K68" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="L68" s="18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="M68" s="9"/>
       <c r="N68" s="2"/>
     </row>
     <row r="69" spans="1:14" ht="87" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B69" s="26" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C69" s="28" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D69" s="9" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E69" s="9" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="F69" s="9"/>
       <c r="G69" s="9" t="s">
@@ -3729,33 +3729,33 @@
       </c>
       <c r="H69" s="9"/>
       <c r="I69" s="9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J69" s="9"/>
       <c r="K69" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="L69" s="9" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="M69" s="9"/>
       <c r="N69" s="2"/>
     </row>
     <row r="70" spans="1:14" ht="87" x14ac:dyDescent="0.35">
       <c r="A70" s="30" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B70" s="26" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C70" s="28" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D70" s="9" t="s">
+        <v>239</v>
+      </c>
+      <c r="E70" s="9" t="s">
         <v>240</v>
-      </c>
-      <c r="E70" s="9" t="s">
-        <v>241</v>
       </c>
       <c r="F70" s="9"/>
       <c r="G70" s="9" t="s">
@@ -3771,19 +3771,19 @@
     </row>
     <row r="71" spans="1:14" ht="87" x14ac:dyDescent="0.35">
       <c r="A71" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B71" s="26" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C71" s="28" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D71" s="9" t="s">
+        <v>241</v>
+      </c>
+      <c r="E71" s="9" t="s">
         <v>242</v>
-      </c>
-      <c r="E71" s="9" t="s">
-        <v>243</v>
       </c>
       <c r="F71" s="9"/>
       <c r="G71" s="9" t="s">
@@ -3799,19 +3799,19 @@
     </row>
     <row r="72" spans="1:14" ht="58" x14ac:dyDescent="0.35">
       <c r="A72" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B72" s="26" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C72" s="28" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D72" s="9" t="s">
+        <v>243</v>
+      </c>
+      <c r="E72" s="9" t="s">
         <v>244</v>
-      </c>
-      <c r="E72" s="9" t="s">
-        <v>245</v>
       </c>
       <c r="F72" s="9"/>
       <c r="G72" s="9" t="s">
@@ -3819,7 +3819,7 @@
       </c>
       <c r="H72" s="9"/>
       <c r="I72" s="9" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="J72" s="9"/>
       <c r="K72" s="9"/>
@@ -3829,16 +3829,16 @@
     </row>
     <row r="73" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A73" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B73" s="26" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C73" s="28" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D73" s="9" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E73" s="9"/>
       <c r="F73" s="9"/>
@@ -3847,7 +3847,7 @@
       </c>
       <c r="H73" s="9"/>
       <c r="I73" s="9" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="J73" s="9"/>
       <c r="K73" s="9"/>
@@ -3857,19 +3857,19 @@
     </row>
     <row r="74" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A74" s="30" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B74" s="26" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C74" s="28" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D74" s="9" t="s">
+        <v>247</v>
+      </c>
+      <c r="E74" s="9" t="s">
         <v>248</v>
-      </c>
-      <c r="E74" s="9" t="s">
-        <v>249</v>
       </c>
       <c r="F74" s="9"/>
       <c r="G74" s="9" t="s">
@@ -3885,26 +3885,26 @@
     </row>
     <row r="75" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A75" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B75" s="26" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C75" s="28" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D75" s="9" t="s">
+        <v>249</v>
+      </c>
+      <c r="E75" s="9" t="s">
         <v>250</v>
-      </c>
-      <c r="E75" s="9" t="s">
-        <v>251</v>
       </c>
       <c r="F75" s="9"/>
       <c r="G75" s="25" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="H75" s="9" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I75" s="9"/>
       <c r="J75" s="9"/>
@@ -3912,26 +3912,26 @@
         <v>42</v>
       </c>
       <c r="L75" s="9" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="M75" s="9"/>
       <c r="N75" s="2"/>
     </row>
     <row r="76" spans="1:14" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A76" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B76" s="26" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C76" s="28" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D76" s="9" t="s">
+        <v>253</v>
+      </c>
+      <c r="E76" s="9" t="s">
         <v>254</v>
-      </c>
-      <c r="E76" s="9" t="s">
-        <v>255</v>
       </c>
       <c r="F76" s="9"/>
       <c r="G76" s="9" t="s">
@@ -3939,30 +3939,30 @@
       </c>
       <c r="H76" s="9"/>
       <c r="I76" s="9" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="J76" s="9"/>
       <c r="K76" s="8">
         <v>42</v>
       </c>
       <c r="L76" s="9" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="M76" s="9"/>
       <c r="N76" s="2"/>
     </row>
     <row r="77" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A77" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B77" s="26" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C77" s="28" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D77" s="9" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E77" s="9"/>
       <c r="F77" s="9"/>
@@ -3971,33 +3971,33 @@
       </c>
       <c r="H77" s="9"/>
       <c r="I77" s="9" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="J77" s="9"/>
       <c r="K77" s="8">
         <v>42</v>
       </c>
       <c r="L77" s="9" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="M77" s="9"/>
       <c r="N77" s="2"/>
     </row>
     <row r="78" spans="1:14" ht="116" x14ac:dyDescent="0.35">
       <c r="A78" s="30" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B78" s="26" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C78" s="28" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D78" s="9" t="s">
+        <v>256</v>
+      </c>
+      <c r="E78" s="9" t="s">
         <v>257</v>
-      </c>
-      <c r="E78" s="9" t="s">
-        <v>258</v>
       </c>
       <c r="F78" s="9"/>
       <c r="G78" s="9" t="s">
@@ -4005,30 +4005,30 @@
       </c>
       <c r="H78" s="9"/>
       <c r="I78" s="9" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="J78" s="9"/>
       <c r="K78" s="8">
         <v>42</v>
       </c>
       <c r="L78" s="9" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="M78" s="9"/>
       <c r="N78" s="2"/>
     </row>
     <row r="79" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A79" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B79" s="26" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C79" s="28" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D79" s="9" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E79" s="9"/>
       <c r="F79" s="9"/>
@@ -4037,33 +4037,33 @@
       </c>
       <c r="H79" s="9"/>
       <c r="I79" s="9" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="J79" s="9"/>
       <c r="K79" s="8">
         <v>42</v>
       </c>
       <c r="L79" s="9" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="M79" s="9"/>
       <c r="N79" s="2"/>
     </row>
     <row r="80" spans="1:14" ht="116" x14ac:dyDescent="0.35">
       <c r="A80" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B80" s="26" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C80" s="28" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D80" s="9" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E80" s="9" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F80" s="9"/>
       <c r="G80" s="9" t="s">
@@ -4071,30 +4071,30 @@
       </c>
       <c r="H80" s="9"/>
       <c r="I80" s="9" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="J80" s="9"/>
       <c r="K80" s="8">
         <v>42</v>
       </c>
       <c r="L80" s="9" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="M80" s="9"/>
       <c r="N80" s="2"/>
     </row>
     <row r="81" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A81" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B81" s="26" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C81" s="28" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D81" s="9" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E81" s="9"/>
       <c r="F81" s="9"/>
@@ -4103,33 +4103,33 @@
       </c>
       <c r="H81" s="9"/>
       <c r="I81" s="9" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="J81" s="9"/>
       <c r="K81" s="8">
         <v>42</v>
       </c>
       <c r="L81" s="9" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="M81" s="9"/>
       <c r="N81" s="2"/>
     </row>
     <row r="82" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A82" s="30" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B82" s="26" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C82" s="28" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D82" s="9" t="s">
+        <v>261</v>
+      </c>
+      <c r="E82" s="9" t="s">
         <v>262</v>
-      </c>
-      <c r="E82" s="9" t="s">
-        <v>263</v>
       </c>
       <c r="F82" s="9"/>
       <c r="G82" s="9" t="s">
@@ -4137,33 +4137,33 @@
       </c>
       <c r="H82" s="9"/>
       <c r="I82" s="9" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="J82" s="9"/>
       <c r="K82" s="8">
         <v>42</v>
       </c>
       <c r="L82" s="9" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="M82" s="9"/>
       <c r="N82" s="2"/>
     </row>
     <row r="83" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A83" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B83" s="26" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C83" s="28" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D83" s="9" t="s">
+        <v>264</v>
+      </c>
+      <c r="E83" s="9" t="s">
         <v>265</v>
-      </c>
-      <c r="E83" s="9" t="s">
-        <v>266</v>
       </c>
       <c r="F83" s="9"/>
       <c r="G83" s="9" t="s">
@@ -4171,33 +4171,33 @@
       </c>
       <c r="H83" s="9"/>
       <c r="I83" s="9" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="J83" s="9"/>
       <c r="K83" s="8">
         <v>42</v>
       </c>
       <c r="L83" s="9" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="M83" s="9"/>
       <c r="N83" s="2"/>
     </row>
     <row r="84" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A84" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B84" s="26" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C84" s="28" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D84" s="9" t="s">
+        <v>266</v>
+      </c>
+      <c r="E84" s="9" t="s">
         <v>267</v>
-      </c>
-      <c r="E84" s="9" t="s">
-        <v>268</v>
       </c>
       <c r="F84" s="9"/>
       <c r="G84" s="9" t="s">
@@ -4210,26 +4210,26 @@
         <v>42</v>
       </c>
       <c r="L84" s="18" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="M84" s="9"/>
       <c r="N84" s="2"/>
     </row>
     <row r="85" spans="1:14" ht="58" x14ac:dyDescent="0.35">
       <c r="A85" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B85" s="26" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C85" s="28" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D85" s="9" t="s">
+        <v>268</v>
+      </c>
+      <c r="E85" s="9" t="s">
         <v>269</v>
-      </c>
-      <c r="E85" s="9" t="s">
-        <v>270</v>
       </c>
       <c r="F85" s="9"/>
       <c r="G85" s="9" t="s">
@@ -4237,33 +4237,33 @@
       </c>
       <c r="H85" s="9"/>
       <c r="I85" s="9" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J85" s="9"/>
       <c r="K85" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="L85" s="18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="M85" s="9"/>
       <c r="N85" s="2"/>
     </row>
     <row r="86" spans="1:14" ht="58" x14ac:dyDescent="0.35">
       <c r="A86" s="30" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B86" s="26" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C86" s="28" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D86" s="9" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E86" s="9" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="F86" s="9"/>
       <c r="G86" s="9" t="s">
@@ -4271,33 +4271,33 @@
       </c>
       <c r="H86" s="9"/>
       <c r="I86" s="9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J86" s="9"/>
       <c r="K86" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="L86" s="9" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="M86" s="9"/>
       <c r="N86" s="2"/>
     </row>
     <row r="87" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A87" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B87" s="26" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C87" s="28" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D87" s="9" t="s">
+        <v>271</v>
+      </c>
+      <c r="E87" s="9" t="s">
         <v>272</v>
-      </c>
-      <c r="E87" s="9" t="s">
-        <v>273</v>
       </c>
       <c r="F87" s="9"/>
       <c r="G87" s="9" t="s">
@@ -4313,19 +4313,19 @@
     </row>
     <row r="88" spans="1:14" ht="145" x14ac:dyDescent="0.35">
       <c r="A88" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B88" s="26" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C88" s="28" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D88" s="9" t="s">
+        <v>273</v>
+      </c>
+      <c r="E88" s="9" t="s">
         <v>274</v>
-      </c>
-      <c r="E88" s="9" t="s">
-        <v>275</v>
       </c>
       <c r="F88" s="9"/>
       <c r="G88" s="9" t="s">
@@ -4333,7 +4333,7 @@
       </c>
       <c r="H88" s="9"/>
       <c r="I88" s="9" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="J88" s="9"/>
       <c r="K88" s="9"/>
@@ -4343,16 +4343,16 @@
     </row>
     <row r="89" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A89" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B89" s="26" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C89" s="28" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D89" s="9" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E89" s="9"/>
       <c r="F89" s="9"/>
@@ -4361,7 +4361,7 @@
       </c>
       <c r="H89" s="9"/>
       <c r="I89" s="9" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="J89" s="9"/>
       <c r="K89" s="9"/>
@@ -4371,16 +4371,16 @@
     </row>
     <row r="90" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A90" s="30" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B90" s="26" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C90" s="28" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D90" s="9" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E90" s="9"/>
       <c r="F90" s="9"/>
@@ -4389,7 +4389,7 @@
       </c>
       <c r="H90" s="9"/>
       <c r="I90" s="9" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="J90" s="9"/>
       <c r="K90" s="9"/>
@@ -4399,16 +4399,16 @@
     </row>
     <row r="91" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A91" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B91" s="26" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C91" s="28" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D91" s="9" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E91" s="9"/>
       <c r="F91" s="9"/>
@@ -4417,7 +4417,7 @@
       </c>
       <c r="H91" s="9"/>
       <c r="I91" s="9" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="J91" s="2"/>
       <c r="K91" s="9"/>
@@ -4427,23 +4427,23 @@
     </row>
     <row r="92" spans="1:14" ht="304.5" x14ac:dyDescent="0.35">
       <c r="A92" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B92" s="26" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C92" s="28" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D92" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="E92" s="9" t="s">
         <v>279</v>
-      </c>
-      <c r="E92" s="9" t="s">
-        <v>280</v>
       </c>
       <c r="F92" s="9"/>
       <c r="G92" s="9" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="H92" s="9"/>
       <c r="I92" s="9"/>
@@ -4455,19 +4455,19 @@
     </row>
     <row r="93" spans="1:14" ht="116" x14ac:dyDescent="0.35">
       <c r="A93" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B93" s="26" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C93" s="28" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D93" s="9" t="s">
+        <v>281</v>
+      </c>
+      <c r="E93" s="9" t="s">
         <v>282</v>
-      </c>
-      <c r="E93" s="9" t="s">
-        <v>283</v>
       </c>
       <c r="F93" s="9"/>
       <c r="G93" s="9" t="s">
@@ -4483,22 +4483,22 @@
     </row>
     <row r="94" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A94" s="30" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B94" s="26" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C94" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D94" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="G94" t="s">
         <v>17</v>
       </c>
       <c r="I94" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
   </sheetData>
@@ -4525,58 +4525,58 @@
   <sheetData>
     <row r="1" spans="1:14" s="24" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="20" t="s">
+        <v>284</v>
+      </c>
+      <c r="B1" s="21" t="s">
         <v>285</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="C1" s="16" t="s">
         <v>286</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="D1" s="21" t="s">
         <v>287</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="E1" s="22" t="s">
         <v>288</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="F1" s="22" t="s">
         <v>289</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="G1" s="16" t="s">
         <v>290</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="H1" s="21" t="s">
         <v>291</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="I1" s="21" t="s">
         <v>292</v>
       </c>
-      <c r="I1" s="21" t="s">
+      <c r="J1" s="21" t="s">
         <v>293</v>
       </c>
-      <c r="J1" s="21" t="s">
+      <c r="K1" s="23" t="s">
         <v>294</v>
       </c>
-      <c r="K1" s="23" t="s">
+      <c r="L1" s="21" t="s">
         <v>295</v>
       </c>
-      <c r="L1" s="21" t="s">
+      <c r="M1" s="21" t="s">
         <v>296</v>
-      </c>
-      <c r="M1" s="21" t="s">
-        <v>297</v>
       </c>
       <c r="N1" s="21"/>
     </row>
     <row r="2" spans="1:14" ht="87" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E2" s="9"/>
       <c r="F2" s="9"/>
@@ -4584,11 +4584,11 @@
         <v>79</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="I2" s="9"/>
       <c r="J2" s="28" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="K2" s="9"/>
       <c r="L2" s="9"/>
@@ -4597,16 +4597,16 @@
     </row>
     <row r="3" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E3" s="9"/>
       <c r="F3" s="9"/>
@@ -4623,16 +4623,16 @@
     </row>
     <row r="4" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E4" s="9"/>
       <c r="F4" s="9"/>
@@ -4641,30 +4641,30 @@
       </c>
       <c r="H4" s="9"/>
       <c r="I4" s="9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J4" s="9"/>
       <c r="K4" s="9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="L4" s="18" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="M4" s="9"/>
       <c r="N4" s="2"/>
     </row>
     <row r="5" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E5" s="9"/>
       <c r="F5" s="9"/>
@@ -4673,30 +4673,30 @@
       </c>
       <c r="H5" s="9"/>
       <c r="I5" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J5" s="9"/>
       <c r="K5" s="9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="L5" s="18" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="M5" s="9"/>
       <c r="N5" s="2"/>
     </row>
     <row r="6" spans="1:14" ht="58" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E6" s="9"/>
       <c r="F6" s="9"/>
@@ -4705,30 +4705,30 @@
       </c>
       <c r="H6" s="9"/>
       <c r="I6" s="9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J6" s="9"/>
       <c r="K6" s="9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="L6" s="18" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="M6" s="9"/>
       <c r="N6" s="2"/>
     </row>
     <row r="7" spans="1:14" ht="58" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
@@ -4737,30 +4737,30 @@
       </c>
       <c r="H7" s="9"/>
       <c r="I7" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J7" s="9"/>
       <c r="K7" s="9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="L7" s="18" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="M7" s="9"/>
       <c r="N7" s="2"/>
     </row>
     <row r="8" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E8" s="9"/>
       <c r="F8" s="9"/>
@@ -4769,30 +4769,30 @@
       </c>
       <c r="H8" s="9"/>
       <c r="I8" s="9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J8" s="9"/>
       <c r="K8" s="9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="L8" s="18" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="M8" s="9"/>
       <c r="N8" s="2"/>
     </row>
     <row r="9" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E9" s="9"/>
       <c r="F9" s="9"/>
@@ -4801,14 +4801,14 @@
       </c>
       <c r="H9" s="9"/>
       <c r="I9" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J9" s="9"/>
       <c r="K9" s="9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="L9" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="M9" s="9"/>
       <c r="N9" s="2"/>
@@ -4839,43 +4839,43 @@
   <sheetData>
     <row r="1" spans="1:14" s="24" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="20" t="s">
+        <v>284</v>
+      </c>
+      <c r="B1" s="21" t="s">
         <v>285</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="C1" s="16" t="s">
         <v>286</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="D1" s="21" t="s">
         <v>287</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="E1" s="22" t="s">
         <v>288</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="F1" s="22" t="s">
         <v>289</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="G1" s="16" t="s">
         <v>290</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="H1" s="21" t="s">
         <v>291</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="I1" s="21" t="s">
         <v>292</v>
       </c>
-      <c r="I1" s="21" t="s">
+      <c r="J1" s="21" t="s">
         <v>293</v>
       </c>
-      <c r="J1" s="21" t="s">
+      <c r="K1" s="23" t="s">
         <v>294</v>
       </c>
-      <c r="K1" s="23" t="s">
+      <c r="L1" s="21" t="s">
         <v>295</v>
       </c>
-      <c r="L1" s="21" t="s">
+      <c r="M1" s="21" t="s">
         <v>296</v>
-      </c>
-      <c r="M1" s="21" t="s">
-        <v>297</v>
       </c>
       <c r="N1" s="21"/>
     </row>
@@ -5089,7 +5089,7 @@
       <c r="M9" s="9"/>
       <c r="N9" s="2"/>
     </row>
-    <row r="10" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>73</v>
       </c>
@@ -5115,7 +5115,7 @@
       <c r="M10" s="9"/>
       <c r="N10" s="2"/>
     </row>
-    <row r="11" spans="1:14" ht="58" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>75</v>
       </c>
@@ -5141,7 +5141,7 @@
       <c r="M11" s="9"/>
       <c r="N11" s="2"/>
     </row>
-    <row r="12" spans="1:14" ht="58" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>77</v>
       </c>
@@ -5194,55 +5194,55 @@
   <sheetData>
     <row r="1" spans="1:14" s="24" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="20" t="s">
+        <v>284</v>
+      </c>
+      <c r="B1" s="21" t="s">
         <v>285</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="C1" s="16" t="s">
         <v>286</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="D1" s="21" t="s">
         <v>287</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="E1" s="22" t="s">
         <v>288</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="F1" s="22" t="s">
         <v>289</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="G1" s="16" t="s">
         <v>290</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="H1" s="21" t="s">
         <v>291</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="I1" s="21" t="s">
         <v>292</v>
       </c>
-      <c r="I1" s="21" t="s">
+      <c r="J1" s="21" t="s">
         <v>293</v>
       </c>
-      <c r="J1" s="21" t="s">
+      <c r="K1" s="23" t="s">
         <v>294</v>
       </c>
-      <c r="K1" s="23" t="s">
+      <c r="L1" s="21" t="s">
         <v>295</v>
       </c>
-      <c r="L1" s="21" t="s">
+      <c r="M1" s="21" t="s">
         <v>296</v>
-      </c>
-      <c r="M1" s="21" t="s">
-        <v>297</v>
       </c>
       <c r="N1" s="21"/>
     </row>
     <row r="2" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D2" s="9" t="s">
         <v>64</v>
@@ -5262,16 +5262,16 @@
     </row>
     <row r="3" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E3" s="9"/>
       <c r="F3" s="9"/>
@@ -5280,30 +5280,30 @@
       </c>
       <c r="H3" s="9"/>
       <c r="I3" s="9" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J3" s="9"/>
       <c r="K3" s="9" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="L3" s="18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="M3" s="9"/>
       <c r="N3" s="2"/>
     </row>
     <row r="4" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E4" s="9"/>
       <c r="F4" s="9"/>
@@ -5312,14 +5312,14 @@
       </c>
       <c r="H4" s="9"/>
       <c r="I4" s="9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J4" s="9"/>
       <c r="K4" s="9" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="L4" s="9" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="M4" s="9"/>
       <c r="N4" s="2"/>
@@ -5347,43 +5347,43 @@
   <sheetData>
     <row r="1" spans="1:14" s="24" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="20" t="s">
+        <v>284</v>
+      </c>
+      <c r="B1" s="21" t="s">
         <v>285</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="C1" s="16" t="s">
         <v>286</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="D1" s="21" t="s">
         <v>287</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="E1" s="22" t="s">
         <v>288</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="F1" s="22" t="s">
         <v>289</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="G1" s="16" t="s">
         <v>290</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="H1" s="21" t="s">
         <v>291</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="I1" s="21" t="s">
         <v>292</v>
       </c>
-      <c r="I1" s="21" t="s">
+      <c r="J1" s="21" t="s">
         <v>293</v>
       </c>
-      <c r="J1" s="21" t="s">
+      <c r="K1" s="23" t="s">
         <v>294</v>
       </c>
-      <c r="K1" s="23" t="s">
+      <c r="L1" s="21" t="s">
         <v>295</v>
       </c>
-      <c r="L1" s="21" t="s">
+      <c r="M1" s="21" t="s">
         <v>296</v>
-      </c>
-      <c r="M1" s="21" t="s">
-        <v>297</v>
       </c>
       <c r="N1" s="21"/>
     </row>
@@ -5484,50 +5484,51 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="18" customWidth="1"/>
+    <col min="3" max="3" width="21.7265625" customWidth="1"/>
     <col min="4" max="4" width="18.453125" customWidth="1"/>
     <col min="5" max="5" width="78.6328125" customWidth="1"/>
+    <col min="7" max="7" width="17.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="24" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="20" t="s">
+        <v>284</v>
+      </c>
+      <c r="B1" s="21" t="s">
         <v>285</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="C1" s="16" t="s">
         <v>286</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="D1" s="21" t="s">
         <v>287</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="E1" s="22" t="s">
         <v>288</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="F1" s="22" t="s">
         <v>289</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="G1" s="16" t="s">
         <v>290</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="H1" s="21" t="s">
         <v>291</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="I1" s="21" t="s">
         <v>292</v>
       </c>
-      <c r="I1" s="21" t="s">
+      <c r="J1" s="21" t="s">
         <v>293</v>
       </c>
-      <c r="J1" s="21" t="s">
+      <c r="K1" s="23" t="s">
         <v>294</v>
       </c>
-      <c r="K1" s="23" t="s">
+      <c r="L1" s="21" t="s">
         <v>295</v>
       </c>
-      <c r="L1" s="21" t="s">
+      <c r="M1" s="21" t="s">
         <v>296</v>
-      </c>
-      <c r="M1" s="21" t="s">
-        <v>297</v>
       </c>
       <c r="N1" s="21"/>
     </row>

</xml_diff>

<commit_message>
introduces pollution emission component
</commit_message>
<xml_diff>
--- a/dataland-framework-toolbox/inputs/sme/sme.xlsx
+++ b/dataland-framework-toolbox/inputs/sme/sme.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d92048\IdeaProjects\Dataland5\dataland-framework-toolbox\inputs\sme\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AACFCC4-0C62-412B-92DA-6CACD4E82399}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7645F185-D2D6-4652-97B8-4537AC7004B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C4E498E0-8E09-4328-BD54-6E3CD29DBCBD}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="892" uniqueCount="323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="887" uniqueCount="323">
   <si>
     <t>1</t>
   </si>
@@ -963,9 +963,6 @@
     <t>Subsidiary</t>
   </si>
   <si>
-    <t>Custom Component Pollution</t>
-  </si>
-  <si>
     <t>Custom Component Employees</t>
   </si>
   <si>
@@ -1026,13 +1023,16 @@
     <t>Cubic Meters</t>
   </si>
   <si>
-    <t>Dummy Value Please Delete</t>
-  </si>
-  <si>
     <t>Sme Subsidiary</t>
   </si>
   <si>
     <t>Total nature-oriented area off-site previous year</t>
+  </si>
+  <si>
+    <t>Sme Pollution Emission</t>
+  </si>
+  <si>
+    <t>Pollution Emission</t>
   </si>
 </sst>
 </file>
@@ -1113,7 +1113,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1128,18 +1128,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
-        <bgColor rgb="FFCCCCCC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FFCCCCCC"/>
       </patternFill>
     </fill>
@@ -1202,7 +1190,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
@@ -1288,37 +1276,6 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="5" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -1636,11 +1593,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DE53926-978F-4910-9169-F720F1E0A6DD}">
-  <dimension ref="A1:N94"/>
+  <dimension ref="A1:N93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1706,10 +1663,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="26" t="s">
+        <v>304</v>
+      </c>
+      <c r="C2" s="27" t="s">
         <v>305</v>
-      </c>
-      <c r="C2" s="27" t="s">
-        <v>306</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>3</v>
@@ -1736,10 +1693,10 @@
         <v>11</v>
       </c>
       <c r="B3" s="26" t="s">
+        <v>304</v>
+      </c>
+      <c r="C3" s="27" t="s">
         <v>305</v>
-      </c>
-      <c r="C3" s="27" t="s">
-        <v>306</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>298</v>
@@ -1749,7 +1706,7 @@
       </c>
       <c r="F3" s="5"/>
       <c r="G3" s="27" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
@@ -1764,10 +1721,10 @@
         <v>14</v>
       </c>
       <c r="B4" s="26" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C4" s="28" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>12</v>
@@ -1792,10 +1749,10 @@
         <v>19</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C5" s="28" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>15</v>
@@ -1822,10 +1779,10 @@
         <v>22</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C6" s="28" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>20</v>
@@ -1842,7 +1799,7 @@
         <v>18</v>
       </c>
       <c r="J6" s="11" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="K6" s="12"/>
       <c r="L6" s="11"/>
@@ -1854,10 +1811,10 @@
         <v>24</v>
       </c>
       <c r="B7" s="26" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C7" s="28" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>23</v>
@@ -1882,10 +1839,10 @@
         <v>26</v>
       </c>
       <c r="B8" s="26" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C8" s="28" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>25</v>
@@ -1910,10 +1867,10 @@
         <v>30</v>
       </c>
       <c r="B9" s="26" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C9" s="28" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>27</v>
@@ -1930,7 +1887,7 @@
         <v>29</v>
       </c>
       <c r="J9" s="11" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="K9" s="12"/>
       <c r="L9" s="11"/>
@@ -1942,10 +1899,10 @@
         <v>33</v>
       </c>
       <c r="B10" s="26" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C10" s="28" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>31</v>
@@ -1962,7 +1919,7 @@
         <v>29</v>
       </c>
       <c r="J10" s="11" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="K10" s="12"/>
       <c r="L10" s="11"/>
@@ -1974,10 +1931,10 @@
         <v>36</v>
       </c>
       <c r="B11" s="26" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C11" s="28" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>34</v>
@@ -1994,7 +1951,7 @@
         <v>29</v>
       </c>
       <c r="J11" s="11" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="K11" s="12"/>
       <c r="L11" s="11"/>
@@ -2006,10 +1963,10 @@
         <v>39</v>
       </c>
       <c r="B12" s="26" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C12" s="28" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>37</v>
@@ -2026,7 +1983,7 @@
         <v>29</v>
       </c>
       <c r="J12" s="11" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="K12" s="12"/>
       <c r="L12" s="11"/>
@@ -2038,18 +1995,20 @@
         <v>42</v>
       </c>
       <c r="B13" s="26" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C13" s="28" t="s">
-        <v>309</v>
-      </c>
-      <c r="D13" s="3"/>
+        <v>308</v>
+      </c>
+      <c r="D13" s="27" t="s">
+        <v>322</v>
+      </c>
       <c r="E13" s="9" t="s">
         <v>41</v>
       </c>
       <c r="F13" s="10"/>
       <c r="G13" s="19" t="s">
-        <v>299</v>
+        <v>321</v>
       </c>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
@@ -2059,72 +2018,72 @@
       <c r="M13" s="3"/>
       <c r="N13" s="2"/>
     </row>
-    <row r="14" spans="1:14" s="41" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A14" s="31" t="s">
-        <v>45</v>
-      </c>
-      <c r="B14" s="32" t="s">
-        <v>305</v>
-      </c>
-      <c r="C14" s="33" t="s">
+    <row r="14" spans="1:14" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" s="26" t="s">
+        <v>304</v>
+      </c>
+      <c r="C14" s="28" t="s">
         <v>309</v>
       </c>
-      <c r="D14" s="34" t="s">
-        <v>320</v>
-      </c>
-      <c r="E14" s="33" t="s">
-        <v>320</v>
-      </c>
-      <c r="F14" s="35"/>
-      <c r="G14" s="36" t="s">
-        <v>9</v>
-      </c>
-      <c r="H14" s="37"/>
-      <c r="I14" s="37"/>
-      <c r="J14" s="37"/>
-      <c r="K14" s="38"/>
-      <c r="L14" s="39"/>
-      <c r="M14" s="37"/>
-      <c r="N14" s="40"/>
-    </row>
-    <row r="15" spans="1:14" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="D14" s="3"/>
+      <c r="E14" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="F14" s="10"/>
+      <c r="G14" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="12"/>
+      <c r="L14" s="11"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="2"/>
+    </row>
+    <row r="15" spans="1:14" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B15" s="26" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C15" s="28" t="s">
-        <v>310</v>
-      </c>
-      <c r="D15" s="3"/>
+        <v>309</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>84</v>
+      </c>
       <c r="E15" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="F15" s="10"/>
-      <c r="G15" s="3" t="s">
-        <v>301</v>
-      </c>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="11"/>
-      <c r="K15" s="12"/>
-      <c r="L15" s="11"/>
-      <c r="M15" s="3"/>
+        <v>82</v>
+      </c>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
+      <c r="L15" s="9"/>
+      <c r="M15" s="9"/>
       <c r="N15" s="2"/>
     </row>
     <row r="16" spans="1:14" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B16" s="26" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C16" s="28" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="E16" s="9" t="s">
         <v>82</v>
@@ -2142,24 +2101,24 @@
       <c r="N16" s="2"/>
     </row>
     <row r="17" spans="1:14" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="1" t="s">
-        <v>55</v>
+      <c r="A17" s="30" t="s">
+        <v>57</v>
       </c>
       <c r="B17" s="26" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C17" s="28" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="E17" s="9" t="s">
         <v>82</v>
       </c>
       <c r="F17" s="9"/>
       <c r="G17" s="9" t="s">
-        <v>17</v>
+        <v>89</v>
       </c>
       <c r="H17" s="9"/>
       <c r="I17" s="9"/>
@@ -2170,24 +2129,24 @@
       <c r="N17" s="2"/>
     </row>
     <row r="18" spans="1:14" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="30" t="s">
-        <v>57</v>
+      <c r="A18" s="1" t="s">
+        <v>59</v>
       </c>
       <c r="B18" s="26" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C18" s="28" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="E18" s="9" t="s">
         <v>82</v>
       </c>
       <c r="F18" s="9"/>
       <c r="G18" s="9" t="s">
-        <v>89</v>
+        <v>17</v>
       </c>
       <c r="H18" s="9"/>
       <c r="I18" s="9"/>
@@ -2199,16 +2158,16 @@
     </row>
     <row r="19" spans="1:14" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B19" s="26" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C19" s="28" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="E19" s="9" t="s">
         <v>82</v>
@@ -2227,23 +2186,23 @@
     </row>
     <row r="20" spans="1:14" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B20" s="26" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C20" s="28" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="E20" s="9" t="s">
         <v>82</v>
       </c>
       <c r="F20" s="9"/>
       <c r="G20" s="9" t="s">
-        <v>17</v>
+        <v>89</v>
       </c>
       <c r="H20" s="9"/>
       <c r="I20" s="9"/>
@@ -2254,24 +2213,24 @@
       <c r="N20" s="2"/>
     </row>
     <row r="21" spans="1:14" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A21" s="1" t="s">
-        <v>63</v>
+      <c r="A21" s="30" t="s">
+        <v>66</v>
       </c>
       <c r="B21" s="26" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C21" s="28" t="s">
-        <v>310</v>
-      </c>
-      <c r="D21" s="9" t="s">
-        <v>95</v>
+        <v>309</v>
+      </c>
+      <c r="D21" s="28" t="s">
+        <v>320</v>
       </c>
       <c r="E21" s="9" t="s">
         <v>82</v>
       </c>
       <c r="F21" s="9"/>
       <c r="G21" s="9" t="s">
-        <v>89</v>
+        <v>17</v>
       </c>
       <c r="H21" s="9"/>
       <c r="I21" s="9"/>
@@ -2282,17 +2241,17 @@
       <c r="N21" s="2"/>
     </row>
     <row r="22" spans="1:14" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A22" s="30" t="s">
-        <v>66</v>
+      <c r="A22" s="1" t="s">
+        <v>69</v>
       </c>
       <c r="B22" s="26" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C22" s="28" t="s">
-        <v>310</v>
-      </c>
-      <c r="D22" s="28" t="s">
-        <v>322</v>
+        <v>309</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>98</v>
       </c>
       <c r="E22" s="9" t="s">
         <v>82</v>
@@ -2311,23 +2270,23 @@
     </row>
     <row r="23" spans="1:14" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B23" s="26" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C23" s="28" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E23" s="9" t="s">
         <v>82</v>
       </c>
       <c r="F23" s="9"/>
       <c r="G23" s="9" t="s">
-        <v>17</v>
+        <v>89</v>
       </c>
       <c r="H23" s="9"/>
       <c r="I23" s="9"/>
@@ -2339,23 +2298,23 @@
     </row>
     <row r="24" spans="1:14" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B24" s="26" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C24" s="28" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="E24" s="9" t="s">
         <v>82</v>
       </c>
       <c r="F24" s="9"/>
       <c r="G24" s="9" t="s">
-        <v>89</v>
+        <v>17</v>
       </c>
       <c r="H24" s="9"/>
       <c r="I24" s="9"/>
@@ -2366,17 +2325,17 @@
       <c r="N24" s="2"/>
     </row>
     <row r="25" spans="1:14" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A25" s="1" t="s">
-        <v>73</v>
+      <c r="A25" s="30" t="s">
+        <v>75</v>
       </c>
       <c r="B25" s="26" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C25" s="28" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="E25" s="9" t="s">
         <v>82</v>
@@ -2394,24 +2353,24 @@
       <c r="N25" s="2"/>
     </row>
     <row r="26" spans="1:14" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A26" s="30" t="s">
-        <v>75</v>
+      <c r="A26" s="1" t="s">
+        <v>77</v>
       </c>
       <c r="B26" s="26" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C26" s="28" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="E26" s="9" t="s">
         <v>82</v>
       </c>
       <c r="F26" s="9"/>
       <c r="G26" s="9" t="s">
-        <v>17</v>
+        <v>89</v>
       </c>
       <c r="H26" s="9"/>
       <c r="I26" s="9"/>
@@ -2421,87 +2380,89 @@
       <c r="M26" s="9"/>
       <c r="N26" s="2"/>
     </row>
-    <row r="27" spans="1:14" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:14" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="B27" s="26" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C27" s="28" t="s">
-        <v>310</v>
+        <v>315</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>82</v>
+        <v>109</v>
       </c>
       <c r="F27" s="9"/>
       <c r="G27" s="9" t="s">
-        <v>89</v>
+        <v>17</v>
       </c>
       <c r="H27" s="9"/>
-      <c r="I27" s="9"/>
-      <c r="J27" s="9"/>
+      <c r="I27" s="29" t="s">
+        <v>318</v>
+      </c>
+      <c r="J27" s="11" t="s">
+        <v>316</v>
+      </c>
       <c r="K27" s="9"/>
       <c r="L27" s="9"/>
       <c r="M27" s="9"/>
       <c r="N27" s="2"/>
     </row>
-    <row r="28" spans="1:14" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B28" s="26" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C28" s="28" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="E28" s="9" t="s">
-        <v>109</v>
-      </c>
+        <v>112</v>
+      </c>
+      <c r="E28" s="9"/>
       <c r="F28" s="9"/>
       <c r="G28" s="9" t="s">
         <v>17</v>
       </c>
       <c r="H28" s="9"/>
       <c r="I28" s="29" t="s">
-        <v>319</v>
-      </c>
-      <c r="J28" s="11" t="s">
-        <v>317</v>
-      </c>
+        <v>318</v>
+      </c>
+      <c r="J28" s="9"/>
       <c r="K28" s="9"/>
       <c r="L28" s="9"/>
       <c r="M28" s="9"/>
       <c r="N28" s="2"/>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A29" s="1" t="s">
-        <v>83</v>
+    <row r="29" spans="1:14" ht="131.5" x14ac:dyDescent="0.35">
+      <c r="A29" s="30" t="s">
+        <v>85</v>
       </c>
       <c r="B29" s="26" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C29" s="28" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="E29" s="9"/>
+        <v>114</v>
+      </c>
+      <c r="E29" s="9" t="s">
+        <v>297</v>
+      </c>
       <c r="F29" s="9"/>
       <c r="G29" s="9" t="s">
         <v>17</v>
       </c>
       <c r="H29" s="9"/>
       <c r="I29" s="29" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="J29" s="9"/>
       <c r="K29" s="9"/>
@@ -2509,29 +2470,27 @@
       <c r="M29" s="9"/>
       <c r="N29" s="2"/>
     </row>
-    <row r="30" spans="1:14" ht="131.5" x14ac:dyDescent="0.35">
-      <c r="A30" s="30" t="s">
-        <v>85</v>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A30" s="1" t="s">
+        <v>87</v>
       </c>
       <c r="B30" s="26" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C30" s="28" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="E30" s="9" t="s">
-        <v>297</v>
-      </c>
+        <v>116</v>
+      </c>
+      <c r="E30" s="9"/>
       <c r="F30" s="9"/>
       <c r="G30" s="9" t="s">
         <v>17</v>
       </c>
       <c r="H30" s="9"/>
       <c r="I30" s="29" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="J30" s="9"/>
       <c r="K30" s="9"/>
@@ -2541,16 +2500,16 @@
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="B31" s="26" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C31" s="28" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="E31" s="9"/>
       <c r="F31" s="9"/>
@@ -2559,7 +2518,7 @@
       </c>
       <c r="H31" s="9"/>
       <c r="I31" s="29" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="J31" s="9"/>
       <c r="K31" s="9"/>
@@ -2569,16 +2528,16 @@
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B32" s="26" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C32" s="28" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="E32" s="9"/>
       <c r="F32" s="9"/>
@@ -2587,7 +2546,7 @@
       </c>
       <c r="H32" s="9"/>
       <c r="I32" s="29" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="J32" s="9"/>
       <c r="K32" s="9"/>
@@ -2596,17 +2555,17 @@
       <c r="N32" s="2"/>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A33" s="1" t="s">
-        <v>92</v>
+      <c r="A33" s="30" t="s">
+        <v>94</v>
       </c>
       <c r="B33" s="26" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C33" s="28" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="E33" s="9"/>
       <c r="F33" s="9"/>
@@ -2615,7 +2574,7 @@
       </c>
       <c r="H33" s="9"/>
       <c r="I33" s="29" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="J33" s="9"/>
       <c r="K33" s="9"/>
@@ -2623,18 +2582,18 @@
       <c r="M33" s="9"/>
       <c r="N33" s="2"/>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A34" s="30" t="s">
-        <v>94</v>
+    <row r="34" spans="1:14" ht="29" x14ac:dyDescent="0.35">
+      <c r="A34" s="1" t="s">
+        <v>96</v>
       </c>
       <c r="B34" s="26" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C34" s="28" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="E34" s="9"/>
       <c r="F34" s="9"/>
@@ -2643,7 +2602,7 @@
       </c>
       <c r="H34" s="9"/>
       <c r="I34" s="29" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="J34" s="9"/>
       <c r="K34" s="9"/>
@@ -2651,27 +2610,29 @@
       <c r="M34" s="9"/>
       <c r="N34" s="2"/>
     </row>
-    <row r="35" spans="1:14" ht="29" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:14" ht="391.5" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B35" s="26" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C35" s="28" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>124</v>
-      </c>
-      <c r="E35" s="9"/>
+        <v>127</v>
+      </c>
+      <c r="E35" s="9" t="s">
+        <v>128</v>
+      </c>
       <c r="F35" s="9"/>
       <c r="G35" s="9" t="s">
         <v>17</v>
       </c>
       <c r="H35" s="9"/>
-      <c r="I35" s="29" t="s">
-        <v>319</v>
+      <c r="I35" s="9" t="s">
+        <v>129</v>
       </c>
       <c r="J35" s="9"/>
       <c r="K35" s="9"/>
@@ -2679,22 +2640,20 @@
       <c r="M35" s="9"/>
       <c r="N35" s="2"/>
     </row>
-    <row r="36" spans="1:14" ht="391.5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B36" s="26" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C36" s="28" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>127</v>
-      </c>
-      <c r="E36" s="9" t="s">
-        <v>128</v>
-      </c>
+        <v>131</v>
+      </c>
+      <c r="E36" s="9"/>
       <c r="F36" s="9"/>
       <c r="G36" s="9" t="s">
         <v>17</v>
@@ -2710,27 +2669,25 @@
       <c r="N36" s="2"/>
     </row>
     <row r="37" spans="1:14" ht="29" x14ac:dyDescent="0.35">
-      <c r="A37" s="1" t="s">
-        <v>99</v>
+      <c r="A37" s="30" t="s">
+        <v>101</v>
       </c>
       <c r="B37" s="26" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C37" s="28" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="E37" s="9"/>
       <c r="F37" s="9"/>
       <c r="G37" s="9" t="s">
-        <v>17</v>
+        <v>89</v>
       </c>
       <c r="H37" s="9"/>
-      <c r="I37" s="9" t="s">
-        <v>129</v>
-      </c>
+      <c r="I37" s="9"/>
       <c r="J37" s="9"/>
       <c r="K37" s="9"/>
       <c r="L37" s="9"/>
@@ -2738,25 +2695,27 @@
       <c r="N37" s="2"/>
     </row>
     <row r="38" spans="1:14" ht="29" x14ac:dyDescent="0.35">
-      <c r="A38" s="30" t="s">
-        <v>101</v>
+      <c r="A38" s="1" t="s">
+        <v>103</v>
       </c>
       <c r="B38" s="26" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C38" s="28" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="E38" s="9"/>
       <c r="F38" s="9"/>
       <c r="G38" s="9" t="s">
-        <v>89</v>
+        <v>17</v>
       </c>
       <c r="H38" s="9"/>
-      <c r="I38" s="9"/>
+      <c r="I38" s="9" t="s">
+        <v>129</v>
+      </c>
       <c r="J38" s="9"/>
       <c r="K38" s="9"/>
       <c r="L38" s="9"/>
@@ -2765,154 +2724,160 @@
     </row>
     <row r="39" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B39" s="26" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C39" s="28" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>135</v>
+        <v>302</v>
       </c>
       <c r="E39" s="9"/>
       <c r="F39" s="9"/>
       <c r="G39" s="9" t="s">
-        <v>17</v>
+        <v>89</v>
       </c>
       <c r="H39" s="9"/>
-      <c r="I39" s="9" t="s">
-        <v>129</v>
-      </c>
+      <c r="I39" s="9"/>
       <c r="J39" s="9"/>
       <c r="K39" s="9"/>
       <c r="L39" s="9"/>
       <c r="M39" s="9"/>
       <c r="N39" s="2"/>
     </row>
-    <row r="40" spans="1:14" ht="29" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:14" ht="174" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B40" s="26" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C40" s="28" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D40" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="E40" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="F40" s="9"/>
+      <c r="G40" s="25" t="s">
         <v>303</v>
       </c>
-      <c r="E40" s="9"/>
-      <c r="F40" s="9"/>
-      <c r="G40" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="H40" s="9"/>
+      <c r="H40" s="9" t="s">
+        <v>140</v>
+      </c>
       <c r="I40" s="9"/>
-      <c r="J40" s="9"/>
+      <c r="J40" s="2"/>
       <c r="K40" s="9"/>
       <c r="L40" s="9"/>
       <c r="M40" s="9"/>
       <c r="N40" s="2"/>
     </row>
-    <row r="41" spans="1:14" ht="174" x14ac:dyDescent="0.35">
-      <c r="A41" s="1" t="s">
-        <v>107</v>
+    <row r="41" spans="1:14" ht="29" x14ac:dyDescent="0.35">
+      <c r="A41" s="30" t="s">
+        <v>111</v>
       </c>
       <c r="B41" s="26" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C41" s="28" t="s">
-        <v>315</v>
-      </c>
-      <c r="D41" s="9" t="s">
-        <v>138</v>
-      </c>
-      <c r="E41" s="9" t="s">
-        <v>139</v>
-      </c>
+        <v>314</v>
+      </c>
+      <c r="D41" s="9"/>
+      <c r="E41" s="9"/>
       <c r="F41" s="9"/>
-      <c r="G41" s="25" t="s">
-        <v>304</v>
-      </c>
-      <c r="H41" s="9" t="s">
-        <v>140</v>
-      </c>
+      <c r="G41" s="8" t="s">
+        <v>301</v>
+      </c>
+      <c r="H41" s="9"/>
       <c r="I41" s="9"/>
-      <c r="J41" s="2"/>
+      <c r="J41" s="9"/>
       <c r="K41" s="9"/>
       <c r="L41" s="9"/>
       <c r="M41" s="9"/>
       <c r="N41" s="2"/>
     </row>
-    <row r="42" spans="1:14" ht="29" x14ac:dyDescent="0.35">
-      <c r="A42" s="30" t="s">
-        <v>111</v>
+    <row r="42" spans="1:14" ht="116" x14ac:dyDescent="0.35">
+      <c r="A42" s="1" t="s">
+        <v>113</v>
       </c>
       <c r="B42" s="26" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C42" s="28" t="s">
-        <v>315</v>
-      </c>
-      <c r="D42" s="9"/>
-      <c r="E42" s="9"/>
+        <v>313</v>
+      </c>
+      <c r="D42" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="E42" s="9" t="s">
+        <v>164</v>
+      </c>
       <c r="F42" s="9"/>
-      <c r="G42" s="8" t="s">
-        <v>302</v>
-      </c>
-      <c r="H42" s="9"/>
+      <c r="G42" s="25" t="s">
+        <v>303</v>
+      </c>
+      <c r="H42" s="9" t="s">
+        <v>165</v>
+      </c>
       <c r="I42" s="9"/>
       <c r="J42" s="9"/>
       <c r="K42" s="9"/>
-      <c r="L42" s="9"/>
+      <c r="L42" s="18"/>
       <c r="M42" s="9"/>
       <c r="N42" s="2"/>
     </row>
-    <row r="43" spans="1:14" ht="116" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B43" s="26" t="s">
+        <v>304</v>
+      </c>
+      <c r="C43" s="28" t="s">
+        <v>313</v>
+      </c>
+      <c r="D43" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="E43" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="F43" s="9"/>
+      <c r="G43" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="H43" s="9"/>
+      <c r="I43" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="J43" s="9"/>
+      <c r="K43" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B43" s="26" t="s">
-        <v>305</v>
-      </c>
-      <c r="C43" s="28" t="s">
-        <v>314</v>
-      </c>
-      <c r="D43" s="9" t="s">
-        <v>163</v>
-      </c>
-      <c r="E43" s="9" t="s">
-        <v>164</v>
-      </c>
-      <c r="F43" s="9"/>
-      <c r="G43" s="25" t="s">
-        <v>304</v>
-      </c>
-      <c r="H43" s="9" t="s">
-        <v>165</v>
-      </c>
-      <c r="I43" s="9"/>
-      <c r="J43" s="9"/>
-      <c r="K43" s="9"/>
-      <c r="L43" s="18"/>
+      <c r="L43" s="18" t="s">
+        <v>170</v>
+      </c>
       <c r="M43" s="9"/>
       <c r="N43" s="2"/>
     </row>
     <row r="44" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B44" s="26" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C44" s="28" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D44" s="9" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="E44" s="9" t="s">
         <v>168</v>
@@ -2923,33 +2888,33 @@
       </c>
       <c r="H44" s="9"/>
       <c r="I44" s="9" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="J44" s="9"/>
       <c r="K44" s="1" t="s">
         <v>113</v>
       </c>
       <c r="L44" s="18" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="M44" s="9"/>
       <c r="N44" s="2"/>
     </row>
-    <row r="45" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A45" s="1" t="s">
-        <v>117</v>
+    <row r="45" spans="1:14" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A45" s="30" t="s">
+        <v>119</v>
       </c>
       <c r="B45" s="26" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C45" s="28" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D45" s="9" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="E45" s="9" t="s">
-        <v>168</v>
+        <v>177</v>
       </c>
       <c r="F45" s="9"/>
       <c r="G45" s="9" t="s">
@@ -2957,30 +2922,30 @@
       </c>
       <c r="H45" s="9"/>
       <c r="I45" s="9" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="J45" s="9"/>
       <c r="K45" s="1" t="s">
         <v>113</v>
       </c>
       <c r="L45" s="18" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="M45" s="9"/>
       <c r="N45" s="2"/>
     </row>
     <row r="46" spans="1:14" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A46" s="30" t="s">
-        <v>119</v>
+      <c r="A46" s="1" t="s">
+        <v>121</v>
       </c>
       <c r="B46" s="26" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C46" s="28" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D46" s="9" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="E46" s="9" t="s">
         <v>177</v>
@@ -2991,64 +2956,62 @@
       </c>
       <c r="H46" s="9"/>
       <c r="I46" s="9" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="J46" s="9"/>
       <c r="K46" s="1" t="s">
         <v>113</v>
       </c>
       <c r="L46" s="18" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="M46" s="9"/>
       <c r="N46" s="2"/>
     </row>
-    <row r="47" spans="1:14" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B47" s="26" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C47" s="28" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D47" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="E47" s="9" t="s">
-        <v>177</v>
-      </c>
+        <v>181</v>
+      </c>
+      <c r="E47" s="9"/>
       <c r="F47" s="9"/>
       <c r="G47" s="9" t="s">
         <v>17</v>
       </c>
       <c r="H47" s="9"/>
       <c r="I47" s="9" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="J47" s="9"/>
       <c r="K47" s="1" t="s">
         <v>113</v>
       </c>
       <c r="L47" s="18" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="M47" s="9"/>
       <c r="N47" s="2"/>
     </row>
-    <row r="48" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B48" s="26" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C48" s="28" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D48" s="9" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="E48" s="9"/>
       <c r="F48" s="9"/>
@@ -3057,62 +3020,64 @@
       </c>
       <c r="H48" s="9"/>
       <c r="I48" s="9" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="J48" s="9"/>
       <c r="K48" s="1" t="s">
         <v>113</v>
       </c>
       <c r="L48" s="18" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="M48" s="9"/>
       <c r="N48" s="2"/>
     </row>
-    <row r="49" spans="1:14" ht="29" x14ac:dyDescent="0.35">
-      <c r="A49" s="1" t="s">
-        <v>125</v>
+    <row r="49" spans="1:14" ht="87" x14ac:dyDescent="0.35">
+      <c r="A49" s="30" t="s">
+        <v>130</v>
       </c>
       <c r="B49" s="26" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C49" s="28" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D49" s="9" t="s">
-        <v>183</v>
-      </c>
-      <c r="E49" s="9"/>
+        <v>185</v>
+      </c>
+      <c r="E49" s="9" t="s">
+        <v>186</v>
+      </c>
       <c r="F49" s="9"/>
       <c r="G49" s="9" t="s">
         <v>17</v>
       </c>
       <c r="H49" s="9"/>
       <c r="I49" s="9" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="J49" s="9"/>
       <c r="K49" s="1" t="s">
         <v>113</v>
       </c>
       <c r="L49" s="18" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="M49" s="9"/>
       <c r="N49" s="2"/>
     </row>
     <row r="50" spans="1:14" ht="87" x14ac:dyDescent="0.35">
-      <c r="A50" s="30" t="s">
-        <v>130</v>
+      <c r="A50" s="1" t="s">
+        <v>132</v>
       </c>
       <c r="B50" s="26" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C50" s="28" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D50" s="9" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="E50" s="9" t="s">
         <v>186</v>
@@ -3123,64 +3088,62 @@
       </c>
       <c r="H50" s="9"/>
       <c r="I50" s="9" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="J50" s="9"/>
       <c r="K50" s="1" t="s">
         <v>113</v>
       </c>
       <c r="L50" s="18" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="M50" s="9"/>
       <c r="N50" s="2"/>
     </row>
-    <row r="51" spans="1:14" ht="87" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B51" s="26" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C51" s="28" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D51" s="9" t="s">
-        <v>188</v>
-      </c>
-      <c r="E51" s="9" t="s">
-        <v>186</v>
-      </c>
+        <v>190</v>
+      </c>
+      <c r="E51" s="9"/>
       <c r="F51" s="9"/>
       <c r="G51" s="9" t="s">
         <v>17</v>
       </c>
       <c r="H51" s="9"/>
       <c r="I51" s="9" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="J51" s="9"/>
       <c r="K51" s="1" t="s">
         <v>113</v>
       </c>
       <c r="L51" s="18" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="M51" s="9"/>
       <c r="N51" s="2"/>
     </row>
-    <row r="52" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B52" s="26" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C52" s="28" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D52" s="9" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="E52" s="9"/>
       <c r="F52" s="9"/>
@@ -3189,30 +3152,30 @@
       </c>
       <c r="H52" s="9"/>
       <c r="I52" s="9" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="J52" s="9"/>
       <c r="K52" s="1" t="s">
         <v>113</v>
       </c>
       <c r="L52" s="18" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="M52" s="9"/>
       <c r="N52" s="2"/>
     </row>
-    <row r="53" spans="1:14" ht="29" x14ac:dyDescent="0.35">
-      <c r="A53" s="1" t="s">
-        <v>136</v>
+    <row r="53" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A53" s="30" t="s">
+        <v>137</v>
       </c>
       <c r="B53" s="26" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C53" s="28" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D53" s="9" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="E53" s="9"/>
       <c r="F53" s="9"/>
@@ -3221,30 +3184,30 @@
       </c>
       <c r="H53" s="9"/>
       <c r="I53" s="9" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="J53" s="9"/>
       <c r="K53" s="1" t="s">
         <v>113</v>
       </c>
       <c r="L53" s="18" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="M53" s="9"/>
       <c r="N53" s="2"/>
     </row>
-    <row r="54" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A54" s="30" t="s">
-        <v>137</v>
+    <row r="54" spans="1:14" ht="29" x14ac:dyDescent="0.35">
+      <c r="A54" s="1" t="s">
+        <v>141</v>
       </c>
       <c r="B54" s="26" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C54" s="28" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D54" s="9" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="E54" s="9"/>
       <c r="F54" s="9"/>
@@ -3253,30 +3216,30 @@
       </c>
       <c r="H54" s="9"/>
       <c r="I54" s="9" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="J54" s="9"/>
       <c r="K54" s="1" t="s">
         <v>113</v>
       </c>
       <c r="L54" s="18" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="M54" s="9"/>
       <c r="N54" s="2"/>
     </row>
-    <row r="55" spans="1:14" ht="29" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B55" s="26" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C55" s="28" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D55" s="9" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="E55" s="9"/>
       <c r="F55" s="9"/>
@@ -3285,102 +3248,100 @@
       </c>
       <c r="H55" s="9"/>
       <c r="I55" s="9" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="J55" s="9"/>
       <c r="K55" s="1" t="s">
         <v>113</v>
       </c>
       <c r="L55" s="18" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="M55" s="9"/>
       <c r="N55" s="2"/>
     </row>
-    <row r="56" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="B56" s="26" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C56" s="28" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D56" s="9" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="E56" s="9"/>
       <c r="F56" s="9"/>
-      <c r="G56" s="9" t="s">
+      <c r="G56" s="19" t="s">
         <v>17</v>
       </c>
       <c r="H56" s="9"/>
       <c r="I56" s="9" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="J56" s="9"/>
       <c r="K56" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="L56" s="18" t="s">
-        <v>170</v>
+      <c r="L56" s="9" t="s">
+        <v>174</v>
       </c>
       <c r="M56" s="9"/>
       <c r="N56" s="2"/>
     </row>
-    <row r="57" spans="1:14" ht="29" x14ac:dyDescent="0.35">
-      <c r="A57" s="1" t="s">
-        <v>145</v>
+    <row r="57" spans="1:14" ht="87" x14ac:dyDescent="0.35">
+      <c r="A57" s="30" t="s">
+        <v>147</v>
       </c>
       <c r="B57" s="26" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C57" s="28" t="s">
-        <v>314</v>
-      </c>
-      <c r="D57" s="9" t="s">
-        <v>200</v>
-      </c>
-      <c r="E57" s="9"/>
+        <v>313</v>
+      </c>
+      <c r="D57" s="9"/>
+      <c r="E57" s="9" t="s">
+        <v>202</v>
+      </c>
       <c r="F57" s="9"/>
       <c r="G57" s="19" t="s">
-        <v>17</v>
+        <v>299</v>
       </c>
       <c r="H57" s="9"/>
-      <c r="I57" s="9" t="s">
-        <v>173</v>
-      </c>
+      <c r="I57" s="9"/>
       <c r="J57" s="9"/>
-      <c r="K57" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="L57" s="9" t="s">
-        <v>174</v>
-      </c>
+      <c r="K57" s="9"/>
+      <c r="L57" s="9"/>
       <c r="M57" s="9"/>
       <c r="N57" s="2"/>
     </row>
-    <row r="58" spans="1:14" ht="87" x14ac:dyDescent="0.35">
-      <c r="A58" s="30" t="s">
-        <v>147</v>
+    <row r="58" spans="1:14" ht="58" x14ac:dyDescent="0.35">
+      <c r="A58" s="1" t="s">
+        <v>150</v>
       </c>
       <c r="B58" s="26" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C58" s="28" t="s">
-        <v>314</v>
-      </c>
-      <c r="D58" s="9"/>
+        <v>312</v>
+      </c>
+      <c r="D58" s="9" t="s">
+        <v>209</v>
+      </c>
       <c r="E58" s="9" t="s">
-        <v>202</v>
+        <v>210</v>
       </c>
       <c r="F58" s="9"/>
-      <c r="G58" s="19" t="s">
-        <v>300</v>
+      <c r="G58" s="9" t="s">
+        <v>17</v>
       </c>
       <c r="H58" s="9"/>
-      <c r="I58" s="9"/>
+      <c r="I58" s="9" t="s">
+        <v>211</v>
+      </c>
       <c r="J58" s="9"/>
       <c r="K58" s="9"/>
       <c r="L58" s="9"/>
@@ -3389,102 +3350,106 @@
     </row>
     <row r="59" spans="1:14" ht="58" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="B59" s="26" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C59" s="28" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D59" s="9" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="E59" s="9" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="F59" s="9"/>
       <c r="G59" s="9" t="s">
-        <v>17</v>
+        <v>215</v>
       </c>
       <c r="H59" s="9"/>
-      <c r="I59" s="9" t="s">
-        <v>211</v>
-      </c>
+      <c r="I59" s="9"/>
       <c r="J59" s="9"/>
       <c r="K59" s="9"/>
       <c r="L59" s="9"/>
       <c r="M59" s="9"/>
       <c r="N59" s="2"/>
     </row>
-    <row r="60" spans="1:14" ht="58" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:14" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B60" s="26" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C60" s="28" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D60" s="9" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="E60" s="9" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="F60" s="9"/>
       <c r="G60" s="9" t="s">
-        <v>215</v>
+        <v>17</v>
       </c>
       <c r="H60" s="9"/>
       <c r="I60" s="9"/>
       <c r="J60" s="9"/>
       <c r="K60" s="9"/>
-      <c r="L60" s="9"/>
+      <c r="L60" s="18"/>
       <c r="M60" s="9"/>
       <c r="N60" s="2"/>
     </row>
-    <row r="61" spans="1:14" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A61" s="1" t="s">
-        <v>155</v>
+    <row r="61" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A61" s="30" t="s">
+        <v>157</v>
       </c>
       <c r="B61" s="26" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C61" s="28" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D61" s="9" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="E61" s="9" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="F61" s="9"/>
       <c r="G61" s="9" t="s">
-        <v>17</v>
+        <v>215</v>
       </c>
       <c r="H61" s="9"/>
-      <c r="I61" s="9"/>
+      <c r="I61" s="9" t="s">
+        <v>169</v>
+      </c>
       <c r="J61" s="9"/>
-      <c r="K61" s="9"/>
-      <c r="L61" s="18"/>
+      <c r="K61" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="L61" s="18" t="s">
+        <v>170</v>
+      </c>
       <c r="M61" s="9"/>
       <c r="N61" s="2"/>
     </row>
     <row r="62" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A62" s="30" t="s">
-        <v>157</v>
+      <c r="A62" s="1" t="s">
+        <v>159</v>
       </c>
       <c r="B62" s="26" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C62" s="28" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D62" s="9" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="E62" s="9" t="s">
         <v>221</v>
@@ -3495,33 +3460,33 @@
       </c>
       <c r="H62" s="9"/>
       <c r="I62" s="9" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="J62" s="9"/>
       <c r="K62" s="1" t="s">
         <v>113</v>
       </c>
       <c r="L62" s="18" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="M62" s="9"/>
       <c r="N62" s="2"/>
     </row>
-    <row r="63" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:14" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="B63" s="26" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C63" s="28" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D63" s="9" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="E63" s="9" t="s">
-        <v>221</v>
+        <v>226</v>
       </c>
       <c r="F63" s="9"/>
       <c r="G63" s="9" t="s">
@@ -3529,30 +3494,30 @@
       </c>
       <c r="H63" s="9"/>
       <c r="I63" s="9" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="J63" s="9"/>
       <c r="K63" s="1" t="s">
         <v>113</v>
       </c>
       <c r="L63" s="18" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="M63" s="9"/>
       <c r="N63" s="2"/>
     </row>
     <row r="64" spans="1:14" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="B64" s="26" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C64" s="28" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D64" s="9" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="E64" s="9" t="s">
         <v>226</v>
@@ -3563,64 +3528,62 @@
       </c>
       <c r="H64" s="9"/>
       <c r="I64" s="9" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="J64" s="9"/>
       <c r="K64" s="1" t="s">
         <v>113</v>
       </c>
       <c r="L64" s="18" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="M64" s="9"/>
       <c r="N64" s="2"/>
     </row>
-    <row r="65" spans="1:14" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A65" s="1" t="s">
-        <v>166</v>
+    <row r="65" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A65" s="30" t="s">
+        <v>171</v>
       </c>
       <c r="B65" s="26" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C65" s="28" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D65" s="9" t="s">
-        <v>228</v>
-      </c>
-      <c r="E65" s="9" t="s">
-        <v>226</v>
-      </c>
+        <v>230</v>
+      </c>
+      <c r="E65" s="9"/>
       <c r="F65" s="9"/>
       <c r="G65" s="9" t="s">
         <v>215</v>
       </c>
       <c r="H65" s="9"/>
       <c r="I65" s="9" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="J65" s="9"/>
       <c r="K65" s="1" t="s">
         <v>113</v>
       </c>
       <c r="L65" s="18" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="M65" s="9"/>
       <c r="N65" s="2"/>
     </row>
-    <row r="66" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A66" s="30" t="s">
-        <v>171</v>
+    <row r="66" spans="1:14" ht="29" x14ac:dyDescent="0.35">
+      <c r="A66" s="1" t="s">
+        <v>175</v>
       </c>
       <c r="B66" s="26" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C66" s="28" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D66" s="9" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="E66" s="9"/>
       <c r="F66" s="9"/>
@@ -3629,62 +3592,64 @@
       </c>
       <c r="H66" s="9"/>
       <c r="I66" s="9" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="J66" s="9"/>
       <c r="K66" s="1" t="s">
         <v>113</v>
       </c>
       <c r="L66" s="18" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="M66" s="9"/>
       <c r="N66" s="2"/>
     </row>
-    <row r="67" spans="1:14" ht="29" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:14" ht="87" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="B67" s="26" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C67" s="28" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D67" s="9" t="s">
-        <v>232</v>
-      </c>
-      <c r="E67" s="9"/>
+        <v>234</v>
+      </c>
+      <c r="E67" s="9" t="s">
+        <v>235</v>
+      </c>
       <c r="F67" s="9"/>
       <c r="G67" s="9" t="s">
-        <v>215</v>
+        <v>17</v>
       </c>
       <c r="H67" s="9"/>
       <c r="I67" s="9" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="J67" s="9"/>
       <c r="K67" s="1" t="s">
         <v>113</v>
       </c>
       <c r="L67" s="18" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="M67" s="9"/>
       <c r="N67" s="2"/>
     </row>
     <row r="68" spans="1:14" ht="87" x14ac:dyDescent="0.35">
       <c r="A68" s="1" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="B68" s="26" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C68" s="28" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D68" s="9" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="E68" s="9" t="s">
         <v>235</v>
@@ -3695,71 +3660,65 @@
       </c>
       <c r="H68" s="9"/>
       <c r="I68" s="9" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="J68" s="9"/>
       <c r="K68" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="L68" s="18" t="s">
-        <v>170</v>
+      <c r="L68" s="9" t="s">
+        <v>174</v>
       </c>
       <c r="M68" s="9"/>
       <c r="N68" s="2"/>
     </row>
     <row r="69" spans="1:14" ht="87" x14ac:dyDescent="0.35">
-      <c r="A69" s="1" t="s">
-        <v>180</v>
+      <c r="A69" s="30" t="s">
+        <v>182</v>
       </c>
       <c r="B69" s="26" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C69" s="28" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D69" s="9" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="E69" s="9" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="F69" s="9"/>
       <c r="G69" s="9" t="s">
-        <v>17</v>
+        <v>89</v>
       </c>
       <c r="H69" s="9"/>
-      <c r="I69" s="9" t="s">
-        <v>173</v>
-      </c>
+      <c r="I69" s="9"/>
       <c r="J69" s="9"/>
-      <c r="K69" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="L69" s="9" t="s">
-        <v>174</v>
-      </c>
+      <c r="K69" s="9"/>
+      <c r="L69" s="9"/>
       <c r="M69" s="9"/>
       <c r="N69" s="2"/>
     </row>
     <row r="70" spans="1:14" ht="87" x14ac:dyDescent="0.35">
-      <c r="A70" s="30" t="s">
-        <v>182</v>
+      <c r="A70" s="1" t="s">
+        <v>184</v>
       </c>
       <c r="B70" s="26" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C70" s="28" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D70" s="9" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="E70" s="9" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="F70" s="9"/>
       <c r="G70" s="9" t="s">
-        <v>89</v>
+        <v>5</v>
       </c>
       <c r="H70" s="9"/>
       <c r="I70" s="9"/>
@@ -3769,50 +3728,50 @@
       <c r="M70" s="9"/>
       <c r="N70" s="2"/>
     </row>
-    <row r="71" spans="1:14" ht="87" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:14" ht="58" x14ac:dyDescent="0.35">
       <c r="A71" s="1" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="B71" s="26" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C71" s="28" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D71" s="9" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="E71" s="9" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="F71" s="9"/>
       <c r="G71" s="9" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="H71" s="9"/>
-      <c r="I71" s="9"/>
+      <c r="I71" s="9" t="s">
+        <v>245</v>
+      </c>
       <c r="J71" s="9"/>
       <c r="K71" s="9"/>
       <c r="L71" s="9"/>
       <c r="M71" s="9"/>
       <c r="N71" s="2"/>
     </row>
-    <row r="72" spans="1:14" ht="58" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A72" s="1" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="B72" s="26" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C72" s="28" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D72" s="9" t="s">
-        <v>243</v>
-      </c>
-      <c r="E72" s="9" t="s">
-        <v>244</v>
-      </c>
+        <v>246</v>
+      </c>
+      <c r="E72" s="9"/>
       <c r="F72" s="9"/>
       <c r="G72" s="9" t="s">
         <v>17</v>
@@ -3828,85 +3787,91 @@
       <c r="N72" s="2"/>
     </row>
     <row r="73" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A73" s="1" t="s">
-        <v>189</v>
+      <c r="A73" s="30" t="s">
+        <v>191</v>
       </c>
       <c r="B73" s="26" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C73" s="28" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D73" s="9" t="s">
-        <v>246</v>
-      </c>
-      <c r="E73" s="9"/>
+        <v>247</v>
+      </c>
+      <c r="E73" s="9" t="s">
+        <v>248</v>
+      </c>
       <c r="F73" s="9"/>
       <c r="G73" s="9" t="s">
         <v>17</v>
       </c>
       <c r="H73" s="9"/>
-      <c r="I73" s="9" t="s">
-        <v>245</v>
-      </c>
+      <c r="I73" s="9"/>
       <c r="J73" s="9"/>
-      <c r="K73" s="9"/>
+      <c r="K73" s="8"/>
       <c r="L73" s="9"/>
       <c r="M73" s="9"/>
       <c r="N73" s="2"/>
     </row>
-    <row r="74" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A74" s="30" t="s">
-        <v>191</v>
+    <row r="74" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A74" s="1" t="s">
+        <v>193</v>
       </c>
       <c r="B74" s="26" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C74" s="28" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D74" s="9" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="E74" s="9" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="F74" s="9"/>
-      <c r="G74" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="H74" s="9"/>
+      <c r="G74" s="25" t="s">
+        <v>303</v>
+      </c>
+      <c r="H74" s="9" t="s">
+        <v>251</v>
+      </c>
       <c r="I74" s="9"/>
       <c r="J74" s="9"/>
-      <c r="K74" s="8"/>
-      <c r="L74" s="9"/>
+      <c r="K74" s="8">
+        <v>42</v>
+      </c>
+      <c r="L74" s="9" t="s">
+        <v>252</v>
+      </c>
       <c r="M74" s="9"/>
       <c r="N74" s="2"/>
     </row>
-    <row r="75" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:14" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A75" s="1" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="B75" s="26" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C75" s="28" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D75" s="9" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="E75" s="9" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="F75" s="9"/>
-      <c r="G75" s="25" t="s">
-        <v>304</v>
-      </c>
-      <c r="H75" s="9" t="s">
-        <v>251</v>
-      </c>
-      <c r="I75" s="9"/>
+      <c r="G75" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="H75" s="9"/>
+      <c r="I75" s="9" t="s">
+        <v>245</v>
+      </c>
       <c r="J75" s="9"/>
       <c r="K75" s="8">
         <v>42</v>
@@ -3917,22 +3882,20 @@
       <c r="M75" s="9"/>
       <c r="N75" s="2"/>
     </row>
-    <row r="76" spans="1:14" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A76" s="1" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="B76" s="26" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C76" s="28" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D76" s="9" t="s">
-        <v>253</v>
-      </c>
-      <c r="E76" s="9" t="s">
-        <v>254</v>
-      </c>
+        <v>255</v>
+      </c>
+      <c r="E76" s="9"/>
       <c r="F76" s="9"/>
       <c r="G76" s="9" t="s">
         <v>17</v>
@@ -3951,27 +3914,29 @@
       <c r="M76" s="9"/>
       <c r="N76" s="2"/>
     </row>
-    <row r="77" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A77" s="1" t="s">
-        <v>197</v>
+    <row r="77" spans="1:14" ht="116" x14ac:dyDescent="0.35">
+      <c r="A77" s="30" t="s">
+        <v>199</v>
       </c>
       <c r="B77" s="26" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C77" s="28" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D77" s="9" t="s">
-        <v>255</v>
-      </c>
-      <c r="E77" s="9"/>
+        <v>256</v>
+      </c>
+      <c r="E77" s="9" t="s">
+        <v>257</v>
+      </c>
       <c r="F77" s="9"/>
       <c r="G77" s="9" t="s">
         <v>17</v>
       </c>
       <c r="H77" s="9"/>
       <c r="I77" s="9" t="s">
-        <v>245</v>
+        <v>211</v>
       </c>
       <c r="J77" s="9"/>
       <c r="K77" s="8">
@@ -3983,22 +3948,20 @@
       <c r="M77" s="9"/>
       <c r="N77" s="2"/>
     </row>
-    <row r="78" spans="1:14" ht="116" x14ac:dyDescent="0.35">
-      <c r="A78" s="30" t="s">
-        <v>199</v>
+    <row r="78" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A78" s="1" t="s">
+        <v>201</v>
       </c>
       <c r="B78" s="26" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C78" s="28" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D78" s="9" t="s">
-        <v>256</v>
-      </c>
-      <c r="E78" s="9" t="s">
-        <v>257</v>
-      </c>
+        <v>258</v>
+      </c>
+      <c r="E78" s="9"/>
       <c r="F78" s="9"/>
       <c r="G78" s="9" t="s">
         <v>17</v>
@@ -4017,20 +3980,22 @@
       <c r="M78" s="9"/>
       <c r="N78" s="2"/>
     </row>
-    <row r="79" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:14" ht="116" x14ac:dyDescent="0.35">
       <c r="A79" s="1" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="B79" s="26" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C79" s="28" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D79" s="9" t="s">
-        <v>258</v>
-      </c>
-      <c r="E79" s="9"/>
+        <v>259</v>
+      </c>
+      <c r="E79" s="9" t="s">
+        <v>257</v>
+      </c>
       <c r="F79" s="9"/>
       <c r="G79" s="9" t="s">
         <v>17</v>
@@ -4049,22 +4014,20 @@
       <c r="M79" s="9"/>
       <c r="N79" s="2"/>
     </row>
-    <row r="80" spans="1:14" ht="116" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A80" s="1" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B80" s="26" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C80" s="28" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D80" s="9" t="s">
-        <v>259</v>
-      </c>
-      <c r="E80" s="9" t="s">
-        <v>257</v>
-      </c>
+        <v>260</v>
+      </c>
+      <c r="E80" s="9"/>
       <c r="F80" s="9"/>
       <c r="G80" s="9" t="s">
         <v>17</v>
@@ -4084,26 +4047,28 @@
       <c r="N80" s="2"/>
     </row>
     <row r="81" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A81" s="1" t="s">
-        <v>204</v>
+      <c r="A81" s="30" t="s">
+        <v>206</v>
       </c>
       <c r="B81" s="26" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C81" s="28" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D81" s="9" t="s">
-        <v>260</v>
-      </c>
-      <c r="E81" s="9"/>
+        <v>261</v>
+      </c>
+      <c r="E81" s="9" t="s">
+        <v>262</v>
+      </c>
       <c r="F81" s="9"/>
       <c r="G81" s="9" t="s">
         <v>17</v>
       </c>
       <c r="H81" s="9"/>
       <c r="I81" s="9" t="s">
-        <v>211</v>
+        <v>263</v>
       </c>
       <c r="J81" s="9"/>
       <c r="K81" s="8">
@@ -4116,20 +4081,20 @@
       <c r="N81" s="2"/>
     </row>
     <row r="82" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A82" s="30" t="s">
-        <v>206</v>
+      <c r="A82" s="1" t="s">
+        <v>208</v>
       </c>
       <c r="B82" s="26" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C82" s="28" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D82" s="9" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="E82" s="9" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="F82" s="9"/>
       <c r="G82" s="9" t="s">
@@ -4151,82 +4116,82 @@
     </row>
     <row r="83" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A83" s="1" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="B83" s="26" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C83" s="28" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D83" s="9" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="E83" s="9" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="F83" s="9"/>
       <c r="G83" s="9" t="s">
         <v>17</v>
       </c>
       <c r="H83" s="9"/>
-      <c r="I83" s="9" t="s">
-        <v>263</v>
-      </c>
+      <c r="I83" s="9"/>
       <c r="J83" s="9"/>
-      <c r="K83" s="8">
+      <c r="K83" s="9">
         <v>42</v>
       </c>
-      <c r="L83" s="9" t="s">
+      <c r="L83" s="18" t="s">
         <v>252</v>
       </c>
       <c r="M83" s="9"/>
       <c r="N83" s="2"/>
     </row>
-    <row r="84" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:14" ht="58" x14ac:dyDescent="0.35">
       <c r="A84" s="1" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="B84" s="26" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C84" s="28" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D84" s="9" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="E84" s="9" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="F84" s="9"/>
       <c r="G84" s="9" t="s">
         <v>17</v>
       </c>
       <c r="H84" s="9"/>
-      <c r="I84" s="9"/>
+      <c r="I84" s="9" t="s">
+        <v>169</v>
+      </c>
       <c r="J84" s="9"/>
-      <c r="K84" s="9">
-        <v>42</v>
+      <c r="K84" s="1" t="s">
+        <v>113</v>
       </c>
       <c r="L84" s="18" t="s">
-        <v>252</v>
+        <v>170</v>
       </c>
       <c r="M84" s="9"/>
       <c r="N84" s="2"/>
     </row>
     <row r="85" spans="1:14" ht="58" x14ac:dyDescent="0.35">
-      <c r="A85" s="1" t="s">
-        <v>216</v>
+      <c r="A85" s="30" t="s">
+        <v>219</v>
       </c>
       <c r="B85" s="26" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C85" s="28" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D85" s="9" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="E85" s="9" t="s">
         <v>269</v>
@@ -4237,96 +4202,90 @@
       </c>
       <c r="H85" s="9"/>
       <c r="I85" s="9" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="J85" s="9"/>
       <c r="K85" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="L85" s="18" t="s">
-        <v>170</v>
+      <c r="L85" s="9" t="s">
+        <v>174</v>
       </c>
       <c r="M85" s="9"/>
       <c r="N85" s="2"/>
     </row>
-    <row r="86" spans="1:14" ht="58" x14ac:dyDescent="0.35">
-      <c r="A86" s="30" t="s">
-        <v>219</v>
+    <row r="86" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A86" s="1" t="s">
+        <v>222</v>
       </c>
       <c r="B86" s="26" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C86" s="28" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D86" s="9" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="E86" s="9" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="F86" s="9"/>
       <c r="G86" s="9" t="s">
-        <v>17</v>
+        <v>89</v>
       </c>
       <c r="H86" s="9"/>
-      <c r="I86" s="9" t="s">
-        <v>173</v>
-      </c>
+      <c r="I86" s="9"/>
       <c r="J86" s="9"/>
-      <c r="K86" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="L86" s="9" t="s">
-        <v>174</v>
-      </c>
+      <c r="K86" s="9"/>
+      <c r="L86" s="9"/>
       <c r="M86" s="9"/>
       <c r="N86" s="2"/>
     </row>
-    <row r="87" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:14" ht="145" x14ac:dyDescent="0.35">
       <c r="A87" s="1" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B87" s="26" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C87" s="28" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D87" s="9" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="E87" s="9" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="F87" s="9"/>
       <c r="G87" s="9" t="s">
-        <v>89</v>
+        <v>17</v>
       </c>
       <c r="H87" s="9"/>
-      <c r="I87" s="9"/>
+      <c r="I87" s="9" t="s">
+        <v>211</v>
+      </c>
       <c r="J87" s="9"/>
       <c r="K87" s="9"/>
       <c r="L87" s="9"/>
       <c r="M87" s="9"/>
       <c r="N87" s="2"/>
     </row>
-    <row r="88" spans="1:14" ht="145" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A88" s="1" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="B88" s="26" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C88" s="28" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D88" s="9" t="s">
-        <v>273</v>
-      </c>
-      <c r="E88" s="9" t="s">
-        <v>274</v>
-      </c>
+        <v>275</v>
+      </c>
+      <c r="E88" s="9"/>
       <c r="F88" s="9"/>
       <c r="G88" s="9" t="s">
         <v>17</v>
@@ -4342,17 +4301,17 @@
       <c r="N88" s="2"/>
     </row>
     <row r="89" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A89" s="1" t="s">
-        <v>227</v>
+      <c r="A89" s="30" t="s">
+        <v>229</v>
       </c>
       <c r="B89" s="26" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C89" s="28" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D89" s="9" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="E89" s="9"/>
       <c r="F89" s="9"/>
@@ -4370,17 +4329,17 @@
       <c r="N89" s="2"/>
     </row>
     <row r="90" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A90" s="30" t="s">
-        <v>229</v>
+      <c r="A90" s="1" t="s">
+        <v>231</v>
       </c>
       <c r="B90" s="26" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C90" s="28" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D90" s="9" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="E90" s="9"/>
       <c r="F90" s="9"/>
@@ -4391,59 +4350,59 @@
       <c r="I90" s="9" t="s">
         <v>211</v>
       </c>
-      <c r="J90" s="9"/>
+      <c r="J90" s="2"/>
       <c r="K90" s="9"/>
       <c r="L90" s="9"/>
       <c r="M90" s="9"/>
       <c r="N90" s="2"/>
     </row>
-    <row r="91" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:14" ht="304.5" x14ac:dyDescent="0.35">
       <c r="A91" s="1" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="B91" s="26" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C91" s="28" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="D91" s="9" t="s">
-        <v>277</v>
-      </c>
-      <c r="E91" s="9"/>
+        <v>278</v>
+      </c>
+      <c r="E91" s="9" t="s">
+        <v>279</v>
+      </c>
       <c r="F91" s="9"/>
       <c r="G91" s="9" t="s">
-        <v>17</v>
+        <v>280</v>
       </c>
       <c r="H91" s="9"/>
-      <c r="I91" s="9" t="s">
-        <v>211</v>
-      </c>
-      <c r="J91" s="2"/>
+      <c r="I91" s="9"/>
+      <c r="J91" s="9"/>
       <c r="K91" s="9"/>
       <c r="L91" s="9"/>
       <c r="M91" s="9"/>
       <c r="N91" s="2"/>
     </row>
-    <row r="92" spans="1:14" ht="304.5" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:14" ht="116" x14ac:dyDescent="0.35">
       <c r="A92" s="1" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="B92" s="26" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C92" s="28" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D92" s="9" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="E92" s="9" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="F92" s="9"/>
       <c r="G92" s="9" t="s">
-        <v>280</v>
+        <v>17</v>
       </c>
       <c r="H92" s="9"/>
       <c r="I92" s="9"/>
@@ -4453,51 +4412,23 @@
       <c r="M92" s="9"/>
       <c r="N92" s="2"/>
     </row>
-    <row r="93" spans="1:14" ht="116" x14ac:dyDescent="0.35">
-      <c r="A93" s="1" t="s">
-        <v>236</v>
+    <row r="93" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A93" s="30" t="s">
+        <v>238</v>
       </c>
       <c r="B93" s="26" t="s">
-        <v>305</v>
-      </c>
-      <c r="C93" s="28" t="s">
-        <v>311</v>
-      </c>
-      <c r="D93" s="9" t="s">
-        <v>281</v>
-      </c>
-      <c r="E93" s="9" t="s">
-        <v>282</v>
-      </c>
-      <c r="F93" s="9"/>
-      <c r="G93" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="H93" s="9"/>
-      <c r="I93" s="9"/>
-      <c r="J93" s="9"/>
-      <c r="K93" s="9"/>
-      <c r="L93" s="9"/>
-      <c r="M93" s="9"/>
-      <c r="N93" s="2"/>
-    </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A94" s="30" t="s">
-        <v>238</v>
-      </c>
-      <c r="B94" s="26" t="s">
-        <v>305</v>
-      </c>
-      <c r="C94" t="s">
-        <v>311</v>
-      </c>
-      <c r="D94" t="s">
+        <v>304</v>
+      </c>
+      <c r="C93" t="s">
+        <v>310</v>
+      </c>
+      <c r="D93" t="s">
         <v>283</v>
       </c>
-      <c r="G94" t="s">
-        <v>17</v>
-      </c>
-      <c r="I94" t="s">
+      <c r="G93" t="s">
+        <v>17</v>
+      </c>
+      <c r="I93" t="s">
         <v>245</v>
       </c>
     </row>
@@ -4588,7 +4519,7 @@
       </c>
       <c r="I2" s="9"/>
       <c r="J2" s="28" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="K2" s="9"/>
       <c r="L2" s="9"/>

</xml_diff>

<commit_message>
updates upload page and dependencies of sme data dictionary
</commit_message>
<xml_diff>
--- a/dataland-framework-toolbox/inputs/sme/sme.xlsx
+++ b/dataland-framework-toolbox/inputs/sme/sme.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d92048\IdeaProjects\Dataland5\dataland-framework-toolbox\inputs\sme\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7645F185-D2D6-4652-97B8-4537AC7004B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB34D211-6A68-4E8D-90B7-6023B87C5353}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C4E498E0-8E09-4328-BD54-6E3CD29DBCBD}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="887" uniqueCount="323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="887" uniqueCount="325">
   <si>
     <t>1</t>
   </si>
@@ -1034,12 +1034,18 @@
   <si>
     <t>Pollution Emission</t>
   </si>
+  <si>
+    <t>FullTimeEquivalents</t>
+  </si>
+  <si>
+    <t>HeadCount</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1111,6 +1117,13 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF9876AA"/>
+      <name val="Courier New"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1190,7 +1203,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
@@ -1275,6 +1288,9 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1595,9 +1611,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DE53926-978F-4910-9169-F720F1E0A6DD}">
   <dimension ref="A1:N93"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2860,8 +2876,8 @@
       <c r="K43" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="L43" s="18" t="s">
-        <v>170</v>
+      <c r="L43" s="31" t="s">
+        <v>323</v>
       </c>
       <c r="M43" s="9"/>
       <c r="N43" s="2"/>
@@ -2894,8 +2910,8 @@
       <c r="K44" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="L44" s="18" t="s">
-        <v>174</v>
+      <c r="L44" s="31" t="s">
+        <v>324</v>
       </c>
       <c r="M44" s="9"/>
       <c r="N44" s="2"/>
@@ -2928,8 +2944,8 @@
       <c r="K45" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="L45" s="18" t="s">
-        <v>170</v>
+      <c r="L45" s="31" t="s">
+        <v>323</v>
       </c>
       <c r="M45" s="9"/>
       <c r="N45" s="2"/>
@@ -2962,8 +2978,8 @@
       <c r="K46" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="L46" s="18" t="s">
-        <v>174</v>
+      <c r="L46" s="31" t="s">
+        <v>324</v>
       </c>
       <c r="M46" s="9"/>
       <c r="N46" s="2"/>
@@ -2994,8 +3010,8 @@
       <c r="K47" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="L47" s="18" t="s">
-        <v>170</v>
+      <c r="L47" s="31" t="s">
+        <v>323</v>
       </c>
       <c r="M47" s="9"/>
       <c r="N47" s="2"/>
@@ -3026,8 +3042,8 @@
       <c r="K48" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="L48" s="18" t="s">
-        <v>174</v>
+      <c r="L48" s="31" t="s">
+        <v>324</v>
       </c>
       <c r="M48" s="9"/>
       <c r="N48" s="2"/>
@@ -3060,8 +3076,8 @@
       <c r="K49" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="L49" s="18" t="s">
-        <v>170</v>
+      <c r="L49" s="31" t="s">
+        <v>323</v>
       </c>
       <c r="M49" s="9"/>
       <c r="N49" s="2"/>
@@ -3094,8 +3110,8 @@
       <c r="K50" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="L50" s="18" t="s">
-        <v>174</v>
+      <c r="L50" s="31" t="s">
+        <v>324</v>
       </c>
       <c r="M50" s="9"/>
       <c r="N50" s="2"/>
@@ -3126,8 +3142,8 @@
       <c r="K51" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="L51" s="18" t="s">
-        <v>170</v>
+      <c r="L51" s="31" t="s">
+        <v>323</v>
       </c>
       <c r="M51" s="9"/>
       <c r="N51" s="2"/>
@@ -3158,8 +3174,8 @@
       <c r="K52" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="L52" s="18" t="s">
-        <v>174</v>
+      <c r="L52" s="31" t="s">
+        <v>324</v>
       </c>
       <c r="M52" s="9"/>
       <c r="N52" s="2"/>
@@ -3190,8 +3206,8 @@
       <c r="K53" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="L53" s="18" t="s">
-        <v>170</v>
+      <c r="L53" s="31" t="s">
+        <v>323</v>
       </c>
       <c r="M53" s="9"/>
       <c r="N53" s="2"/>
@@ -3222,8 +3238,8 @@
       <c r="K54" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="L54" s="18" t="s">
-        <v>174</v>
+      <c r="L54" s="31" t="s">
+        <v>324</v>
       </c>
       <c r="M54" s="9"/>
       <c r="N54" s="2"/>
@@ -3254,8 +3270,8 @@
       <c r="K55" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="L55" s="18" t="s">
-        <v>170</v>
+      <c r="L55" s="31" t="s">
+        <v>323</v>
       </c>
       <c r="M55" s="9"/>
       <c r="N55" s="2"/>
@@ -3286,8 +3302,8 @@
       <c r="K56" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="L56" s="9" t="s">
-        <v>174</v>
+      <c r="L56" s="31" t="s">
+        <v>324</v>
       </c>
       <c r="M56" s="9"/>
       <c r="N56" s="2"/>
@@ -3432,8 +3448,8 @@
       <c r="K61" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="L61" s="18" t="s">
-        <v>170</v>
+      <c r="L61" s="31" t="s">
+        <v>323</v>
       </c>
       <c r="M61" s="9"/>
       <c r="N61" s="2"/>
@@ -3466,8 +3482,8 @@
       <c r="K62" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="L62" s="18" t="s">
-        <v>174</v>
+      <c r="L62" s="31" t="s">
+        <v>324</v>
       </c>
       <c r="M62" s="9"/>
       <c r="N62" s="2"/>
@@ -3500,8 +3516,8 @@
       <c r="K63" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="L63" s="18" t="s">
-        <v>170</v>
+      <c r="L63" s="31" t="s">
+        <v>323</v>
       </c>
       <c r="M63" s="9"/>
       <c r="N63" s="2"/>
@@ -3534,8 +3550,8 @@
       <c r="K64" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="L64" s="18" t="s">
-        <v>174</v>
+      <c r="L64" s="31" t="s">
+        <v>324</v>
       </c>
       <c r="M64" s="9"/>
       <c r="N64" s="2"/>
@@ -3566,8 +3582,8 @@
       <c r="K65" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="L65" s="18" t="s">
-        <v>170</v>
+      <c r="L65" s="31" t="s">
+        <v>323</v>
       </c>
       <c r="M65" s="9"/>
       <c r="N65" s="2"/>
@@ -3598,8 +3614,8 @@
       <c r="K66" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="L66" s="18" t="s">
-        <v>174</v>
+      <c r="L66" s="31" t="s">
+        <v>324</v>
       </c>
       <c r="M66" s="9"/>
       <c r="N66" s="2"/>
@@ -3632,8 +3648,8 @@
       <c r="K67" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="L67" s="18" t="s">
-        <v>170</v>
+      <c r="L67" s="31" t="s">
+        <v>323</v>
       </c>
       <c r="M67" s="9"/>
       <c r="N67" s="2"/>
@@ -3666,8 +3682,8 @@
       <c r="K68" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="L68" s="9" t="s">
-        <v>174</v>
+      <c r="L68" s="31" t="s">
+        <v>324</v>
       </c>
       <c r="M68" s="9"/>
       <c r="N68" s="2"/>
@@ -4174,8 +4190,8 @@
       <c r="K84" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="L84" s="18" t="s">
-        <v>170</v>
+      <c r="L84" s="31" t="s">
+        <v>323</v>
       </c>
       <c r="M84" s="9"/>
       <c r="N84" s="2"/>
@@ -4208,8 +4224,8 @@
       <c r="K85" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="L85" s="9" t="s">
-        <v>174</v>
+      <c r="L85" s="31" t="s">
+        <v>324</v>
       </c>
       <c r="M85" s="9"/>
       <c r="N85" s="2"/>

</xml_diff>

<commit_message>
adds sites and areas component wip
</commit_message>
<xml_diff>
--- a/dataland-framework-toolbox/inputs/sme/sme.xlsx
+++ b/dataland-framework-toolbox/inputs/sme/sme.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d92048\IdeaProjects\Dataland5\dataland-framework-toolbox\inputs\sme\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB34D211-6A68-4E8D-90B7-6023B87C5353}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0BA2551-A377-4777-9A91-969902A48703}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C4E498E0-8E09-4328-BD54-6E3CD29DBCBD}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="887" uniqueCount="325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="888" uniqueCount="326">
   <si>
     <t>1</t>
   </si>
@@ -966,9 +966,6 @@
     <t>Custom Component Employees</t>
   </si>
   <si>
-    <t>Custom Component Sites And Area</t>
-  </si>
-  <si>
     <t>Custom Component Waste</t>
   </si>
   <si>
@@ -1039,13 +1036,19 @@
   </si>
   <si>
     <t>HeadCount</t>
+  </si>
+  <si>
+    <t>Sme Site And Area</t>
+  </si>
+  <si>
+    <t>Sites and Areas</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1117,11 +1120,18 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF9876AA"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF6A8759"/>
       <name val="Courier New"/>
       <family val="3"/>
     </font>
@@ -1203,7 +1213,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
@@ -1290,6 +1300,9 @@
       <alignment readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1612,8 +1625,8 @@
   <dimension ref="A1:N93"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G42" sqref="G42"/>
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1679,10 +1692,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="26" t="s">
+        <v>303</v>
+      </c>
+      <c r="C2" s="27" t="s">
         <v>304</v>
-      </c>
-      <c r="C2" s="27" t="s">
-        <v>305</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>3</v>
@@ -1709,10 +1722,10 @@
         <v>11</v>
       </c>
       <c r="B3" s="26" t="s">
+        <v>303</v>
+      </c>
+      <c r="C3" s="27" t="s">
         <v>304</v>
-      </c>
-      <c r="C3" s="27" t="s">
-        <v>305</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>298</v>
@@ -1722,7 +1735,7 @@
       </c>
       <c r="F3" s="5"/>
       <c r="G3" s="27" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
@@ -1737,10 +1750,10 @@
         <v>14</v>
       </c>
       <c r="B4" s="26" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C4" s="28" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>12</v>
@@ -1765,10 +1778,10 @@
         <v>19</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C5" s="28" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>15</v>
@@ -1795,10 +1808,10 @@
         <v>22</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C6" s="28" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>20</v>
@@ -1815,7 +1828,7 @@
         <v>18</v>
       </c>
       <c r="J6" s="11" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="K6" s="12"/>
       <c r="L6" s="11"/>
@@ -1827,10 +1840,10 @@
         <v>24</v>
       </c>
       <c r="B7" s="26" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C7" s="28" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>23</v>
@@ -1855,10 +1868,10 @@
         <v>26</v>
       </c>
       <c r="B8" s="26" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C8" s="28" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>25</v>
@@ -1883,10 +1896,10 @@
         <v>30</v>
       </c>
       <c r="B9" s="26" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C9" s="28" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>27</v>
@@ -1903,7 +1916,7 @@
         <v>29</v>
       </c>
       <c r="J9" s="11" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="K9" s="12"/>
       <c r="L9" s="11"/>
@@ -1915,10 +1928,10 @@
         <v>33</v>
       </c>
       <c r="B10" s="26" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C10" s="28" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>31</v>
@@ -1935,7 +1948,7 @@
         <v>29</v>
       </c>
       <c r="J10" s="11" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="K10" s="12"/>
       <c r="L10" s="11"/>
@@ -1947,10 +1960,10 @@
         <v>36</v>
       </c>
       <c r="B11" s="26" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C11" s="28" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>34</v>
@@ -1967,7 +1980,7 @@
         <v>29</v>
       </c>
       <c r="J11" s="11" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="K11" s="12"/>
       <c r="L11" s="11"/>
@@ -1979,10 +1992,10 @@
         <v>39</v>
       </c>
       <c r="B12" s="26" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C12" s="28" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>37</v>
@@ -1999,7 +2012,7 @@
         <v>29</v>
       </c>
       <c r="J12" s="11" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="K12" s="12"/>
       <c r="L12" s="11"/>
@@ -2011,20 +2024,20 @@
         <v>42</v>
       </c>
       <c r="B13" s="26" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C13" s="28" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D13" s="27" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E13" s="9" t="s">
         <v>41</v>
       </c>
       <c r="F13" s="10"/>
       <c r="G13" s="19" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
@@ -2039,18 +2052,20 @@
         <v>48</v>
       </c>
       <c r="B14" s="26" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C14" s="28" t="s">
-        <v>309</v>
-      </c>
-      <c r="D14" s="3"/>
+        <v>308</v>
+      </c>
+      <c r="D14" s="27" t="s">
+        <v>325</v>
+      </c>
       <c r="E14" s="9" t="s">
         <v>54</v>
       </c>
       <c r="F14" s="10"/>
-      <c r="G14" s="3" t="s">
-        <v>300</v>
+      <c r="G14" s="32" t="s">
+        <v>324</v>
       </c>
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
@@ -2065,10 +2080,10 @@
         <v>52</v>
       </c>
       <c r="B15" s="26" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C15" s="28" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D15" s="9" t="s">
         <v>84</v>
@@ -2093,10 +2108,10 @@
         <v>55</v>
       </c>
       <c r="B16" s="26" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C16" s="28" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D16" s="9" t="s">
         <v>86</v>
@@ -2121,10 +2136,10 @@
         <v>57</v>
       </c>
       <c r="B17" s="26" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C17" s="28" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D17" s="9" t="s">
         <v>88</v>
@@ -2149,10 +2164,10 @@
         <v>59</v>
       </c>
       <c r="B18" s="26" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C18" s="28" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D18" s="9" t="s">
         <v>91</v>
@@ -2177,10 +2192,10 @@
         <v>61</v>
       </c>
       <c r="B19" s="26" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C19" s="28" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D19" s="9" t="s">
         <v>93</v>
@@ -2205,10 +2220,10 @@
         <v>63</v>
       </c>
       <c r="B20" s="26" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C20" s="28" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D20" s="9" t="s">
         <v>95</v>
@@ -2233,13 +2248,13 @@
         <v>66</v>
       </c>
       <c r="B21" s="26" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C21" s="28" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D21" s="28" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="E21" s="9" t="s">
         <v>82</v>
@@ -2261,10 +2276,10 @@
         <v>69</v>
       </c>
       <c r="B22" s="26" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C22" s="28" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D22" s="9" t="s">
         <v>98</v>
@@ -2289,10 +2304,10 @@
         <v>71</v>
       </c>
       <c r="B23" s="26" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C23" s="28" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D23" s="9" t="s">
         <v>100</v>
@@ -2317,10 +2332,10 @@
         <v>73</v>
       </c>
       <c r="B24" s="26" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C24" s="28" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D24" s="9" t="s">
         <v>102</v>
@@ -2345,10 +2360,10 @@
         <v>75</v>
       </c>
       <c r="B25" s="26" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C25" s="28" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D25" s="9" t="s">
         <v>104</v>
@@ -2373,10 +2388,10 @@
         <v>77</v>
       </c>
       <c r="B26" s="26" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C26" s="28" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D26" s="9" t="s">
         <v>106</v>
@@ -2401,10 +2416,10 @@
         <v>81</v>
       </c>
       <c r="B27" s="26" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C27" s="28" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D27" s="9" t="s">
         <v>108</v>
@@ -2418,10 +2433,10 @@
       </c>
       <c r="H27" s="9"/>
       <c r="I27" s="29" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="J27" s="11" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="K27" s="9"/>
       <c r="L27" s="9"/>
@@ -2433,10 +2448,10 @@
         <v>83</v>
       </c>
       <c r="B28" s="26" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C28" s="28" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D28" s="9" t="s">
         <v>112</v>
@@ -2448,7 +2463,7 @@
       </c>
       <c r="H28" s="9"/>
       <c r="I28" s="29" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="J28" s="9"/>
       <c r="K28" s="9"/>
@@ -2461,10 +2476,10 @@
         <v>85</v>
       </c>
       <c r="B29" s="26" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C29" s="28" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D29" s="9" t="s">
         <v>114</v>
@@ -2478,7 +2493,7 @@
       </c>
       <c r="H29" s="9"/>
       <c r="I29" s="29" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="J29" s="9"/>
       <c r="K29" s="9"/>
@@ -2491,10 +2506,10 @@
         <v>87</v>
       </c>
       <c r="B30" s="26" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C30" s="28" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D30" s="9" t="s">
         <v>116</v>
@@ -2506,7 +2521,7 @@
       </c>
       <c r="H30" s="9"/>
       <c r="I30" s="29" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="J30" s="9"/>
       <c r="K30" s="9"/>
@@ -2519,10 +2534,10 @@
         <v>90</v>
       </c>
       <c r="B31" s="26" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C31" s="28" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D31" s="9" t="s">
         <v>118</v>
@@ -2534,7 +2549,7 @@
       </c>
       <c r="H31" s="9"/>
       <c r="I31" s="29" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="J31" s="9"/>
       <c r="K31" s="9"/>
@@ -2547,10 +2562,10 @@
         <v>92</v>
       </c>
       <c r="B32" s="26" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C32" s="28" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D32" s="9" t="s">
         <v>120</v>
@@ -2562,7 +2577,7 @@
       </c>
       <c r="H32" s="9"/>
       <c r="I32" s="29" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="J32" s="9"/>
       <c r="K32" s="9"/>
@@ -2575,10 +2590,10 @@
         <v>94</v>
       </c>
       <c r="B33" s="26" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C33" s="28" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D33" s="9" t="s">
         <v>122</v>
@@ -2590,7 +2605,7 @@
       </c>
       <c r="H33" s="9"/>
       <c r="I33" s="29" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="J33" s="9"/>
       <c r="K33" s="9"/>
@@ -2603,10 +2618,10 @@
         <v>96</v>
       </c>
       <c r="B34" s="26" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C34" s="28" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D34" s="9" t="s">
         <v>124</v>
@@ -2618,7 +2633,7 @@
       </c>
       <c r="H34" s="9"/>
       <c r="I34" s="29" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="J34" s="9"/>
       <c r="K34" s="9"/>
@@ -2631,10 +2646,10 @@
         <v>97</v>
       </c>
       <c r="B35" s="26" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C35" s="28" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D35" s="9" t="s">
         <v>127</v>
@@ -2661,10 +2676,10 @@
         <v>99</v>
       </c>
       <c r="B36" s="26" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C36" s="28" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D36" s="9" t="s">
         <v>131</v>
@@ -2689,10 +2704,10 @@
         <v>101</v>
       </c>
       <c r="B37" s="26" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C37" s="28" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D37" s="9" t="s">
         <v>133</v>
@@ -2715,10 +2730,10 @@
         <v>103</v>
       </c>
       <c r="B38" s="26" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C38" s="28" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D38" s="9" t="s">
         <v>135</v>
@@ -2743,13 +2758,13 @@
         <v>105</v>
       </c>
       <c r="B39" s="26" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C39" s="28" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="E39" s="9"/>
       <c r="F39" s="9"/>
@@ -2769,10 +2784,10 @@
         <v>107</v>
       </c>
       <c r="B40" s="26" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C40" s="28" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D40" s="9" t="s">
         <v>138</v>
@@ -2782,7 +2797,7 @@
       </c>
       <c r="F40" s="9"/>
       <c r="G40" s="25" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="H40" s="9" t="s">
         <v>140</v>
@@ -2799,16 +2814,16 @@
         <v>111</v>
       </c>
       <c r="B41" s="26" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C41" s="28" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D41" s="9"/>
       <c r="E41" s="9"/>
       <c r="F41" s="9"/>
       <c r="G41" s="8" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="H41" s="9"/>
       <c r="I41" s="9"/>
@@ -2823,10 +2838,10 @@
         <v>113</v>
       </c>
       <c r="B42" s="26" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C42" s="28" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D42" s="9" t="s">
         <v>163</v>
@@ -2836,7 +2851,7 @@
       </c>
       <c r="F42" s="9"/>
       <c r="G42" s="25" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="H42" s="9" t="s">
         <v>165</v>
@@ -2853,10 +2868,10 @@
         <v>115</v>
       </c>
       <c r="B43" s="26" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C43" s="28" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D43" s="9" t="s">
         <v>167</v>
@@ -2877,7 +2892,7 @@
         <v>113</v>
       </c>
       <c r="L43" s="31" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="M43" s="9"/>
       <c r="N43" s="2"/>
@@ -2887,10 +2902,10 @@
         <v>117</v>
       </c>
       <c r="B44" s="26" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C44" s="28" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D44" s="9" t="s">
         <v>172</v>
@@ -2911,7 +2926,7 @@
         <v>113</v>
       </c>
       <c r="L44" s="31" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="M44" s="9"/>
       <c r="N44" s="2"/>
@@ -2921,10 +2936,10 @@
         <v>119</v>
       </c>
       <c r="B45" s="26" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C45" s="28" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D45" s="9" t="s">
         <v>176</v>
@@ -2945,7 +2960,7 @@
         <v>113</v>
       </c>
       <c r="L45" s="31" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="M45" s="9"/>
       <c r="N45" s="2"/>
@@ -2955,10 +2970,10 @@
         <v>121</v>
       </c>
       <c r="B46" s="26" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C46" s="28" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D46" s="9" t="s">
         <v>179</v>
@@ -2979,7 +2994,7 @@
         <v>113</v>
       </c>
       <c r="L46" s="31" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="M46" s="9"/>
       <c r="N46" s="2"/>
@@ -2989,10 +3004,10 @@
         <v>123</v>
       </c>
       <c r="B47" s="26" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C47" s="28" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D47" s="9" t="s">
         <v>181</v>
@@ -3011,7 +3026,7 @@
         <v>113</v>
       </c>
       <c r="L47" s="31" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="M47" s="9"/>
       <c r="N47" s="2"/>
@@ -3021,10 +3036,10 @@
         <v>125</v>
       </c>
       <c r="B48" s="26" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C48" s="28" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D48" s="9" t="s">
         <v>183</v>
@@ -3043,7 +3058,7 @@
         <v>113</v>
       </c>
       <c r="L48" s="31" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="M48" s="9"/>
       <c r="N48" s="2"/>
@@ -3053,10 +3068,10 @@
         <v>130</v>
       </c>
       <c r="B49" s="26" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C49" s="28" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D49" s="9" t="s">
         <v>185</v>
@@ -3077,7 +3092,7 @@
         <v>113</v>
       </c>
       <c r="L49" s="31" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="M49" s="9"/>
       <c r="N49" s="2"/>
@@ -3087,10 +3102,10 @@
         <v>132</v>
       </c>
       <c r="B50" s="26" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C50" s="28" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D50" s="9" t="s">
         <v>188</v>
@@ -3111,7 +3126,7 @@
         <v>113</v>
       </c>
       <c r="L50" s="31" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="M50" s="9"/>
       <c r="N50" s="2"/>
@@ -3121,10 +3136,10 @@
         <v>134</v>
       </c>
       <c r="B51" s="26" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C51" s="28" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D51" s="9" t="s">
         <v>190</v>
@@ -3143,7 +3158,7 @@
         <v>113</v>
       </c>
       <c r="L51" s="31" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="M51" s="9"/>
       <c r="N51" s="2"/>
@@ -3153,10 +3168,10 @@
         <v>136</v>
       </c>
       <c r="B52" s="26" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C52" s="28" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D52" s="9" t="s">
         <v>192</v>
@@ -3175,7 +3190,7 @@
         <v>113</v>
       </c>
       <c r="L52" s="31" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="M52" s="9"/>
       <c r="N52" s="2"/>
@@ -3185,10 +3200,10 @@
         <v>137</v>
       </c>
       <c r="B53" s="26" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C53" s="28" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D53" s="9" t="s">
         <v>194</v>
@@ -3207,7 +3222,7 @@
         <v>113</v>
       </c>
       <c r="L53" s="31" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="M53" s="9"/>
       <c r="N53" s="2"/>
@@ -3217,10 +3232,10 @@
         <v>141</v>
       </c>
       <c r="B54" s="26" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C54" s="28" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D54" s="9" t="s">
         <v>196</v>
@@ -3239,7 +3254,7 @@
         <v>113</v>
       </c>
       <c r="L54" s="31" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="M54" s="9"/>
       <c r="N54" s="2"/>
@@ -3249,10 +3264,10 @@
         <v>142</v>
       </c>
       <c r="B55" s="26" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C55" s="28" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D55" s="9" t="s">
         <v>198</v>
@@ -3271,7 +3286,7 @@
         <v>113</v>
       </c>
       <c r="L55" s="31" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="M55" s="9"/>
       <c r="N55" s="2"/>
@@ -3281,10 +3296,10 @@
         <v>145</v>
       </c>
       <c r="B56" s="26" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C56" s="28" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D56" s="9" t="s">
         <v>200</v>
@@ -3303,7 +3318,7 @@
         <v>113</v>
       </c>
       <c r="L56" s="31" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="M56" s="9"/>
       <c r="N56" s="2"/>
@@ -3313,10 +3328,10 @@
         <v>147</v>
       </c>
       <c r="B57" s="26" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C57" s="28" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D57" s="9"/>
       <c r="E57" s="9" t="s">
@@ -3339,10 +3354,10 @@
         <v>150</v>
       </c>
       <c r="B58" s="26" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C58" s="28" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D58" s="9" t="s">
         <v>209</v>
@@ -3369,10 +3384,10 @@
         <v>153</v>
       </c>
       <c r="B59" s="26" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C59" s="28" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D59" s="9" t="s">
         <v>213</v>
@@ -3397,10 +3412,10 @@
         <v>155</v>
       </c>
       <c r="B60" s="26" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C60" s="28" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D60" s="9" t="s">
         <v>217</v>
@@ -3425,10 +3440,10 @@
         <v>157</v>
       </c>
       <c r="B61" s="26" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C61" s="28" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D61" s="9" t="s">
         <v>220</v>
@@ -3449,7 +3464,7 @@
         <v>113</v>
       </c>
       <c r="L61" s="31" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="M61" s="9"/>
       <c r="N61" s="2"/>
@@ -3459,10 +3474,10 @@
         <v>159</v>
       </c>
       <c r="B62" s="26" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C62" s="28" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D62" s="9" t="s">
         <v>223</v>
@@ -3483,7 +3498,7 @@
         <v>113</v>
       </c>
       <c r="L62" s="31" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="M62" s="9"/>
       <c r="N62" s="2"/>
@@ -3493,10 +3508,10 @@
         <v>161</v>
       </c>
       <c r="B63" s="26" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C63" s="28" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D63" s="9" t="s">
         <v>225</v>
@@ -3517,7 +3532,7 @@
         <v>113</v>
       </c>
       <c r="L63" s="31" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="M63" s="9"/>
       <c r="N63" s="2"/>
@@ -3527,10 +3542,10 @@
         <v>166</v>
       </c>
       <c r="B64" s="26" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C64" s="28" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D64" s="9" t="s">
         <v>228</v>
@@ -3551,7 +3566,7 @@
         <v>113</v>
       </c>
       <c r="L64" s="31" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="M64" s="9"/>
       <c r="N64" s="2"/>
@@ -3561,10 +3576,10 @@
         <v>171</v>
       </c>
       <c r="B65" s="26" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C65" s="28" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D65" s="9" t="s">
         <v>230</v>
@@ -3583,7 +3598,7 @@
         <v>113</v>
       </c>
       <c r="L65" s="31" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="M65" s="9"/>
       <c r="N65" s="2"/>
@@ -3593,10 +3608,10 @@
         <v>175</v>
       </c>
       <c r="B66" s="26" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C66" s="28" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D66" s="9" t="s">
         <v>232</v>
@@ -3615,7 +3630,7 @@
         <v>113</v>
       </c>
       <c r="L66" s="31" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="M66" s="9"/>
       <c r="N66" s="2"/>
@@ -3625,10 +3640,10 @@
         <v>178</v>
       </c>
       <c r="B67" s="26" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C67" s="28" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D67" s="9" t="s">
         <v>234</v>
@@ -3649,7 +3664,7 @@
         <v>113</v>
       </c>
       <c r="L67" s="31" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="M67" s="9"/>
       <c r="N67" s="2"/>
@@ -3659,10 +3674,10 @@
         <v>180</v>
       </c>
       <c r="B68" s="26" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C68" s="28" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D68" s="9" t="s">
         <v>237</v>
@@ -3683,7 +3698,7 @@
         <v>113</v>
       </c>
       <c r="L68" s="31" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="M68" s="9"/>
       <c r="N68" s="2"/>
@@ -3693,10 +3708,10 @@
         <v>182</v>
       </c>
       <c r="B69" s="26" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C69" s="28" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D69" s="9" t="s">
         <v>239</v>
@@ -3721,10 +3736,10 @@
         <v>184</v>
       </c>
       <c r="B70" s="26" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C70" s="28" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D70" s="9" t="s">
         <v>241</v>
@@ -3749,10 +3764,10 @@
         <v>187</v>
       </c>
       <c r="B71" s="26" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C71" s="28" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D71" s="9" t="s">
         <v>243</v>
@@ -3779,10 +3794,10 @@
         <v>189</v>
       </c>
       <c r="B72" s="26" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C72" s="28" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D72" s="9" t="s">
         <v>246</v>
@@ -3807,10 +3822,10 @@
         <v>191</v>
       </c>
       <c r="B73" s="26" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C73" s="28" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D73" s="9" t="s">
         <v>247</v>
@@ -3835,10 +3850,10 @@
         <v>193</v>
       </c>
       <c r="B74" s="26" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C74" s="28" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D74" s="9" t="s">
         <v>249</v>
@@ -3848,7 +3863,7 @@
       </c>
       <c r="F74" s="9"/>
       <c r="G74" s="25" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="H74" s="9" t="s">
         <v>251</v>
@@ -3869,10 +3884,10 @@
         <v>195</v>
       </c>
       <c r="B75" s="26" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C75" s="28" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D75" s="9" t="s">
         <v>253</v>
@@ -3903,10 +3918,10 @@
         <v>197</v>
       </c>
       <c r="B76" s="26" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C76" s="28" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D76" s="9" t="s">
         <v>255</v>
@@ -3935,10 +3950,10 @@
         <v>199</v>
       </c>
       <c r="B77" s="26" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C77" s="28" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D77" s="9" t="s">
         <v>256</v>
@@ -3969,10 +3984,10 @@
         <v>201</v>
       </c>
       <c r="B78" s="26" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C78" s="28" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D78" s="9" t="s">
         <v>258</v>
@@ -4001,10 +4016,10 @@
         <v>203</v>
       </c>
       <c r="B79" s="26" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C79" s="28" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D79" s="9" t="s">
         <v>259</v>
@@ -4035,10 +4050,10 @@
         <v>204</v>
       </c>
       <c r="B80" s="26" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C80" s="28" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D80" s="9" t="s">
         <v>260</v>
@@ -4067,10 +4082,10 @@
         <v>206</v>
       </c>
       <c r="B81" s="26" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C81" s="28" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D81" s="9" t="s">
         <v>261</v>
@@ -4101,10 +4116,10 @@
         <v>208</v>
       </c>
       <c r="B82" s="26" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C82" s="28" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D82" s="9" t="s">
         <v>264</v>
@@ -4135,10 +4150,10 @@
         <v>212</v>
       </c>
       <c r="B83" s="26" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C83" s="28" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D83" s="9" t="s">
         <v>266</v>
@@ -4167,10 +4182,10 @@
         <v>216</v>
       </c>
       <c r="B84" s="26" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C84" s="28" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D84" s="9" t="s">
         <v>268</v>
@@ -4191,7 +4206,7 @@
         <v>113</v>
       </c>
       <c r="L84" s="31" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="M84" s="9"/>
       <c r="N84" s="2"/>
@@ -4201,10 +4216,10 @@
         <v>219</v>
       </c>
       <c r="B85" s="26" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C85" s="28" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D85" s="9" t="s">
         <v>270</v>
@@ -4225,7 +4240,7 @@
         <v>113</v>
       </c>
       <c r="L85" s="31" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="M85" s="9"/>
       <c r="N85" s="2"/>
@@ -4235,10 +4250,10 @@
         <v>222</v>
       </c>
       <c r="B86" s="26" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C86" s="28" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D86" s="9" t="s">
         <v>271</v>
@@ -4263,10 +4278,10 @@
         <v>224</v>
       </c>
       <c r="B87" s="26" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C87" s="28" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D87" s="9" t="s">
         <v>273</v>
@@ -4293,10 +4308,10 @@
         <v>227</v>
       </c>
       <c r="B88" s="26" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C88" s="28" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D88" s="9" t="s">
         <v>275</v>
@@ -4321,10 +4336,10 @@
         <v>229</v>
       </c>
       <c r="B89" s="26" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C89" s="28" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D89" s="9" t="s">
         <v>276</v>
@@ -4349,10 +4364,10 @@
         <v>231</v>
       </c>
       <c r="B90" s="26" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C90" s="28" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D90" s="9" t="s">
         <v>277</v>
@@ -4377,10 +4392,10 @@
         <v>233</v>
       </c>
       <c r="B91" s="26" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C91" s="28" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D91" s="9" t="s">
         <v>278</v>
@@ -4405,10 +4420,10 @@
         <v>236</v>
       </c>
       <c r="B92" s="26" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C92" s="28" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D92" s="9" t="s">
         <v>281</v>
@@ -4433,10 +4448,10 @@
         <v>238</v>
       </c>
       <c r="B93" s="26" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C93" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D93" t="s">
         <v>283</v>
@@ -4535,7 +4550,7 @@
       </c>
       <c r="I2" s="9"/>
       <c r="J2" s="28" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="K2" s="9"/>
       <c r="L2" s="9"/>
@@ -4770,7 +4785,7 @@
   <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="D6" sqref="D6:D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5118,6 +5133,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
document upload with comment
</commit_message>
<xml_diff>
--- a/dataland-framework-toolbox/inputs/sme/sme.xlsx
+++ b/dataland-framework-toolbox/inputs/sme/sme.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d92048\IdeaProjects\Dataland5\dataland-framework-toolbox\inputs\sme\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d92928\Documents\Projects\Dataland\Dataland\dataland-framework-toolbox\inputs\sme\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47A2F47E-3AD2-4188-8A87-3994DDFE96BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC72491D-8161-42BE-B726-4F9901CF7A24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C4E498E0-8E09-4328-BD54-6E3CD29DBCBD}"/>
+    <workbookView xWindow="19090" yWindow="-11000" windowWidth="25820" windowHeight="14020" xr2:uid="{C4E498E0-8E09-4328-BD54-6E3CD29DBCBD}"/>
   </bookViews>
   <sheets>
     <sheet name="Framework Data Model" sheetId="1" r:id="rId1"/>
@@ -883,9 +883,6 @@
     <t>Please disclose whether you have a process in place for identifying wether there are value chain workers, affected communities, or consumers and end-users who are affected or are likely to be affected by severe negative impacts in relation to the undertaking’s operations (i.e., its products, services and activities). If this is in place, please describe this process. If identified, please also describe the types of impacts, including where they arise and the groups that are affected by them.</t>
   </si>
   <si>
-    <t>FreeText</t>
-  </si>
-  <si>
     <t>Number convictions</t>
   </si>
   <si>
@@ -1057,6 +1054,9 @@
   </si>
   <si>
     <t> </t>
+  </si>
+  <si>
+    <t>Multiple Documents With Descriptions</t>
   </si>
 </sst>
 </file>
@@ -1651,77 +1651,77 @@
   <dimension ref="A1:N94"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+      <pane ySplit="1" topLeftCell="A88" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F92" sqref="F92"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.81640625" customWidth="1"/>
-    <col min="4" max="4" width="26.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="38.453125" customWidth="1"/>
-    <col min="6" max="6" width="27.1796875" customWidth="1"/>
-    <col min="7" max="7" width="58.54296875" customWidth="1"/>
-    <col min="8" max="8" width="13.08984375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.54296875" customWidth="1"/>
-    <col min="10" max="10" width="17.1796875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.77734375" customWidth="1"/>
+    <col min="4" max="4" width="26.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="38.44140625" customWidth="1"/>
+    <col min="6" max="6" width="27.21875" customWidth="1"/>
+    <col min="7" max="7" width="58.5546875" customWidth="1"/>
+    <col min="8" max="8" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.5546875" customWidth="1"/>
+    <col min="10" max="10" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="24" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" s="24" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
+        <v>282</v>
+      </c>
+      <c r="B1" s="21" t="s">
         <v>283</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="C1" s="16" t="s">
         <v>284</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="D1" s="21" t="s">
         <v>285</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="E1" s="22" t="s">
         <v>286</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="F1" s="22" t="s">
         <v>287</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="G1" s="16" t="s">
         <v>288</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="H1" s="21" t="s">
         <v>289</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="I1" s="21" t="s">
         <v>290</v>
       </c>
-      <c r="I1" s="21" t="s">
+      <c r="J1" s="21" t="s">
         <v>291</v>
       </c>
-      <c r="J1" s="21" t="s">
+      <c r="K1" s="23" t="s">
         <v>292</v>
       </c>
-      <c r="K1" s="23" t="s">
+      <c r="L1" s="21" t="s">
         <v>293</v>
       </c>
-      <c r="L1" s="21" t="s">
+      <c r="M1" s="21" t="s">
         <v>294</v>
       </c>
-      <c r="M1" s="21" t="s">
-        <v>295</v>
-      </c>
       <c r="N1" s="21"/>
     </row>
-    <row r="2" spans="1:14" ht="87" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A2" s="35" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="26" t="s">
+        <v>299</v>
+      </c>
+      <c r="C2" s="27" t="s">
         <v>300</v>
-      </c>
-      <c r="C2" s="27" t="s">
-        <v>301</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>3</v>
@@ -1743,25 +1743,25 @@
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
     </row>
-    <row r="3" spans="1:14" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="35" t="s">
         <v>11</v>
       </c>
       <c r="B3" s="26" t="s">
+        <v>299</v>
+      </c>
+      <c r="C3" s="27" t="s">
         <v>300</v>
       </c>
-      <c r="C3" s="27" t="s">
-        <v>301</v>
-      </c>
       <c r="D3" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>8</v>
       </c>
       <c r="F3" s="5"/>
       <c r="G3" s="27" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
@@ -1771,45 +1771,45 @@
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
     </row>
-    <row r="4" spans="1:14" s="33" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="34">
         <v>3</v>
       </c>
       <c r="B4" s="26" t="s">
+        <v>299</v>
+      </c>
+      <c r="C4" s="27" t="s">
         <v>300</v>
       </c>
-      <c r="C4" s="27" t="s">
-        <v>301</v>
-      </c>
       <c r="D4" s="32" t="s">
+        <v>325</v>
+      </c>
+      <c r="E4" s="32" t="s">
         <v>326</v>
       </c>
-      <c r="E4" s="32" t="s">
+      <c r="F4" s="32" t="s">
         <v>327</v>
       </c>
-      <c r="F4" s="32" t="s">
+      <c r="G4" s="32" t="s">
         <v>328</v>
-      </c>
-      <c r="G4" s="32" t="s">
-        <v>329</v>
       </c>
       <c r="H4" s="32"/>
       <c r="I4" s="32" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="J4" s="32" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="34" t="s">
         <v>18</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C5" s="28" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>12</v>
@@ -1818,8 +1818,8 @@
         <v>13</v>
       </c>
       <c r="F5" s="10"/>
-      <c r="G5" s="3" t="s">
-        <v>279</v>
+      <c r="G5" s="27" t="s">
+        <v>330</v>
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
@@ -1829,15 +1829,15 @@
       <c r="M5" s="3"/>
       <c r="N5" s="2"/>
     </row>
-    <row r="6" spans="1:14" ht="58" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="35" t="s">
         <v>21</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C6" s="28" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>14</v>
@@ -1859,15 +1859,15 @@
       <c r="M6" s="3"/>
       <c r="N6" s="2"/>
     </row>
-    <row r="7" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="34" t="s">
         <v>23</v>
       </c>
       <c r="B7" s="26" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C7" s="28" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>19</v>
@@ -1884,22 +1884,22 @@
         <v>17</v>
       </c>
       <c r="J7" s="11" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="K7" s="12"/>
       <c r="L7" s="11"/>
       <c r="M7" s="3"/>
       <c r="N7" s="2"/>
     </row>
-    <row r="8" spans="1:14" ht="29" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="35" t="s">
         <v>25</v>
       </c>
       <c r="B8" s="26" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C8" s="28" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>22</v>
@@ -1919,15 +1919,15 @@
       <c r="M8" s="3"/>
       <c r="N8" s="2"/>
     </row>
-    <row r="9" spans="1:14" ht="29" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="34" t="s">
         <v>29</v>
       </c>
       <c r="B9" s="26" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C9" s="28" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>24</v>
@@ -1947,15 +1947,15 @@
       <c r="M9" s="3"/>
       <c r="N9" s="2"/>
     </row>
-    <row r="10" spans="1:14" ht="87" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A10" s="35" t="s">
         <v>32</v>
       </c>
       <c r="B10" s="26" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C10" s="28" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>26</v>
@@ -1972,22 +1972,22 @@
         <v>28</v>
       </c>
       <c r="J10" s="11" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="K10" s="12"/>
       <c r="L10" s="11"/>
       <c r="M10" s="3"/>
       <c r="N10" s="2"/>
     </row>
-    <row r="11" spans="1:14" ht="29" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="34" t="s">
         <v>35</v>
       </c>
       <c r="B11" s="26" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C11" s="28" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>30</v>
@@ -2004,22 +2004,22 @@
         <v>28</v>
       </c>
       <c r="J11" s="11" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="K11" s="12"/>
       <c r="L11" s="11"/>
       <c r="M11" s="3"/>
       <c r="N11" s="2"/>
     </row>
-    <row r="12" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="35" t="s">
         <v>38</v>
       </c>
       <c r="B12" s="26" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C12" s="28" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>33</v>
@@ -2036,22 +2036,22 @@
         <v>28</v>
       </c>
       <c r="J12" s="11" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="K12" s="12"/>
       <c r="L12" s="11"/>
       <c r="M12" s="3"/>
       <c r="N12" s="2"/>
     </row>
-    <row r="13" spans="1:14" ht="29" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="34" t="s">
         <v>41</v>
       </c>
       <c r="B13" s="26" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C13" s="28" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>36</v>
@@ -2068,32 +2068,32 @@
         <v>28</v>
       </c>
       <c r="J13" s="11" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="K13" s="12"/>
       <c r="L13" s="11"/>
       <c r="M13" s="3"/>
       <c r="N13" s="2"/>
     </row>
-    <row r="14" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A14" s="35" t="s">
         <v>44</v>
       </c>
       <c r="B14" s="26" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C14" s="28" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D14" s="27" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E14" s="9" t="s">
         <v>40</v>
       </c>
       <c r="F14" s="10"/>
       <c r="G14" s="19" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
@@ -2103,25 +2103,25 @@
       <c r="M14" s="3"/>
       <c r="N14" s="2"/>
     </row>
-    <row r="15" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A15" s="34" t="s">
         <v>47</v>
       </c>
       <c r="B15" s="26" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C15" s="28" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D15" s="27" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E15" s="9" t="s">
         <v>53</v>
       </c>
       <c r="F15" s="10"/>
       <c r="G15" s="31" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
@@ -2131,15 +2131,15 @@
       <c r="M15" s="3"/>
       <c r="N15" s="2"/>
     </row>
-    <row r="16" spans="1:14" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A16" s="35" t="s">
         <v>51</v>
       </c>
       <c r="B16" s="26" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C16" s="28" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D16" s="9" t="s">
         <v>83</v>
@@ -2159,15 +2159,15 @@
       <c r="M16" s="9"/>
       <c r="N16" s="2"/>
     </row>
-    <row r="17" spans="1:14" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:14" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A17" s="34" t="s">
         <v>54</v>
       </c>
       <c r="B17" s="26" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C17" s="28" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D17" s="9" t="s">
         <v>85</v>
@@ -2187,15 +2187,15 @@
       <c r="M17" s="9"/>
       <c r="N17" s="2"/>
     </row>
-    <row r="18" spans="1:14" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:14" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A18" s="35" t="s">
         <v>56</v>
       </c>
       <c r="B18" s="26" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C18" s="28" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D18" s="9" t="s">
         <v>87</v>
@@ -2215,15 +2215,15 @@
       <c r="M18" s="9"/>
       <c r="N18" s="2"/>
     </row>
-    <row r="19" spans="1:14" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:14" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A19" s="34" t="s">
         <v>58</v>
       </c>
       <c r="B19" s="26" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C19" s="28" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D19" s="9" t="s">
         <v>90</v>
@@ -2243,15 +2243,15 @@
       <c r="M19" s="9"/>
       <c r="N19" s="2"/>
     </row>
-    <row r="20" spans="1:14" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:14" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A20" s="35" t="s">
         <v>60</v>
       </c>
       <c r="B20" s="26" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C20" s="28" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D20" s="9" t="s">
         <v>92</v>
@@ -2271,15 +2271,15 @@
       <c r="M20" s="9"/>
       <c r="N20" s="2"/>
     </row>
-    <row r="21" spans="1:14" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:14" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A21" s="34" t="s">
         <v>62</v>
       </c>
       <c r="B21" s="26" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C21" s="28" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D21" s="9" t="s">
         <v>94</v>
@@ -2299,18 +2299,18 @@
       <c r="M21" s="9"/>
       <c r="N21" s="2"/>
     </row>
-    <row r="22" spans="1:14" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:14" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A22" s="35" t="s">
         <v>65</v>
       </c>
       <c r="B22" s="26" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C22" s="28" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D22" s="28" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E22" s="9" t="s">
         <v>81</v>
@@ -2327,15 +2327,15 @@
       <c r="M22" s="9"/>
       <c r="N22" s="2"/>
     </row>
-    <row r="23" spans="1:14" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:14" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A23" s="34" t="s">
         <v>68</v>
       </c>
       <c r="B23" s="26" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C23" s="28" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D23" s="9" t="s">
         <v>97</v>
@@ -2355,15 +2355,15 @@
       <c r="M23" s="9"/>
       <c r="N23" s="2"/>
     </row>
-    <row r="24" spans="1:14" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:14" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A24" s="35" t="s">
         <v>70</v>
       </c>
       <c r="B24" s="26" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C24" s="28" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D24" s="9" t="s">
         <v>99</v>
@@ -2383,15 +2383,15 @@
       <c r="M24" s="9"/>
       <c r="N24" s="2"/>
     </row>
-    <row r="25" spans="1:14" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:14" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A25" s="34" t="s">
         <v>72</v>
       </c>
       <c r="B25" s="26" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C25" s="28" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D25" s="9" t="s">
         <v>101</v>
@@ -2411,15 +2411,15 @@
       <c r="M25" s="9"/>
       <c r="N25" s="2"/>
     </row>
-    <row r="26" spans="1:14" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:14" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A26" s="35" t="s">
         <v>74</v>
       </c>
       <c r="B26" s="26" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C26" s="28" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D26" s="9" t="s">
         <v>103</v>
@@ -2439,15 +2439,15 @@
       <c r="M26" s="9"/>
       <c r="N26" s="2"/>
     </row>
-    <row r="27" spans="1:14" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:14" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A27" s="34" t="s">
         <v>76</v>
       </c>
       <c r="B27" s="26" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C27" s="28" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D27" s="9" t="s">
         <v>105</v>
@@ -2467,15 +2467,15 @@
       <c r="M27" s="9"/>
       <c r="N27" s="2"/>
     </row>
-    <row r="28" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A28" s="35" t="s">
         <v>80</v>
       </c>
       <c r="B28" s="26" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C28" s="28" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D28" s="9" t="s">
         <v>107</v>
@@ -2489,25 +2489,25 @@
       </c>
       <c r="H28" s="9"/>
       <c r="I28" s="29" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="J28" s="11" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="K28" s="9"/>
       <c r="L28" s="9"/>
       <c r="M28" s="9"/>
       <c r="N28" s="2"/>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A29" s="34" t="s">
         <v>82</v>
       </c>
       <c r="B29" s="26" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C29" s="28" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D29" s="9" t="s">
         <v>111</v>
@@ -2519,7 +2519,7 @@
       </c>
       <c r="H29" s="9"/>
       <c r="I29" s="29" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="J29" s="9"/>
       <c r="K29" s="9"/>
@@ -2527,21 +2527,21 @@
       <c r="M29" s="9"/>
       <c r="N29" s="2"/>
     </row>
-    <row r="30" spans="1:14" ht="88" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:14" ht="87.6" x14ac:dyDescent="0.3">
       <c r="A30" s="35" t="s">
         <v>84</v>
       </c>
       <c r="B30" s="26" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C30" s="28" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D30" s="9" t="s">
         <v>113</v>
       </c>
       <c r="E30" s="9" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F30" s="9"/>
       <c r="G30" s="9" t="s">
@@ -2549,7 +2549,7 @@
       </c>
       <c r="H30" s="9"/>
       <c r="I30" s="29" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="J30" s="9"/>
       <c r="K30" s="9"/>
@@ -2557,15 +2557,15 @@
       <c r="M30" s="9"/>
       <c r="N30" s="2"/>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A31" s="34" t="s">
         <v>86</v>
       </c>
       <c r="B31" s="26" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C31" s="28" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D31" s="9" t="s">
         <v>115</v>
@@ -2577,7 +2577,7 @@
       </c>
       <c r="H31" s="9"/>
       <c r="I31" s="29" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="J31" s="9"/>
       <c r="K31" s="9"/>
@@ -2585,15 +2585,15 @@
       <c r="M31" s="9"/>
       <c r="N31" s="2"/>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A32" s="35" t="s">
         <v>89</v>
       </c>
       <c r="B32" s="26" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C32" s="28" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D32" s="9" t="s">
         <v>117</v>
@@ -2605,7 +2605,7 @@
       </c>
       <c r="H32" s="9"/>
       <c r="I32" s="29" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="J32" s="9"/>
       <c r="K32" s="9"/>
@@ -2613,15 +2613,15 @@
       <c r="M32" s="9"/>
       <c r="N32" s="2"/>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A33" s="34" t="s">
         <v>91</v>
       </c>
       <c r="B33" s="26" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C33" s="28" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D33" s="9" t="s">
         <v>119</v>
@@ -2633,7 +2633,7 @@
       </c>
       <c r="H33" s="9"/>
       <c r="I33" s="29" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="J33" s="9"/>
       <c r="K33" s="9"/>
@@ -2641,15 +2641,15 @@
       <c r="M33" s="9"/>
       <c r="N33" s="2"/>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A34" s="35" t="s">
         <v>93</v>
       </c>
       <c r="B34" s="26" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C34" s="28" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D34" s="9" t="s">
         <v>121</v>
@@ -2661,7 +2661,7 @@
       </c>
       <c r="H34" s="9"/>
       <c r="I34" s="29" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="J34" s="9"/>
       <c r="K34" s="9"/>
@@ -2669,15 +2669,15 @@
       <c r="M34" s="9"/>
       <c r="N34" s="2"/>
     </row>
-    <row r="35" spans="1:14" ht="29" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A35" s="34" t="s">
         <v>95</v>
       </c>
       <c r="B35" s="26" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C35" s="28" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D35" s="9" t="s">
         <v>123</v>
@@ -2689,7 +2689,7 @@
       </c>
       <c r="H35" s="9"/>
       <c r="I35" s="29" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="J35" s="9"/>
       <c r="K35" s="9"/>
@@ -2697,15 +2697,15 @@
       <c r="M35" s="9"/>
       <c r="N35" s="2"/>
     </row>
-    <row r="36" spans="1:14" ht="246.5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:14" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A36" s="35" t="s">
         <v>96</v>
       </c>
       <c r="B36" s="26" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C36" s="28" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D36" s="9" t="s">
         <v>126</v>
@@ -2727,15 +2727,15 @@
       <c r="M36" s="9"/>
       <c r="N36" s="2"/>
     </row>
-    <row r="37" spans="1:14" ht="29" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A37" s="34" t="s">
         <v>98</v>
       </c>
       <c r="B37" s="26" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C37" s="28" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D37" s="9" t="s">
         <v>130</v>
@@ -2755,15 +2755,15 @@
       <c r="M37" s="9"/>
       <c r="N37" s="2"/>
     </row>
-    <row r="38" spans="1:14" ht="29" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A38" s="35" t="s">
         <v>100</v>
       </c>
       <c r="B38" s="26" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C38" s="28" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D38" s="9" t="s">
         <v>132</v>
@@ -2781,15 +2781,15 @@
       <c r="M38" s="9"/>
       <c r="N38" s="2"/>
     </row>
-    <row r="39" spans="1:14" ht="29" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A39" s="34" t="s">
         <v>102</v>
       </c>
       <c r="B39" s="26" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C39" s="28" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D39" s="9" t="s">
         <v>134</v>
@@ -2809,18 +2809,18 @@
       <c r="M39" s="9"/>
       <c r="N39" s="2"/>
     </row>
-    <row r="40" spans="1:14" ht="29" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A40" s="35" t="s">
         <v>104</v>
       </c>
       <c r="B40" s="26" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C40" s="28" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D40" s="9" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E40" s="9"/>
       <c r="F40" s="9"/>
@@ -2835,15 +2835,15 @@
       <c r="M40" s="9"/>
       <c r="N40" s="2"/>
     </row>
-    <row r="41" spans="1:14" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:14" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A41" s="34" t="s">
         <v>106</v>
       </c>
       <c r="B41" s="26" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C41" s="28" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D41" s="9" t="s">
         <v>137</v>
@@ -2853,7 +2853,7 @@
       </c>
       <c r="F41" s="9"/>
       <c r="G41" s="25" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="H41" s="9" t="s">
         <v>139</v>
@@ -2865,23 +2865,23 @@
       <c r="M41" s="9"/>
       <c r="N41" s="2"/>
     </row>
-    <row r="42" spans="1:14" ht="29" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A42" s="35" t="s">
         <v>110</v>
       </c>
       <c r="B42" s="26" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C42" s="28" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D42" s="28" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="E42" s="9"/>
       <c r="F42" s="9"/>
       <c r="G42" s="8" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="H42" s="9"/>
       <c r="I42" s="9"/>
@@ -2891,15 +2891,15 @@
       <c r="M42" s="9"/>
       <c r="N42" s="2"/>
     </row>
-    <row r="43" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A43" s="34" t="s">
         <v>112</v>
       </c>
       <c r="B43" s="26" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C43" s="28" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D43" s="9" t="s">
         <v>162</v>
@@ -2909,7 +2909,7 @@
       </c>
       <c r="F43" s="9"/>
       <c r="G43" s="25" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="H43" s="9" t="s">
         <v>164</v>
@@ -2921,15 +2921,15 @@
       <c r="M43" s="9"/>
       <c r="N43" s="2"/>
     </row>
-    <row r="44" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A44" s="35" t="s">
         <v>114</v>
       </c>
       <c r="B44" s="26" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C44" s="28" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D44" s="9" t="s">
         <v>166</v>
@@ -2950,20 +2950,20 @@
         <v>112</v>
       </c>
       <c r="L44" s="30" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="M44" s="9"/>
       <c r="N44" s="2"/>
     </row>
-    <row r="45" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A45" s="34" t="s">
         <v>116</v>
       </c>
       <c r="B45" s="26" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C45" s="28" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D45" s="9" t="s">
         <v>171</v>
@@ -2984,20 +2984,20 @@
         <v>112</v>
       </c>
       <c r="L45" s="30" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="M45" s="9"/>
       <c r="N45" s="2"/>
     </row>
-    <row r="46" spans="1:14" ht="58" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A46" s="35" t="s">
         <v>118</v>
       </c>
       <c r="B46" s="26" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C46" s="28" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D46" s="9" t="s">
         <v>175</v>
@@ -3018,20 +3018,20 @@
         <v>112</v>
       </c>
       <c r="L46" s="30" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="M46" s="9"/>
       <c r="N46" s="2"/>
     </row>
-    <row r="47" spans="1:14" ht="58" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A47" s="34" t="s">
         <v>120</v>
       </c>
       <c r="B47" s="26" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C47" s="28" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D47" s="9" t="s">
         <v>178</v>
@@ -3052,20 +3052,20 @@
         <v>112</v>
       </c>
       <c r="L47" s="30" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="M47" s="9"/>
       <c r="N47" s="2"/>
     </row>
-    <row r="48" spans="1:14" ht="29" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A48" s="35" t="s">
         <v>122</v>
       </c>
       <c r="B48" s="26" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C48" s="28" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D48" s="9" t="s">
         <v>180</v>
@@ -3084,20 +3084,20 @@
         <v>112</v>
       </c>
       <c r="L48" s="30" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="M48" s="9"/>
       <c r="N48" s="2"/>
     </row>
-    <row r="49" spans="1:14" ht="29" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A49" s="34" t="s">
         <v>124</v>
       </c>
       <c r="B49" s="26" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C49" s="28" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D49" s="9" t="s">
         <v>182</v>
@@ -3116,20 +3116,20 @@
         <v>112</v>
       </c>
       <c r="L49" s="30" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="M49" s="9"/>
       <c r="N49" s="2"/>
     </row>
-    <row r="50" spans="1:14" ht="58" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A50" s="35" t="s">
         <v>129</v>
       </c>
       <c r="B50" s="26" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C50" s="28" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D50" s="9" t="s">
         <v>184</v>
@@ -3150,20 +3150,20 @@
         <v>112</v>
       </c>
       <c r="L50" s="30" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="M50" s="9"/>
       <c r="N50" s="2"/>
     </row>
-    <row r="51" spans="1:14" ht="58" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A51" s="34" t="s">
         <v>131</v>
       </c>
       <c r="B51" s="26" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C51" s="28" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D51" s="9" t="s">
         <v>187</v>
@@ -3184,20 +3184,20 @@
         <v>112</v>
       </c>
       <c r="L51" s="30" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="M51" s="9"/>
       <c r="N51" s="2"/>
     </row>
-    <row r="52" spans="1:14" ht="29" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A52" s="35" t="s">
         <v>133</v>
       </c>
       <c r="B52" s="26" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C52" s="28" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D52" s="9" t="s">
         <v>189</v>
@@ -3216,20 +3216,20 @@
         <v>112</v>
       </c>
       <c r="L52" s="30" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="M52" s="9"/>
       <c r="N52" s="2"/>
     </row>
-    <row r="53" spans="1:14" ht="29" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A53" s="34" t="s">
         <v>135</v>
       </c>
       <c r="B53" s="26" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C53" s="28" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D53" s="9" t="s">
         <v>191</v>
@@ -3248,20 +3248,20 @@
         <v>112</v>
       </c>
       <c r="L53" s="30" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="M53" s="9"/>
       <c r="N53" s="2"/>
     </row>
-    <row r="54" spans="1:14" ht="29" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A54" s="35" t="s">
         <v>136</v>
       </c>
       <c r="B54" s="26" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C54" s="28" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D54" s="9" t="s">
         <v>193</v>
@@ -3280,20 +3280,20 @@
         <v>112</v>
       </c>
       <c r="L54" s="30" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="M54" s="9"/>
       <c r="N54" s="2"/>
     </row>
-    <row r="55" spans="1:14" ht="29" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A55" s="34" t="s">
         <v>140</v>
       </c>
       <c r="B55" s="26" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C55" s="28" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D55" s="9" t="s">
         <v>195</v>
@@ -3312,20 +3312,20 @@
         <v>112</v>
       </c>
       <c r="L55" s="30" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="M55" s="9"/>
       <c r="N55" s="2"/>
     </row>
-    <row r="56" spans="1:14" ht="29" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A56" s="35" t="s">
         <v>141</v>
       </c>
       <c r="B56" s="26" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C56" s="28" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D56" s="9" t="s">
         <v>197</v>
@@ -3344,20 +3344,20 @@
         <v>112</v>
       </c>
       <c r="L56" s="30" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="M56" s="9"/>
       <c r="N56" s="2"/>
     </row>
-    <row r="57" spans="1:14" ht="29" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A57" s="34" t="s">
         <v>144</v>
       </c>
       <c r="B57" s="26" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C57" s="28" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D57" s="9" t="s">
         <v>199</v>
@@ -3376,30 +3376,30 @@
         <v>112</v>
       </c>
       <c r="L57" s="30" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="M57" s="9"/>
       <c r="N57" s="2"/>
     </row>
-    <row r="58" spans="1:14" ht="58" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A58" s="35" t="s">
         <v>146</v>
       </c>
       <c r="B58" s="26" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C58" s="28" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D58" s="28" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="E58" s="9" t="s">
         <v>201</v>
       </c>
       <c r="F58" s="9"/>
       <c r="G58" s="19" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="H58" s="9"/>
       <c r="I58" s="9"/>
@@ -3409,15 +3409,15 @@
       <c r="M58" s="9"/>
       <c r="N58" s="2"/>
     </row>
-    <row r="59" spans="1:14" ht="29" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A59" s="34" t="s">
         <v>149</v>
       </c>
       <c r="B59" s="26" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C59" s="28" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D59" s="9" t="s">
         <v>208</v>
@@ -3439,15 +3439,15 @@
       <c r="M59" s="9"/>
       <c r="N59" s="2"/>
     </row>
-    <row r="60" spans="1:14" ht="29" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A60" s="35" t="s">
         <v>152</v>
       </c>
       <c r="B60" s="26" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C60" s="28" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D60" s="9" t="s">
         <v>212</v>
@@ -3467,15 +3467,15 @@
       <c r="M60" s="9"/>
       <c r="N60" s="2"/>
     </row>
-    <row r="61" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A61" s="34" t="s">
         <v>154</v>
       </c>
       <c r="B61" s="26" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C61" s="28" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D61" s="9" t="s">
         <v>216</v>
@@ -3495,15 +3495,15 @@
       <c r="M61" s="9"/>
       <c r="N61" s="2"/>
     </row>
-    <row r="62" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A62" s="35" t="s">
         <v>156</v>
       </c>
       <c r="B62" s="26" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C62" s="28" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D62" s="9" t="s">
         <v>219</v>
@@ -3524,20 +3524,20 @@
         <v>112</v>
       </c>
       <c r="L62" s="30" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="M62" s="9"/>
       <c r="N62" s="2"/>
     </row>
-    <row r="63" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A63" s="34" t="s">
         <v>158</v>
       </c>
       <c r="B63" s="26" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C63" s="28" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D63" s="9" t="s">
         <v>222</v>
@@ -3558,20 +3558,20 @@
         <v>112</v>
       </c>
       <c r="L63" s="30" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="M63" s="9"/>
       <c r="N63" s="2"/>
     </row>
-    <row r="64" spans="1:14" ht="58" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A64" s="35" t="s">
         <v>160</v>
       </c>
       <c r="B64" s="26" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C64" s="28" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D64" s="9" t="s">
         <v>224</v>
@@ -3592,20 +3592,20 @@
         <v>112</v>
       </c>
       <c r="L64" s="30" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="M64" s="9"/>
       <c r="N64" s="2"/>
     </row>
-    <row r="65" spans="1:14" ht="58" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A65" s="34" t="s">
         <v>165</v>
       </c>
       <c r="B65" s="26" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C65" s="28" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D65" s="9" t="s">
         <v>227</v>
@@ -3626,20 +3626,20 @@
         <v>112</v>
       </c>
       <c r="L65" s="30" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="M65" s="9"/>
       <c r="N65" s="2"/>
     </row>
-    <row r="66" spans="1:14" ht="29" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A66" s="35" t="s">
         <v>170</v>
       </c>
       <c r="B66" s="26" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C66" s="28" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D66" s="9" t="s">
         <v>229</v>
@@ -3658,20 +3658,20 @@
         <v>112</v>
       </c>
       <c r="L66" s="30" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="M66" s="9"/>
       <c r="N66" s="2"/>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A67" s="34" t="s">
         <v>174</v>
       </c>
       <c r="B67" s="26" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C67" s="28" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D67" s="9" t="s">
         <v>231</v>
@@ -3690,20 +3690,20 @@
         <v>112</v>
       </c>
       <c r="L67" s="30" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="M67" s="9"/>
       <c r="N67" s="2"/>
     </row>
-    <row r="68" spans="1:14" ht="58" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A68" s="35" t="s">
         <v>177</v>
       </c>
       <c r="B68" s="26" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C68" s="28" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D68" s="9" t="s">
         <v>233</v>
@@ -3724,20 +3724,20 @@
         <v>112</v>
       </c>
       <c r="L68" s="30" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="M68" s="9"/>
       <c r="N68" s="2"/>
     </row>
-    <row r="69" spans="1:14" ht="58" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A69" s="34" t="s">
         <v>179</v>
       </c>
       <c r="B69" s="26" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C69" s="28" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D69" s="9" t="s">
         <v>236</v>
@@ -3758,20 +3758,20 @@
         <v>112</v>
       </c>
       <c r="L69" s="30" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="M69" s="9"/>
       <c r="N69" s="2"/>
     </row>
-    <row r="70" spans="1:14" ht="58" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A70" s="35" t="s">
         <v>181</v>
       </c>
       <c r="B70" s="26" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C70" s="28" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D70" s="9" t="s">
         <v>238</v>
@@ -3791,15 +3791,15 @@
       <c r="M70" s="9"/>
       <c r="N70" s="2"/>
     </row>
-    <row r="71" spans="1:14" ht="58" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A71" s="34" t="s">
         <v>183</v>
       </c>
       <c r="B71" s="26" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C71" s="28" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D71" s="9" t="s">
         <v>240</v>
@@ -3819,15 +3819,15 @@
       <c r="M71" s="9"/>
       <c r="N71" s="2"/>
     </row>
-    <row r="72" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A72" s="35" t="s">
         <v>186</v>
       </c>
       <c r="B72" s="26" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C72" s="28" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D72" s="9" t="s">
         <v>242</v>
@@ -3849,15 +3849,15 @@
       <c r="M72" s="9"/>
       <c r="N72" s="2"/>
     </row>
-    <row r="73" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A73" s="34" t="s">
         <v>188</v>
       </c>
       <c r="B73" s="26" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C73" s="28" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D73" s="9" t="s">
         <v>245</v>
@@ -3877,15 +3877,15 @@
       <c r="M73" s="9"/>
       <c r="N73" s="2"/>
     </row>
-    <row r="74" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A74" s="35" t="s">
         <v>190</v>
       </c>
       <c r="B74" s="26" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C74" s="28" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D74" s="9" t="s">
         <v>246</v>
@@ -3905,15 +3905,15 @@
       <c r="M74" s="9"/>
       <c r="N74" s="2"/>
     </row>
-    <row r="75" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A75" s="34" t="s">
         <v>192</v>
       </c>
       <c r="B75" s="26" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C75" s="28" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D75" s="9" t="s">
         <v>248</v>
@@ -3923,7 +3923,7 @@
       </c>
       <c r="F75" s="9"/>
       <c r="G75" s="25" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="H75" s="9" t="s">
         <v>250</v>
@@ -3939,15 +3939,15 @@
       <c r="M75" s="9"/>
       <c r="N75" s="2"/>
     </row>
-    <row r="76" spans="1:14" ht="58" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A76" s="35" t="s">
         <v>194</v>
       </c>
       <c r="B76" s="26" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C76" s="28" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D76" s="9" t="s">
         <v>252</v>
@@ -3973,15 +3973,15 @@
       <c r="M76" s="9"/>
       <c r="N76" s="2"/>
     </row>
-    <row r="77" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A77" s="34" t="s">
         <v>196</v>
       </c>
       <c r="B77" s="26" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C77" s="28" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D77" s="9" t="s">
         <v>254</v>
@@ -4005,15 +4005,15 @@
       <c r="M77" s="9"/>
       <c r="N77" s="2"/>
     </row>
-    <row r="78" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A78" s="35" t="s">
         <v>198</v>
       </c>
       <c r="B78" s="26" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C78" s="28" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D78" s="9" t="s">
         <v>255</v>
@@ -4039,15 +4039,15 @@
       <c r="M78" s="9"/>
       <c r="N78" s="2"/>
     </row>
-    <row r="79" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A79" s="34" t="s">
         <v>200</v>
       </c>
       <c r="B79" s="26" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C79" s="28" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D79" s="9" t="s">
         <v>257</v>
@@ -4071,15 +4071,15 @@
       <c r="M79" s="9"/>
       <c r="N79" s="2"/>
     </row>
-    <row r="80" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A80" s="35" t="s">
         <v>202</v>
       </c>
       <c r="B80" s="26" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C80" s="28" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D80" s="9" t="s">
         <v>258</v>
@@ -4105,15 +4105,15 @@
       <c r="M80" s="9"/>
       <c r="N80" s="2"/>
     </row>
-    <row r="81" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A81" s="34" t="s">
         <v>203</v>
       </c>
       <c r="B81" s="26" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C81" s="28" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D81" s="9" t="s">
         <v>259</v>
@@ -4137,15 +4137,15 @@
       <c r="M81" s="9"/>
       <c r="N81" s="2"/>
     </row>
-    <row r="82" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A82" s="35" t="s">
         <v>205</v>
       </c>
       <c r="B82" s="26" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C82" s="28" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D82" s="9" t="s">
         <v>260</v>
@@ -4171,15 +4171,15 @@
       <c r="M82" s="9"/>
       <c r="N82" s="2"/>
     </row>
-    <row r="83" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A83" s="34" t="s">
         <v>207</v>
       </c>
       <c r="B83" s="26" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C83" s="28" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D83" s="9" t="s">
         <v>263</v>
@@ -4205,15 +4205,15 @@
       <c r="M83" s="9"/>
       <c r="N83" s="2"/>
     </row>
-    <row r="84" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A84" s="35" t="s">
         <v>211</v>
       </c>
       <c r="B84" s="26" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C84" s="28" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D84" s="9" t="s">
         <v>265</v>
@@ -4237,15 +4237,15 @@
       <c r="M84" s="9"/>
       <c r="N84" s="2"/>
     </row>
-    <row r="85" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A85" s="34" t="s">
         <v>215</v>
       </c>
       <c r="B85" s="26" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C85" s="28" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D85" s="9" t="s">
         <v>267</v>
@@ -4266,20 +4266,20 @@
         <v>112</v>
       </c>
       <c r="L85" s="30" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="M85" s="9"/>
       <c r="N85" s="2"/>
     </row>
-    <row r="86" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A86" s="35" t="s">
         <v>218</v>
       </c>
       <c r="B86" s="26" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C86" s="28" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D86" s="9" t="s">
         <v>269</v>
@@ -4300,20 +4300,20 @@
         <v>112</v>
       </c>
       <c r="L86" s="30" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="M86" s="9"/>
       <c r="N86" s="2"/>
     </row>
-    <row r="87" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A87" s="34" t="s">
         <v>221</v>
       </c>
       <c r="B87" s="26" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C87" s="28" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D87" s="9" t="s">
         <v>270</v>
@@ -4333,15 +4333,15 @@
       <c r="M87" s="9"/>
       <c r="N87" s="2"/>
     </row>
-    <row r="88" spans="1:14" ht="87" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:14" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A88" s="35" t="s">
         <v>223</v>
       </c>
       <c r="B88" s="26" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C88" s="28" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D88" s="9" t="s">
         <v>272</v>
@@ -4363,15 +4363,15 @@
       <c r="M88" s="9"/>
       <c r="N88" s="2"/>
     </row>
-    <row r="89" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A89" s="34" t="s">
         <v>226</v>
       </c>
       <c r="B89" s="26" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C89" s="28" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D89" s="9" t="s">
         <v>274</v>
@@ -4391,15 +4391,15 @@
       <c r="M89" s="9"/>
       <c r="N89" s="2"/>
     </row>
-    <row r="90" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A90" s="35" t="s">
         <v>228</v>
       </c>
       <c r="B90" s="26" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C90" s="28" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D90" s="9" t="s">
         <v>275</v>
@@ -4419,15 +4419,15 @@
       <c r="M90" s="9"/>
       <c r="N90" s="2"/>
     </row>
-    <row r="91" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A91" s="34" t="s">
         <v>230</v>
       </c>
       <c r="B91" s="26" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C91" s="28" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D91" s="9" t="s">
         <v>276</v>
@@ -4447,15 +4447,15 @@
       <c r="M91" s="9"/>
       <c r="N91" s="2"/>
     </row>
-    <row r="92" spans="1:14" ht="174" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:14" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A92" s="35" t="s">
         <v>232</v>
       </c>
       <c r="B92" s="26" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C92" s="28" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D92" s="9" t="s">
         <v>277</v>
@@ -4465,7 +4465,7 @@
       </c>
       <c r="F92" s="9"/>
       <c r="G92" s="9" t="s">
-        <v>279</v>
+        <v>330</v>
       </c>
       <c r="H92" s="9"/>
       <c r="I92" s="9"/>
@@ -4475,21 +4475,21 @@
       <c r="M92" s="9"/>
       <c r="N92" s="2"/>
     </row>
-    <row r="93" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A93" s="34" t="s">
         <v>235</v>
       </c>
       <c r="B93" s="26" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C93" s="28" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D93" s="9" t="s">
+        <v>279</v>
+      </c>
+      <c r="E93" s="9" t="s">
         <v>280</v>
-      </c>
-      <c r="E93" s="9" t="s">
-        <v>281</v>
       </c>
       <c r="F93" s="9"/>
       <c r="G93" s="9" t="s">
@@ -4503,18 +4503,18 @@
       <c r="M93" s="9"/>
       <c r="N93" s="2"/>
     </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A94" s="35" t="s">
         <v>237</v>
       </c>
       <c r="B94" s="26" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C94" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D94" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="G94" t="s">
         <v>16</v>
@@ -4538,56 +4538,56 @@
       <selection activeCell="E14" sqref="E11:E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="21.81640625" customWidth="1"/>
-    <col min="7" max="7" width="30.1796875" customWidth="1"/>
-    <col min="8" max="8" width="33.1796875" customWidth="1"/>
+    <col min="3" max="3" width="21.77734375" customWidth="1"/>
+    <col min="7" max="7" width="30.21875" customWidth="1"/>
+    <col min="8" max="8" width="33.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="24" customFormat="1" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" s="24" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
+        <v>282</v>
+      </c>
+      <c r="B1" s="21" t="s">
         <v>283</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="C1" s="16" t="s">
         <v>284</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="D1" s="21" t="s">
         <v>285</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="E1" s="22" t="s">
         <v>286</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="F1" s="22" t="s">
         <v>287</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="G1" s="16" t="s">
         <v>288</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="H1" s="21" t="s">
         <v>289</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="I1" s="21" t="s">
         <v>290</v>
       </c>
-      <c r="I1" s="21" t="s">
+      <c r="J1" s="21" t="s">
         <v>291</v>
       </c>
-      <c r="J1" s="21" t="s">
+      <c r="K1" s="23" t="s">
         <v>292</v>
       </c>
-      <c r="K1" s="23" t="s">
+      <c r="L1" s="21" t="s">
         <v>293</v>
       </c>
-      <c r="L1" s="21" t="s">
+      <c r="M1" s="21" t="s">
         <v>294</v>
       </c>
-      <c r="M1" s="21" t="s">
-        <v>295</v>
-      </c>
       <c r="N1" s="21"/>
     </row>
-    <row r="2" spans="1:14" ht="87" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>141</v>
       </c>
@@ -4610,14 +4610,14 @@
       </c>
       <c r="I2" s="9"/>
       <c r="J2" s="28" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="K2" s="9"/>
       <c r="L2" s="9"/>
       <c r="M2" s="9"/>
       <c r="N2" s="2"/>
     </row>
-    <row r="3" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>144</v>
       </c>
@@ -4643,7 +4643,7 @@
       <c r="M3" s="9"/>
       <c r="N3" s="2"/>
     </row>
-    <row r="4" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>146</v>
       </c>
@@ -4675,7 +4675,7 @@
       <c r="M4" s="9"/>
       <c r="N4" s="2"/>
     </row>
-    <row r="5" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>149</v>
       </c>
@@ -4707,7 +4707,7 @@
       <c r="M5" s="9"/>
       <c r="N5" s="2"/>
     </row>
-    <row r="6" spans="1:14" ht="58" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>152</v>
       </c>
@@ -4739,7 +4739,7 @@
       <c r="M6" s="9"/>
       <c r="N6" s="2"/>
     </row>
-    <row r="7" spans="1:14" ht="58" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>154</v>
       </c>
@@ -4771,7 +4771,7 @@
       <c r="M7" s="9"/>
       <c r="N7" s="2"/>
     </row>
-    <row r="8" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>156</v>
       </c>
@@ -4803,7 +4803,7 @@
       <c r="M8" s="9"/>
       <c r="N8" s="2"/>
     </row>
-    <row r="9" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>158</v>
       </c>
@@ -4848,60 +4848,60 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6" customWidth="1"/>
     <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.90625" customWidth="1"/>
-    <col min="4" max="4" width="28.54296875" customWidth="1"/>
-    <col min="5" max="5" width="26.54296875" customWidth="1"/>
-    <col min="6" max="6" width="13.36328125" customWidth="1"/>
-    <col min="7" max="7" width="47.6328125" customWidth="1"/>
+    <col min="3" max="3" width="28.88671875" customWidth="1"/>
+    <col min="4" max="4" width="28.5546875" customWidth="1"/>
+    <col min="5" max="5" width="26.5546875" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" customWidth="1"/>
+    <col min="7" max="7" width="47.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="24" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" s="24" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
+        <v>282</v>
+      </c>
+      <c r="B1" s="21" t="s">
         <v>283</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="C1" s="16" t="s">
         <v>284</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="D1" s="21" t="s">
         <v>285</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="E1" s="22" t="s">
         <v>286</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="F1" s="22" t="s">
         <v>287</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="G1" s="16" t="s">
         <v>288</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="H1" s="21" t="s">
         <v>289</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="I1" s="21" t="s">
         <v>290</v>
       </c>
-      <c r="I1" s="21" t="s">
+      <c r="J1" s="21" t="s">
         <v>291</v>
       </c>
-      <c r="J1" s="21" t="s">
+      <c r="K1" s="23" t="s">
         <v>292</v>
       </c>
-      <c r="K1" s="23" t="s">
+      <c r="L1" s="21" t="s">
         <v>293</v>
       </c>
-      <c r="L1" s="21" t="s">
+      <c r="M1" s="21" t="s">
         <v>294</v>
       </c>
-      <c r="M1" s="21" t="s">
-        <v>295</v>
-      </c>
       <c r="N1" s="21"/>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>54</v>
       </c>
@@ -4927,7 +4927,7 @@
       <c r="M2" s="3"/>
       <c r="N2" s="2"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>56</v>
       </c>
@@ -4953,7 +4953,7 @@
       <c r="M3" s="3"/>
       <c r="N3" s="2"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>58</v>
       </c>
@@ -4979,7 +4979,7 @@
       <c r="M4" s="3"/>
       <c r="N4" s="2"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>60</v>
       </c>
@@ -5005,7 +5005,7 @@
       <c r="M5" s="3"/>
       <c r="N5" s="2"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>62</v>
       </c>
@@ -5031,7 +5031,7 @@
       <c r="M6" s="3"/>
       <c r="N6" s="2"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>65</v>
       </c>
@@ -5059,7 +5059,7 @@
       <c r="M7" s="9"/>
       <c r="N7" s="2"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>68</v>
       </c>
@@ -5085,7 +5085,7 @@
       <c r="M8" s="9"/>
       <c r="N8" s="2"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>70</v>
       </c>
@@ -5111,7 +5111,7 @@
       <c r="M9" s="9"/>
       <c r="N9" s="2"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>72</v>
       </c>
@@ -5137,7 +5137,7 @@
       <c r="M10" s="9"/>
       <c r="N10" s="2"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>74</v>
       </c>
@@ -5163,7 +5163,7 @@
       <c r="M11" s="9"/>
       <c r="N11" s="2"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>76</v>
       </c>
@@ -5205,59 +5205,59 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="34" customWidth="1"/>
-    <col min="4" max="4" width="21.453125" customWidth="1"/>
-    <col min="7" max="7" width="33.81640625" customWidth="1"/>
-    <col min="9" max="9" width="18.81640625" customWidth="1"/>
-    <col min="11" max="11" width="18.453125" customWidth="1"/>
-    <col min="12" max="12" width="28.54296875" customWidth="1"/>
+    <col min="4" max="4" width="21.44140625" customWidth="1"/>
+    <col min="7" max="7" width="33.77734375" customWidth="1"/>
+    <col min="9" max="9" width="18.77734375" customWidth="1"/>
+    <col min="11" max="11" width="18.44140625" customWidth="1"/>
+    <col min="12" max="12" width="28.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="24" customFormat="1" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" s="24" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
+        <v>282</v>
+      </c>
+      <c r="B1" s="21" t="s">
         <v>283</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="C1" s="16" t="s">
         <v>284</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="D1" s="21" t="s">
         <v>285</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="E1" s="22" t="s">
         <v>286</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="F1" s="22" t="s">
         <v>287</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="G1" s="16" t="s">
         <v>288</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="H1" s="21" t="s">
         <v>289</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="I1" s="21" t="s">
         <v>290</v>
       </c>
-      <c r="I1" s="21" t="s">
+      <c r="J1" s="21" t="s">
         <v>291</v>
       </c>
-      <c r="J1" s="21" t="s">
+      <c r="K1" s="23" t="s">
         <v>292</v>
       </c>
-      <c r="K1" s="23" t="s">
+      <c r="L1" s="21" t="s">
         <v>293</v>
       </c>
-      <c r="L1" s="21" t="s">
+      <c r="M1" s="21" t="s">
         <v>294</v>
       </c>
-      <c r="M1" s="21" t="s">
-        <v>295</v>
-      </c>
       <c r="N1" s="21"/>
     </row>
-    <row r="2" spans="1:14" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>202</v>
       </c>
@@ -5283,7 +5283,7 @@
       <c r="M2" s="9"/>
       <c r="N2" s="2"/>
     </row>
-    <row r="3" spans="1:14" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>203</v>
       </c>
@@ -5315,7 +5315,7 @@
       <c r="M3" s="9"/>
       <c r="N3" s="2"/>
     </row>
-    <row r="4" spans="1:14" ht="29" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>205</v>
       </c>
@@ -5361,57 +5361,57 @@
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="47" customWidth="1"/>
-    <col min="4" max="4" width="21.81640625" customWidth="1"/>
-    <col min="7" max="7" width="34.6328125" customWidth="1"/>
-    <col min="8" max="8" width="19.90625" customWidth="1"/>
+    <col min="4" max="4" width="21.77734375" customWidth="1"/>
+    <col min="7" max="7" width="34.6640625" customWidth="1"/>
+    <col min="8" max="8" width="19.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="24" customFormat="1" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" s="24" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
+        <v>282</v>
+      </c>
+      <c r="B1" s="21" t="s">
         <v>283</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="C1" s="16" t="s">
         <v>284</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="D1" s="21" t="s">
         <v>285</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="E1" s="22" t="s">
         <v>286</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="F1" s="22" t="s">
         <v>287</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="G1" s="16" t="s">
         <v>288</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="H1" s="21" t="s">
         <v>289</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="I1" s="21" t="s">
         <v>290</v>
       </c>
-      <c r="I1" s="21" t="s">
+      <c r="J1" s="21" t="s">
         <v>291</v>
       </c>
-      <c r="J1" s="21" t="s">
+      <c r="K1" s="23" t="s">
         <v>292</v>
       </c>
-      <c r="K1" s="23" t="s">
+      <c r="L1" s="21" t="s">
         <v>293</v>
       </c>
-      <c r="L1" s="21" t="s">
+      <c r="M1" s="21" t="s">
         <v>294</v>
       </c>
-      <c r="M1" s="21" t="s">
-        <v>295</v>
-      </c>
       <c r="N1" s="21"/>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>41</v>
       </c>
@@ -5437,7 +5437,7 @@
       <c r="M2" s="3"/>
       <c r="N2" s="2"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>44</v>
       </c>
@@ -5465,7 +5465,7 @@
       <c r="M3" s="3"/>
       <c r="N3" s="2"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>47</v>
       </c>
@@ -5506,57 +5506,57 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="21.81640625" customWidth="1"/>
-    <col min="4" max="4" width="18.453125" customWidth="1"/>
-    <col min="5" max="5" width="78.6328125" customWidth="1"/>
-    <col min="7" max="7" width="17.81640625" customWidth="1"/>
+    <col min="3" max="3" width="21.77734375" customWidth="1"/>
+    <col min="4" max="4" width="18.44140625" customWidth="1"/>
+    <col min="5" max="5" width="78.6640625" customWidth="1"/>
+    <col min="7" max="7" width="17.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="24" customFormat="1" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" s="24" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
+        <v>282</v>
+      </c>
+      <c r="B1" s="21" t="s">
         <v>283</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="C1" s="16" t="s">
         <v>284</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="D1" s="21" t="s">
         <v>285</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="E1" s="22" t="s">
         <v>286</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="F1" s="22" t="s">
         <v>287</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="G1" s="16" t="s">
         <v>288</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="H1" s="21" t="s">
         <v>289</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="I1" s="21" t="s">
         <v>290</v>
       </c>
-      <c r="I1" s="21" t="s">
+      <c r="J1" s="21" t="s">
         <v>291</v>
       </c>
-      <c r="J1" s="21" t="s">
+      <c r="K1" s="23" t="s">
         <v>292</v>
       </c>
-      <c r="K1" s="23" t="s">
+      <c r="L1" s="21" t="s">
         <v>293</v>
       </c>
-      <c r="L1" s="21" t="s">
+      <c r="M1" s="21" t="s">
         <v>294</v>
       </c>
-      <c r="M1" s="21" t="s">
-        <v>295</v>
-      </c>
       <c r="N1" s="21"/>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
         <v>1</v>
@@ -5582,7 +5582,7 @@
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
     </row>
-    <row r="3" spans="1:14" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="2" t="s">
         <v>1</v>

</xml_diff>